<commit_message>
Corrige compensação de horas
</commit_message>
<xml_diff>
--- a/Controle de Ponto.xlsx
+++ b/Controle de Ponto.xlsx
@@ -5,7 +5,7 @@
   <workbookPr date1904="1" codeName="EstaPasta_de_trabalho" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evert\OneDrive\Projetos\ExcelGuru\Controle de Ponto\controle-de-ponto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m362168\OneDrive\Projetos\ExcelGuru\Controle de Ponto\controle-de-ponto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
     <definedName name="lstEvento">tblEvento[Evento]</definedName>
     <definedName name="lstLimiteHora">tblLimiteHora[Limite de horas]</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -399,13 +399,13 @@
     <t>Desenvolvido e distribuído por:</t>
   </si>
   <si>
-    <t>v7.1</t>
+    <t>v7.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="[$-416]d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="[$-416]d\-mmm;@"/>
@@ -949,28 +949,7 @@
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="55">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD5D6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD1D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="51">
     <dxf>
       <font>
         <i/>
@@ -1152,13 +1131,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFD1D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFD5D6"/>
         </patternFill>
       </fill>
@@ -1329,72 +1301,72 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tblEvento" displayName="tblEvento" ref="A2:F13" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tblEvento" displayName="tblEvento" ref="A2:F13" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
   <sortState ref="A3:F13">
     <sortCondition ref="A8"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="Evento" dataDxfId="52"/>
-    <tableColumn id="2" name="Colorir Linha" dataDxfId="51"/>
-    <tableColumn id="5" name="Colorir Período" dataDxfId="50"/>
-    <tableColumn id="6" name="Libera o Período" dataDxfId="49"/>
-    <tableColumn id="4" name="Conta hora Extra" dataDxfId="48"/>
-    <tableColumn id="3" name="Descrição" dataDxfId="47"/>
+    <tableColumn id="1" name="Evento" dataDxfId="48"/>
+    <tableColumn id="2" name="Colorir Linha" dataDxfId="47"/>
+    <tableColumn id="5" name="Colorir Período" dataDxfId="46"/>
+    <tableColumn id="6" name="Libera o Período" dataDxfId="45"/>
+    <tableColumn id="4" name="Conta hora Extra" dataDxfId="44"/>
+    <tableColumn id="3" name="Descrição" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="tblLimiteHora" displayName="tblLimiteHora" ref="H2:J4" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="tblLimiteHora" displayName="tblLimiteHora" ref="H2:J4" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <autoFilter ref="H2:J4"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Limite de horas" dataDxfId="44"/>
-    <tableColumn id="3" name="Limite" dataDxfId="43"/>
-    <tableColumn id="2" name="h" dataDxfId="42"/>
+    <tableColumn id="1" name="Limite de horas" dataDxfId="40"/>
+    <tableColumn id="3" name="Limite" dataDxfId="39"/>
+    <tableColumn id="2" name="h" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="tbl_Mes" displayName="tbl_Mes" ref="L2:L14" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="tbl_Mes" displayName="tbl_Mes" ref="L2:L14" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
   <autoFilter ref="L2:L14"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Mês" dataDxfId="39"/>
+    <tableColumn id="1" name="Mês" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tblDiaUtil" displayName="tblDiaUtil" ref="B10:E17" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tblDiaUtil" displayName="tblDiaUtil" ref="B10:E17" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <tableColumns count="4">
-    <tableColumn id="1" name="Dia da Semana" dataDxfId="35"/>
-    <tableColumn id="4" name="Abreviatura" dataDxfId="34"/>
-    <tableColumn id="2" name="É dia util?" dataDxfId="33"/>
-    <tableColumn id="3" name="Jornada Diferenciada?" dataDxfId="32"/>
+    <tableColumn id="1" name="Dia da Semana" dataDxfId="31"/>
+    <tableColumn id="4" name="Abreviatura" dataDxfId="30"/>
+    <tableColumn id="2" name="É dia util?" dataDxfId="29"/>
+    <tableColumn id="3" name="Jornada Diferenciada?" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblHoras" displayName="tblHoras" ref="B8:T39" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblHoras" displayName="tblHoras" ref="B8:T39" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <tableColumns count="19">
-    <tableColumn id="1" name="Data" dataDxfId="21">
+    <tableColumn id="1" name="Data" dataDxfId="18">
       <calculatedColumnFormula>IF(B8&lt;&gt;"",IF(DAY(B8+1)=1,"",B8+1),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Dia" dataDxfId="20">
+    <tableColumn id="2" name="Dia" dataDxfId="17">
       <calculatedColumnFormula>TEXT(tblHoras[[#This Row],[Data]],"ddd")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Evento _x000a_(1º Período)" dataDxfId="19"/>
-    <tableColumn id="4" name="Entrada - 1" dataDxfId="18"/>
-    <tableColumn id="5" name="Saída - 1 (Almoço)" dataDxfId="17"/>
-    <tableColumn id="6" name="Entrada - 2 (Almoço)" dataDxfId="16"/>
-    <tableColumn id="7" name="Saída - 2" dataDxfId="15"/>
-    <tableColumn id="13" name="Evento _x000a_(2º Período)" dataDxfId="14"/>
-    <tableColumn id="15" name="Horas Trabalhadas (1º Período)" dataDxfId="13">
+    <tableColumn id="3" name="Evento _x000a_(1º Período)" dataDxfId="16"/>
+    <tableColumn id="4" name="Entrada - 1" dataDxfId="15"/>
+    <tableColumn id="5" name="Saída - 1 (Almoço)" dataDxfId="14"/>
+    <tableColumn id="6" name="Entrada - 2 (Almoço)" dataDxfId="13"/>
+    <tableColumn id="7" name="Saída - 2" dataDxfId="12"/>
+    <tableColumn id="13" name="Evento _x000a_(2º Período)" dataDxfId="11"/>
+    <tableColumn id="15" name="Horas Trabalhadas (1º Período)" dataDxfId="10">
       <calculatedColumnFormula>IF($B$6&lt;&gt;"",IF(AND(tblHoras[[#This Row],[Evento 
 (1º Período)]]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[[#This Row],[Evento 
 (1º Período)]],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[[#This Row],[Evento 
@@ -1411,7 +1383,7 @@
                           0)),
                     0)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Horas Trabalhadas (2º Período)" dataDxfId="12">
+    <tableColumn id="16" name="Horas Trabalhadas (2º Período)" dataDxfId="9">
       <calculatedColumnFormula>IF($B$6&lt;&gt;"",IF(AND(tblHoras[[#This Row],[Evento 
 (2º Período)]]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[[#This Row],[Evento 
 (2º Período)]],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[[#This Row],[Evento 
@@ -1428,10 +1400,10 @@
                          0)),
        0)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Horas Trabalhadas" dataDxfId="11">
+    <tableColumn id="8" name="Horas Trabalhadas" dataDxfId="8">
       <calculatedColumnFormula>tblHoras[[#This Row],[Horas Trabalhadas (1º Período)]]+tblHoras[[#This Row],[Horas Trabalhadas (2º Período)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Jornada Diária" dataDxfId="10">
+    <tableColumn id="17" name="Jornada Diária" dataDxfId="7">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Data]]&lt;&gt;"",
         IF(
 AND(VLOOKUP(TEXT(tblHoras[[#This Row],[Data]],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[[#This Row],[Evento 
@@ -1443,7 +1415,7 @@
               ""),
          "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Horas Trabalhadas Além Jornada" dataDxfId="9">
+    <tableColumn id="11" name="Horas Trabalhadas Além Jornada" dataDxfId="6">
       <calculatedColumnFormula>IF(OR(tblHoras[[#This Row],[Horas Trabalhadas (1º Período)]]&lt;&gt;0,tblHoras[[#This Row],[Horas Trabalhadas (2º Período)]]&lt;&gt;0),
         IF(ISNUMBER(tblHoras[[#This Row],[Jornada Diária]]),
               IF(tblHoras[[#This Row],[Jornada Diária]]&gt;(tblHoras[[#This Row],[Horas Trabalhadas (2º Período)]]+tblHoras[[#This Row],[Horas Trabalhadas (1º Período)]]),
@@ -1466,7 +1438,7 @@
 (2º Período)]],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
 )))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Saldo de Horas" dataDxfId="8">
+    <tableColumn id="18" name="Saldo de Horas" dataDxfId="5">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&gt;0,
         IF(tblHoras[[#This Row],[Jornada Diária]]&lt;&gt;"",
               IF(HOUR(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]])&gt;=VLOOKUP(LIMITE,tblLimiteHora[],Tabelas!$I$1,FALSE),
@@ -1475,15 +1447,15 @@
               tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]),
         0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="Atrasos_x000a_(horas)" dataDxfId="7">
+    <tableColumn id="19" name="Atrasos_x000a_(horas)" dataDxfId="4">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&lt;0,IF(OR(tblHoras[[#This Row],[Evento 
 (1º Período)]]="",tblHoras[[#This Row],[Evento 
 (2º Período)]]=""),tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]],""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Faltas_x000a_(dias)" dataDxfId="6">
+    <tableColumn id="14" name="Faltas_x000a_(dias)" dataDxfId="3">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Jornada Diária]]&lt;&gt;"",IF((N(tblHoras[[#This Row],[Jornada Diária]])-ABS(N(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]])))=0,1,""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Hora Extra Normal" dataDxfId="5">
+    <tableColumn id="10" name="Hora Extra Normal" dataDxfId="2">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[[#This Row],[Data]],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[[#This Row],[Evento 
 (1º Período)]]&lt;&gt;"",IF(VLOOKUP(tblHoras[[#This Row],[Evento 
@@ -1492,7 +1464,7 @@
 (2º Período)]],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
 tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]],""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Hora Extra _x000a_Especial" dataDxfId="4">
+    <tableColumn id="9" name="Hora Extra _x000a_Especial" dataDxfId="1">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[[#This Row],[Data]],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[[#This Row],[Evento 
 (1º Período)]]&lt;&gt;"",IF(VLOOKUP(tblHoras[[#This Row],[Evento 
@@ -1501,7 +1473,7 @@
 (2º Período)]],tblEvento[],Tabelas!$E$1,FALSE)="Sim",TRUE,FALSE),FALSE)),
 tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]],""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Informação" dataDxfId="3">
+    <tableColumn id="12" name="Informação" dataDxfId="0">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Evento 
 (1º Período)]]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[[#This Row],[Evento 
 (1º Período)]],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[[#This Row],[Evento 
@@ -1518,7 +1490,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1556,7 +1528,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1628,7 +1600,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2146,7 +2118,7 @@
   </sheetPr>
   <dimension ref="B1:E17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -2310,7 +2282,7 @@
     <mergeCell ref="B9:E9"/>
   </mergeCells>
   <conditionalFormatting sqref="D7">
-    <cfRule type="timePeriod" dxfId="38" priority="3" timePeriod="lastMonth">
+    <cfRule type="timePeriod" dxfId="34" priority="3" timePeriod="lastMonth">
       <formula>AND(MONTH(D7)=MONTH(EDATE(TODAY(),0-1)),YEAR(D7)=YEAR(EDATE(TODAY(),0-1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2660,12 +2632,12 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-tblHoras[[#This Row],[Jornada Diária]], IF(OR(
 IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-tblHoras[[#This Row],[Jornada Diária]]/2,0
 )))</f>
         <v>0</v>
       </c>
@@ -7042,7 +7014,7 @@
     <row r="46" spans="2:21" x14ac:dyDescent="0.25"/>
     <row r="47" spans="2:21" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="OJxlQuhkIK9DNQCfOeWlZSqh2aIz5odm13SvrssWqxZYUX8mYET4ZE5CBuBYwVJJtfqQ19yCfn2pTGripuycTQ==" saltValue="YbBgYVvS1sYOZF1u4p0+0A==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" selectLockedCells="1" autoFilter="0" pivotTables="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="YndaWR3aiSwmSi7G/PmgMxOOjliJrxilCxiCl/r5wArvd+pdaQsPSxpSdTqj5W+uAz+x1jfgeB3eaY6t6XrM4Q==" saltValue="4RzjfPDoa1Y6V3lY+eKnIQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" selectLockedCells="1" autoFilter="0" pivotTables="0"/>
   <dataConsolidate/>
   <mergeCells count="7">
     <mergeCell ref="P6:S6"/>

</xml_diff>

<commit_message>
Horas em Decimais para contabilidade
</commit_message>
<xml_diff>
--- a/Controle de Ponto.xlsx
+++ b/Controle de Ponto.xlsx
@@ -5,7 +5,7 @@
   <workbookPr date1904="1" codeName="EstaPasta_de_trabalho" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m362168\OneDrive\Projetos\ExcelGuru\Controle de Ponto\controle-de-ponto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\Controle de Ponto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="104">
   <si>
     <t>Data</t>
   </si>
@@ -399,7 +399,19 @@
     <t>Desenvolvido e distribuído por:</t>
   </si>
   <si>
-    <t>v7.2</t>
+    <t>Saldo de Horas (Decimal)</t>
+  </si>
+  <si>
+    <t>Atrasos (Decimal)</t>
+  </si>
+  <si>
+    <t>Hora Extra Normal (Decimal)</t>
+  </si>
+  <si>
+    <t>Hora Extra Especial (Decimal)</t>
+  </si>
+  <si>
+    <t>v7.3</t>
   </si>
 </sst>
 </file>
@@ -521,7 +533,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -556,6 +568,18 @@
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor theme="6" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="6" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -743,7 +767,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -944,12 +968,51 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="1" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="51">
+  <dxfs count="61">
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
     <dxf>
       <font>
         <i/>
@@ -978,12 +1041,124 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD5D6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD1D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD5D6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD1D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="167" formatCode="[h]:mm"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="167" formatCode="[h]:mm"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
     </dxf>
@@ -1101,55 +1276,6 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD5D6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD1D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD5D6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD1D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="166" formatCode="h:mm;@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
@@ -1173,16 +1299,6 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1301,72 +1417,72 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tblEvento" displayName="tblEvento" ref="A2:F13" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tblEvento" displayName="tblEvento" ref="A2:F13" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
   <sortState ref="A3:F13">
     <sortCondition ref="A8"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="Evento" dataDxfId="48"/>
-    <tableColumn id="2" name="Colorir Linha" dataDxfId="47"/>
-    <tableColumn id="5" name="Colorir Período" dataDxfId="46"/>
-    <tableColumn id="6" name="Libera o Período" dataDxfId="45"/>
-    <tableColumn id="4" name="Conta hora Extra" dataDxfId="44"/>
-    <tableColumn id="3" name="Descrição" dataDxfId="43"/>
+    <tableColumn id="1" name="Evento" dataDxfId="58"/>
+    <tableColumn id="2" name="Colorir Linha" dataDxfId="57"/>
+    <tableColumn id="5" name="Colorir Período" dataDxfId="56"/>
+    <tableColumn id="6" name="Libera o Período" dataDxfId="55"/>
+    <tableColumn id="4" name="Conta hora Extra" dataDxfId="54"/>
+    <tableColumn id="3" name="Descrição" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="tblLimiteHora" displayName="tblLimiteHora" ref="H2:J4" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="tblLimiteHora" displayName="tblLimiteHora" ref="H2:J4" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
   <autoFilter ref="H2:J4"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Limite de horas" dataDxfId="40"/>
-    <tableColumn id="3" name="Limite" dataDxfId="39"/>
-    <tableColumn id="2" name="h" dataDxfId="38"/>
+    <tableColumn id="1" name="Limite de horas" dataDxfId="50"/>
+    <tableColumn id="3" name="Limite" dataDxfId="49"/>
+    <tableColumn id="2" name="h" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="tbl_Mes" displayName="tbl_Mes" ref="L2:L14" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="tbl_Mes" displayName="tbl_Mes" ref="L2:L14" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="L2:L14"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Mês" dataDxfId="35"/>
+    <tableColumn id="1" name="Mês" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tblDiaUtil" displayName="tblDiaUtil" ref="B10:E17" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tblDiaUtil" displayName="tblDiaUtil" ref="B10:E17" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
   <tableColumns count="4">
-    <tableColumn id="1" name="Dia da Semana" dataDxfId="31"/>
-    <tableColumn id="4" name="Abreviatura" dataDxfId="30"/>
-    <tableColumn id="2" name="É dia util?" dataDxfId="29"/>
-    <tableColumn id="3" name="Jornada Diferenciada?" dataDxfId="28"/>
+    <tableColumn id="1" name="Dia da Semana" dataDxfId="42"/>
+    <tableColumn id="4" name="Abreviatura" dataDxfId="41"/>
+    <tableColumn id="2" name="É dia util?" dataDxfId="40"/>
+    <tableColumn id="3" name="Jornada Diferenciada?" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblHoras" displayName="tblHoras" ref="B8:T39" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <tableColumns count="19">
-    <tableColumn id="1" name="Data" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblHoras" displayName="tblHoras" ref="B8:X39" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+  <tableColumns count="23">
+    <tableColumn id="1" name="Data" dataDxfId="36">
       <calculatedColumnFormula>IF(B8&lt;&gt;"",IF(DAY(B8+1)=1,"",B8+1),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Dia" dataDxfId="17">
+    <tableColumn id="2" name="Dia" dataDxfId="35">
       <calculatedColumnFormula>TEXT(tblHoras[[#This Row],[Data]],"ddd")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Evento _x000a_(1º Período)" dataDxfId="16"/>
-    <tableColumn id="4" name="Entrada - 1" dataDxfId="15"/>
-    <tableColumn id="5" name="Saída - 1 (Almoço)" dataDxfId="14"/>
-    <tableColumn id="6" name="Entrada - 2 (Almoço)" dataDxfId="13"/>
-    <tableColumn id="7" name="Saída - 2" dataDxfId="12"/>
-    <tableColumn id="13" name="Evento _x000a_(2º Período)" dataDxfId="11"/>
-    <tableColumn id="15" name="Horas Trabalhadas (1º Período)" dataDxfId="10">
+    <tableColumn id="3" name="Evento _x000a_(1º Período)" dataDxfId="34"/>
+    <tableColumn id="4" name="Entrada - 1" dataDxfId="33"/>
+    <tableColumn id="5" name="Saída - 1 (Almoço)" dataDxfId="32"/>
+    <tableColumn id="6" name="Entrada - 2 (Almoço)" dataDxfId="31"/>
+    <tableColumn id="7" name="Saída - 2" dataDxfId="30"/>
+    <tableColumn id="13" name="Evento _x000a_(2º Período)" dataDxfId="29"/>
+    <tableColumn id="15" name="Horas Trabalhadas (1º Período)" dataDxfId="28">
       <calculatedColumnFormula>IF($B$6&lt;&gt;"",IF(AND(tblHoras[[#This Row],[Evento 
 (1º Período)]]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[[#This Row],[Evento 
 (1º Período)]],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[[#This Row],[Evento 
@@ -1383,7 +1499,7 @@
                           0)),
                     0)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Horas Trabalhadas (2º Período)" dataDxfId="9">
+    <tableColumn id="16" name="Horas Trabalhadas (2º Período)" dataDxfId="27">
       <calculatedColumnFormula>IF($B$6&lt;&gt;"",IF(AND(tblHoras[[#This Row],[Evento 
 (2º Período)]]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[[#This Row],[Evento 
 (2º Período)]],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[[#This Row],[Evento 
@@ -1400,10 +1516,10 @@
                          0)),
        0)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Horas Trabalhadas" dataDxfId="8">
+    <tableColumn id="8" name="Horas Trabalhadas" dataDxfId="26">
       <calculatedColumnFormula>tblHoras[[#This Row],[Horas Trabalhadas (1º Período)]]+tblHoras[[#This Row],[Horas Trabalhadas (2º Período)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Jornada Diária" dataDxfId="7">
+    <tableColumn id="17" name="Jornada Diária" dataDxfId="25">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Data]]&lt;&gt;"",
         IF(
 AND(VLOOKUP(TEXT(tblHoras[[#This Row],[Data]],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[[#This Row],[Evento 
@@ -1415,7 +1531,7 @@
               ""),
          "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Horas Trabalhadas Além Jornada" dataDxfId="6">
+    <tableColumn id="11" name="Horas Trabalhadas Além Jornada" dataDxfId="24">
       <calculatedColumnFormula>IF(OR(tblHoras[[#This Row],[Horas Trabalhadas (1º Período)]]&lt;&gt;0,tblHoras[[#This Row],[Horas Trabalhadas (2º Período)]]&lt;&gt;0),
         IF(ISNUMBER(tblHoras[[#This Row],[Jornada Diária]]),
               IF(tblHoras[[#This Row],[Jornada Diária]]&gt;(tblHoras[[#This Row],[Horas Trabalhadas (2º Período)]]+tblHoras[[#This Row],[Horas Trabalhadas (1º Período)]]),
@@ -1438,7 +1554,7 @@
 (2º Período)]],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
 )))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Saldo de Horas" dataDxfId="5">
+    <tableColumn id="18" name="Saldo de Horas" dataDxfId="23">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&gt;0,
         IF(tblHoras[[#This Row],[Jornada Diária]]&lt;&gt;"",
               IF(HOUR(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]])&gt;=VLOOKUP(LIMITE,tblLimiteHora[],Tabelas!$I$1,FALSE),
@@ -1447,15 +1563,23 @@
               tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]),
         0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="Atrasos_x000a_(horas)" dataDxfId="4">
+    <tableColumn id="20" name="Saldo de Horas (Decimal)" dataDxfId="22">
+      <calculatedColumnFormula>tblHoras[[#This Row],[Saldo de Horas]]*24</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="19" name="Atrasos_x000a_(horas)" dataDxfId="21">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&lt;0,IF(OR(tblHoras[[#This Row],[Evento 
 (1º Período)]]="",tblHoras[[#This Row],[Evento 
 (2º Período)]]=""),tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]],""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Faltas_x000a_(dias)" dataDxfId="3">
+    <tableColumn id="21" name="Atrasos (Decimal)" dataDxfId="2">
+      <calculatedColumnFormula>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="14" name="Faltas_x000a_(dias)" dataDxfId="20">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Jornada Diária]]&lt;&gt;"",IF((N(tblHoras[[#This Row],[Jornada Diária]])-ABS(N(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]])))=0,1,""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Hora Extra Normal" dataDxfId="2">
+    <tableColumn id="10" name="Hora Extra Normal" dataDxfId="5">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[[#This Row],[Data]],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[[#This Row],[Evento 
 (1º Período)]]&lt;&gt;"",IF(VLOOKUP(tblHoras[[#This Row],[Evento 
@@ -1464,7 +1588,10 @@
 (2º Período)]],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
 tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]],""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Hora Extra _x000a_Especial" dataDxfId="1">
+    <tableColumn id="22" name="Hora Extra Normal (Decimal)" dataDxfId="1">
+      <calculatedColumnFormula>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" name="Hora Extra _x000a_Especial" dataDxfId="4">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[[#This Row],[Data]],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[[#This Row],[Evento 
 (1º Período)]]&lt;&gt;"",IF(VLOOKUP(tblHoras[[#This Row],[Evento 
@@ -1473,7 +1600,12 @@
 (2º Período)]],tblEvento[],Tabelas!$E$1,FALSE)="Sim",TRUE,FALSE),FALSE)),
 tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]],""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Informação" dataDxfId="0">
+    <tableColumn id="23" name="Hora Extra Especial (Decimal)" dataDxfId="0">
+      <calculatedColumnFormula>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="12" name="Informação" dataDxfId="3">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Evento 
 (1º Período)]]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[[#This Row],[Evento 
 (1º Período)]],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[[#This Row],[Evento 
@@ -1756,7 +1888,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2119,7 +2251,7 @@
   <dimension ref="B1:E17"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2282,7 +2414,7 @@
     <mergeCell ref="B9:E9"/>
   </mergeCells>
   <conditionalFormatting sqref="D7">
-    <cfRule type="timePeriod" dxfId="34" priority="3" timePeriod="lastMonth">
+    <cfRule type="timePeriod" dxfId="19" priority="3" timePeriod="lastMonth">
       <formula>AND(MONTH(D7)=MONTH(EDATE(TODAY(),0-1)),YEAR(D7)=YEAR(EDATE(TODAY(),0-1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2308,7 +2440,7 @@
     <tabColor theme="4" tint="0.59999389629810485"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC47"/>
+  <dimension ref="A1:AG47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
@@ -2326,19 +2458,25 @@
     <col min="4" max="9" width="12.7109375" style="5" customWidth="1"/>
     <col min="10" max="14" width="12.7109375" style="5" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="12.7109375" style="5" customWidth="1"/>
-    <col min="16" max="19" width="12.7109375" style="5" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="38.42578125" style="5" customWidth="1"/>
-    <col min="21" max="21" width="2.7109375" style="5" customWidth="1"/>
-    <col min="22" max="22" width="9.140625" style="5" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="12.42578125" style="5" hidden="1" customWidth="1"/>
-    <col min="24" max="25" width="0" style="5" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" style="5" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" style="5" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" style="5" hidden="1" customWidth="1"/>
+    <col min="19" max="20" width="12.7109375" style="5" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" style="5" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="12.7109375" style="5" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="10.7109375" style="5" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="38.42578125" style="5" customWidth="1"/>
+    <col min="25" max="25" width="2.7109375" style="5" customWidth="1"/>
     <col min="26" max="26" width="9.140625" style="5" hidden="1" customWidth="1"/>
     <col min="27" max="27" width="12.42578125" style="5" hidden="1" customWidth="1"/>
     <col min="28" max="29" width="0" style="5" hidden="1" customWidth="1"/>
-    <col min="30" max="16384" width="9.140625" style="5" hidden="1"/>
+    <col min="30" max="30" width="9.140625" style="5" hidden="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="5" hidden="1" customWidth="1"/>
+    <col min="32" max="33" width="0" style="5" hidden="1" customWidth="1"/>
+    <col min="34" max="16384" width="9.140625" style="5" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G1" s="29" t="s">
         <v>58</v>
       </c>
@@ -2355,8 +2493,12 @@
       <c r="R1" s="58"/>
       <c r="S1" s="58"/>
       <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="58"/>
+      <c r="X1" s="58"/>
     </row>
-    <row r="2" spans="2:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:29" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="6"/>
       <c r="G2" s="65"/>
       <c r="H2" s="66"/>
@@ -2368,8 +2510,12 @@
       <c r="R2" s="58"/>
       <c r="S2" s="58"/>
       <c r="T2" s="58"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="58"/>
+      <c r="W2" s="58"/>
+      <c r="X2" s="58"/>
     </row>
-    <row r="3" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
       <c r="G3" s="45" t="s">
         <v>96</v>
@@ -2385,8 +2531,12 @@
       <c r="R3" s="58"/>
       <c r="S3" s="58"/>
       <c r="T3" s="58"/>
+      <c r="U3" s="58"/>
+      <c r="V3" s="58"/>
+      <c r="W3" s="58"/>
+      <c r="X3" s="58"/>
     </row>
-    <row r="4" spans="2:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:29" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6"/>
       <c r="G4" s="46"/>
       <c r="H4" s="59"/>
@@ -2398,8 +2548,12 @@
       <c r="R4" s="58"/>
       <c r="S4" s="58"/>
       <c r="T4" s="58"/>
+      <c r="U4" s="58"/>
+      <c r="V4" s="58"/>
+      <c r="W4" s="58"/>
+      <c r="X4" s="58"/>
     </row>
-    <row r="5" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="61" t="s">
         <v>59</v>
       </c>
@@ -2413,9 +2567,7 @@
       <c r="G5" s="7"/>
       <c r="N5" s="24"/>
       <c r="O5" s="24"/>
-      <c r="P5" s="35" t="s">
-        <v>76</v>
-      </c>
+      <c r="P5" s="24"/>
       <c r="Q5" s="35" t="s">
         <v>76</v>
       </c>
@@ -2425,9 +2577,21 @@
       <c r="S5" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="T5" s="24"/>
+      <c r="T5" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="U5" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="V5" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="W5" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="X5" s="24"/>
     </row>
-    <row r="6" spans="2:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:29" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="63"/>
       <c r="C6" s="64"/>
       <c r="D6" s="31"/>
@@ -2438,15 +2602,19 @@
       </c>
       <c r="N6" s="24"/>
       <c r="O6" s="24"/>
-      <c r="P6" s="56" t="s">
+      <c r="P6" s="24"/>
+      <c r="Q6" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="Q6" s="57"/>
       <c r="R6" s="57"/>
       <c r="S6" s="57"/>
-      <c r="T6" s="24"/>
+      <c r="T6" s="57"/>
+      <c r="U6" s="57"/>
+      <c r="V6" s="57"/>
+      <c r="W6" s="57"/>
+      <c r="X6" s="24"/>
     </row>
-    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:29" x14ac:dyDescent="0.25">
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
@@ -2467,29 +2635,45 @@
       <c r="N7" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="O7" s="24"/>
-      <c r="P7" s="47">
+      <c r="O7" s="47">
+        <f>O39</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="69">
+        <f>P39</f>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="47">
         <f>SUM(tblHoras[Atrasos
 (horas)])</f>
         <v>0</v>
       </c>
-      <c r="Q7" s="48">
+      <c r="R7" s="69">
+        <f>SUM(tblHoras[Atrasos (Decimal)])</f>
+        <v>0</v>
+      </c>
+      <c r="S7" s="48">
         <f>SUM(tblHoras[Faltas
 (dias)])</f>
         <v>0</v>
       </c>
-      <c r="R7" s="47">
+      <c r="T7" s="47">
         <f>SUM(tblHoras[Hora Extra Normal])</f>
         <v>0</v>
       </c>
-      <c r="S7" s="47">
+      <c r="U7" s="69"/>
+      <c r="V7" s="47">
         <f>SUM(tblHoras[Hora Extra 
 Especial])</f>
         <v>0</v>
       </c>
-      <c r="T7" s="24"/>
+      <c r="W7" s="69">
+        <f>SUM(tblHoras[Hora Extra Especial (Decimal)])</f>
+        <v>0</v>
+      </c>
+      <c r="X7" s="24"/>
     </row>
-    <row r="8" spans="2:25" s="9" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:29" s="9" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
         <v>0</v>
       </c>
@@ -2533,23 +2717,35 @@
         <v>49</v>
       </c>
       <c r="P8" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q8" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="Q8" s="9" t="s">
+      <c r="R8" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="S8" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="R8" s="9" t="s">
+      <c r="T8" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="S8" s="9" t="s">
+      <c r="U8" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="V8" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="T8" s="9" t="s">
+      <c r="W8" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="X8" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="W8" s="27"/>
+      <c r="AA8" s="27"/>
     </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="str">
         <f>IF(ISERROR(F6),"",F6)</f>
         <v/>
@@ -2651,17 +2847,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])</f>
         <v>0</v>
       </c>
-      <c r="P9" s="14" t="str">
+      <c r="P9" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q9" s="14" t="str">
+      <c r="R9" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S9" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R9" s="14" t="str">
+      <c r="T9" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -2671,7 +2877,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S9" s="14" t="str">
+      <c r="U9" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V9" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -2681,7 +2891,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T9" s="15" t="str">
+      <c r="W9" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X9" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -2691,10 +2907,10 @@
 (2º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")</f>
         <v/>
       </c>
-      <c r="V9" s="16"/>
-      <c r="Y9" s="17"/>
+      <c r="Z9" s="16"/>
+      <c r="AC9" s="17"/>
     </row>
-    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="str">
         <f>IF(B9&lt;&gt;"",IF(DAY(B9+1)=IF($E$6&lt;&gt;"",$E$6,1),"",B9+1),"")</f>
         <v/>
@@ -2796,17 +3012,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O9</f>
         <v>0</v>
       </c>
-      <c r="P10" s="14" t="str">
+      <c r="P10" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q10" s="14" t="str">
+      <c r="R10" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S10" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R10" s="14" t="str">
+      <c r="T10" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -2816,7 +3042,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S10" s="14" t="str">
+      <c r="U10" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V10" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -2826,7 +3056,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T10" s="15" t="str">
+      <c r="W10" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X10" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -2836,9 +3072,9 @@
 (2º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")</f>
         <v/>
       </c>
-      <c r="Y10" s="17"/>
+      <c r="AC10" s="17"/>
     </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="str">
         <f t="shared" ref="B11:B39" si="0">IF(B10&lt;&gt;"",IF(DAY(B10+1)=IF($E$6&lt;&gt;"",$E$6,1),"",B10+1),"")</f>
         <v/>
@@ -2940,17 +3176,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O10</f>
         <v>0</v>
       </c>
-      <c r="P11" s="14" t="str">
+      <c r="P11" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q11" s="14" t="str">
+      <c r="R11" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S11" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R11" s="14" t="str">
+      <c r="T11" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -2960,7 +3206,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S11" s="14" t="str">
+      <c r="U11" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V11" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -2970,7 +3220,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T11" s="15" t="str">
+      <c r="W11" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X11" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -2981,7 +3237,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3083,17 +3339,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O11</f>
         <v>0</v>
       </c>
-      <c r="P12" s="14" t="str">
+      <c r="P12" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q12" s="14" t="str">
+      <c r="R12" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S12" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R12" s="14" t="str">
+      <c r="T12" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -3103,7 +3369,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S12" s="14" t="str">
+      <c r="U12" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V12" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -3113,7 +3383,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T12" s="15" t="str">
+      <c r="W12" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X12" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -3124,7 +3400,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3226,17 +3502,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O12</f>
         <v>0</v>
       </c>
-      <c r="P13" s="14" t="str">
+      <c r="P13" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q13" s="14" t="str">
+      <c r="R13" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S13" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R13" s="14" t="str">
+      <c r="T13" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -3246,7 +3532,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S13" s="14" t="str">
+      <c r="U13" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V13" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -3256,7 +3546,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T13" s="15" t="str">
+      <c r="W13" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X13" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -3267,7 +3563,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3369,17 +3665,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O13</f>
         <v>0</v>
       </c>
-      <c r="P14" s="14" t="str">
+      <c r="P14" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q14" s="14" t="str">
+      <c r="R14" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S14" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R14" s="14" t="str">
+      <c r="T14" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -3389,7 +3695,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S14" s="14" t="str">
+      <c r="U14" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V14" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -3399,7 +3709,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T14" s="15" t="str">
+      <c r="W14" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X14" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -3409,10 +3725,10 @@
 (2º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")</f>
         <v/>
       </c>
-      <c r="X14" s="18"/>
-      <c r="Y14" s="18"/>
+      <c r="AB14" s="18"/>
+      <c r="AC14" s="18"/>
     </row>
-    <row r="15" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3514,17 +3830,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O14</f>
         <v>0</v>
       </c>
-      <c r="P15" s="14" t="str">
+      <c r="P15" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q15" s="14" t="str">
+      <c r="R15" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S15" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R15" s="14" t="str">
+      <c r="T15" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -3534,7 +3860,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S15" s="14" t="str">
+      <c r="U15" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V15" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -3544,7 +3874,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T15" s="15" t="str">
+      <c r="W15" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X15" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -3554,9 +3890,9 @@
 (2º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")</f>
         <v/>
       </c>
-      <c r="X15" s="17"/>
+      <c r="AB15" s="17"/>
     </row>
-    <row r="16" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3658,17 +3994,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O15</f>
         <v>0</v>
       </c>
-      <c r="P16" s="14" t="str">
+      <c r="P16" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q16" s="14" t="str">
+      <c r="R16" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S16" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R16" s="14" t="str">
+      <c r="T16" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -3678,7 +4024,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S16" s="14" t="str">
+      <c r="U16" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V16" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -3688,7 +4038,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T16" s="15" t="str">
+      <c r="W16" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X16" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -3699,7 +4055,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3801,17 +4157,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O16</f>
         <v>0</v>
       </c>
-      <c r="P17" s="14" t="str">
+      <c r="P17" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q17" s="14" t="str">
+      <c r="R17" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S17" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R17" s="14" t="str">
+      <c r="T17" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -3821,7 +4187,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S17" s="14" t="str">
+      <c r="U17" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V17" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -3831,7 +4201,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T17" s="15" t="str">
+      <c r="W17" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X17" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -3842,7 +4218,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B18" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3944,17 +4320,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O17</f>
         <v>0</v>
       </c>
-      <c r="P18" s="14" t="str">
+      <c r="P18" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q18" s="14" t="str">
+      <c r="R18" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S18" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R18" s="14" t="str">
+      <c r="T18" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -3964,7 +4350,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S18" s="14" t="str">
+      <c r="U18" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V18" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -3974,7 +4364,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T18" s="15" t="str">
+      <c r="W18" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X18" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -3985,7 +4381,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -4087,17 +4483,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O18</f>
         <v>0</v>
       </c>
-      <c r="P19" s="14" t="str">
+      <c r="P19" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q19" s="14" t="str">
+      <c r="R19" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S19" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R19" s="14" t="str">
+      <c r="T19" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -4107,7 +4513,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S19" s="14" t="str">
+      <c r="U19" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V19" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -4117,7 +4527,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T19" s="15" t="str">
+      <c r="W19" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X19" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -4128,7 +4544,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B20" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -4230,17 +4646,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O19</f>
         <v>0</v>
       </c>
-      <c r="P20" s="14" t="str">
+      <c r="P20" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q20" s="14" t="str">
+      <c r="R20" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S20" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R20" s="14" t="str">
+      <c r="T20" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -4250,7 +4676,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S20" s="14" t="str">
+      <c r="U20" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V20" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -4260,7 +4690,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T20" s="15" t="str">
+      <c r="W20" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X20" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -4271,7 +4707,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B21" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -4373,17 +4809,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O20</f>
         <v>0</v>
       </c>
-      <c r="P21" s="14" t="str">
+      <c r="P21" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q21" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q21" s="14" t="str">
+      <c r="R21" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S21" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R21" s="14" t="str">
+      <c r="T21" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -4393,7 +4839,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S21" s="14" t="str">
+      <c r="U21" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V21" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -4403,7 +4853,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T21" s="15" t="str">
+      <c r="W21" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X21" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -4414,7 +4870,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -4516,17 +4972,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O21</f>
         <v>0</v>
       </c>
-      <c r="P22" s="14" t="str">
+      <c r="P22" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q22" s="14" t="str">
+      <c r="R22" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S22" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R22" s="14" t="str">
+      <c r="T22" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -4536,7 +5002,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S22" s="14" t="str">
+      <c r="U22" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V22" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -4546,7 +5016,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T22" s="15" t="str">
+      <c r="W22" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X22" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -4557,7 +5033,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B23" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -4659,17 +5135,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O22</f>
         <v>0</v>
       </c>
-      <c r="P23" s="14" t="str">
+      <c r="P23" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q23" s="14" t="str">
+      <c r="R23" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S23" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R23" s="14" t="str">
+      <c r="T23" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -4679,7 +5165,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S23" s="14" t="str">
+      <c r="U23" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V23" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -4689,7 +5179,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T23" s="15" t="str">
+      <c r="W23" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X23" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -4700,7 +5196,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B24" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -4802,17 +5298,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O23</f>
         <v>0</v>
       </c>
-      <c r="P24" s="14" t="str">
+      <c r="P24" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q24" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q24" s="14" t="str">
+      <c r="R24" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S24" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R24" s="14" t="str">
+      <c r="T24" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -4822,7 +5328,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S24" s="14" t="str">
+      <c r="U24" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V24" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -4832,7 +5342,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T24" s="15" t="str">
+      <c r="W24" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X24" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -4843,7 +5359,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B25" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -4945,17 +5461,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O24</f>
         <v>0</v>
       </c>
-      <c r="P25" s="14" t="str">
+      <c r="P25" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q25" s="14" t="str">
+      <c r="R25" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S25" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R25" s="14" t="str">
+      <c r="T25" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -4965,7 +5491,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S25" s="14" t="str">
+      <c r="U25" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V25" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -4975,7 +5505,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T25" s="15" t="str">
+      <c r="W25" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X25" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -4986,7 +5522,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B26" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -5088,17 +5624,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O25</f>
         <v>0</v>
       </c>
-      <c r="P26" s="14" t="str">
+      <c r="P26" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q26" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q26" s="14" t="str">
+      <c r="R26" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S26" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R26" s="14" t="str">
+      <c r="T26" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -5108,7 +5654,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S26" s="14" t="str">
+      <c r="U26" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V26" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -5118,7 +5668,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T26" s="15" t="str">
+      <c r="W26" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X26" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -5129,7 +5685,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B27" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -5231,17 +5787,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O26</f>
         <v>0</v>
       </c>
-      <c r="P27" s="14" t="str">
+      <c r="P27" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q27" s="14" t="str">
+      <c r="R27" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S27" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R27" s="14" t="str">
+      <c r="T27" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -5251,7 +5817,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S27" s="14" t="str">
+      <c r="U27" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V27" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -5261,7 +5831,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T27" s="15" t="str">
+      <c r="W27" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X27" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -5272,7 +5848,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B28" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -5374,17 +5950,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O27</f>
         <v>0</v>
       </c>
-      <c r="P28" s="14" t="str">
+      <c r="P28" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q28" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q28" s="14" t="str">
+      <c r="R28" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S28" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R28" s="14" t="str">
+      <c r="T28" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -5394,7 +5980,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S28" s="14" t="str">
+      <c r="U28" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V28" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -5404,7 +5994,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T28" s="15" t="str">
+      <c r="W28" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X28" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -5415,7 +6011,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B29" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -5517,17 +6113,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O28</f>
         <v>0</v>
       </c>
-      <c r="P29" s="14" t="str">
+      <c r="P29" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q29" s="14" t="str">
+      <c r="R29" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S29" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R29" s="14" t="str">
+      <c r="T29" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -5537,7 +6143,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S29" s="14" t="str">
+      <c r="U29" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V29" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -5547,7 +6157,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T29" s="15" t="str">
+      <c r="W29" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X29" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -5558,7 +6174,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B30" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -5660,17 +6276,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O29</f>
         <v>0</v>
       </c>
-      <c r="P30" s="14" t="str">
+      <c r="P30" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q30" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q30" s="14" t="str">
+      <c r="R30" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S30" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R30" s="14" t="str">
+      <c r="T30" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -5680,7 +6306,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S30" s="14" t="str">
+      <c r="U30" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V30" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -5690,7 +6320,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T30" s="15" t="str">
+      <c r="W30" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X30" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -5701,7 +6337,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B31" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -5803,17 +6439,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O30</f>
         <v>0</v>
       </c>
-      <c r="P31" s="14" t="str">
+      <c r="P31" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q31" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q31" s="14" t="str">
+      <c r="R31" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S31" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R31" s="14" t="str">
+      <c r="T31" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -5823,7 +6469,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S31" s="14" t="str">
+      <c r="U31" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V31" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -5833,7 +6483,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T31" s="15" t="str">
+      <c r="W31" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X31" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -5844,7 +6500,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B32" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -5946,17 +6602,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O31</f>
         <v>0</v>
       </c>
-      <c r="P32" s="14" t="str">
+      <c r="P32" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q32" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q32" s="14" t="str">
+      <c r="R32" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S32" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R32" s="14" t="str">
+      <c r="T32" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -5966,7 +6632,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S32" s="14" t="str">
+      <c r="U32" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V32" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -5976,7 +6646,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T32" s="15" t="str">
+      <c r="W32" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X32" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -5987,7 +6663,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B33" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6089,17 +6765,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O32</f>
         <v>0</v>
       </c>
-      <c r="P33" s="14" t="str">
+      <c r="P33" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q33" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q33" s="14" t="str">
+      <c r="R33" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S33" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R33" s="14" t="str">
+      <c r="T33" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -6109,7 +6795,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S33" s="14" t="str">
+      <c r="U33" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V33" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -6119,7 +6809,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T33" s="15" t="str">
+      <c r="W33" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X33" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -6130,7 +6826,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B34" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6232,17 +6928,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O33</f>
         <v>0</v>
       </c>
-      <c r="P34" s="14" t="str">
+      <c r="P34" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q34" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q34" s="14" t="str">
+      <c r="R34" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S34" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R34" s="14" t="str">
+      <c r="T34" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -6252,7 +6958,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S34" s="14" t="str">
+      <c r="U34" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V34" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -6262,7 +6972,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T34" s="15" t="str">
+      <c r="W34" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X34" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -6273,7 +6989,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B35" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6375,17 +7091,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O34</f>
         <v>0</v>
       </c>
-      <c r="P35" s="14" t="str">
+      <c r="P35" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q35" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q35" s="14" t="str">
+      <c r="R35" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S35" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R35" s="14" t="str">
+      <c r="T35" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -6395,7 +7121,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S35" s="14" t="str">
+      <c r="U35" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V35" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -6405,7 +7135,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T35" s="15" t="str">
+      <c r="W35" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X35" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -6416,7 +7152,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B36" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6518,17 +7254,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O35</f>
         <v>0</v>
       </c>
-      <c r="P36" s="14" t="str">
+      <c r="P36" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q36" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q36" s="14" t="str">
+      <c r="R36" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S36" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R36" s="14" t="str">
+      <c r="T36" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -6538,7 +7284,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S36" s="14" t="str">
+      <c r="U36" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V36" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -6548,7 +7298,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T36" s="15" t="str">
+      <c r="W36" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X36" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -6559,7 +7315,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B37" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6661,17 +7417,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O36</f>
         <v>0</v>
       </c>
-      <c r="P37" s="14" t="str">
+      <c r="P37" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q37" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q37" s="14" t="str">
+      <c r="R37" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S37" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R37" s="14" t="str">
+      <c r="T37" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -6681,7 +7447,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S37" s="14" t="str">
+      <c r="U37" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V37" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -6691,7 +7461,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T37" s="15" t="str">
+      <c r="W37" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X37" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -6702,7 +7478,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B38" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6804,17 +7580,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O37</f>
         <v>0</v>
       </c>
-      <c r="P38" s="14" t="str">
+      <c r="P38" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q38" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q38" s="14" t="str">
+      <c r="R38" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S38" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R38" s="14" t="str">
+      <c r="T38" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -6824,7 +7610,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S38" s="14" t="str">
+      <c r="U38" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V38" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -6834,7 +7624,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T38" s="15" t="str">
+      <c r="W38" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X38" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -6845,7 +7641,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B39" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6947,17 +7743,27 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O38</f>
         <v>0</v>
       </c>
-      <c r="P39" s="14" t="str">
+      <c r="P39" s="70">
+        <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
+        <v>0</v>
+      </c>
+      <c r="Q39" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="Q39" s="14" t="str">
+      <c r="R39" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Atrasos
+(horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
+(horas)]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="S39" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="R39" s="14" t="str">
+      <c r="T39" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -6967,7 +7773,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="S39" s="14" t="str">
+      <c r="U39" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="V39" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -6977,7 +7787,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="T39" s="15" t="str">
+      <c r="W39" s="70" t="str">
+        <f>IF(tblHoras[[#This Row],[Hora Extra 
+Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
+Especial]]*24,"")</f>
+        <v/>
+      </c>
+      <c r="X39" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -6988,42 +7804,42 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:21" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="T40" s="24"/>
-      <c r="U40" s="24"/>
+    <row r="40" spans="2:25" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X40" s="24"/>
+      <c r="Y40" s="24"/>
     </row>
-    <row r="41" spans="2:21" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="T41" s="36" t="s">
-        <v>99</v>
-      </c>
-      <c r="U41" s="24"/>
+    <row r="41" spans="2:25" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X41" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y41" s="24"/>
     </row>
-    <row r="42" spans="2:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="T42" s="24"/>
-      <c r="U42" s="24"/>
+    <row r="42" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="X42" s="24"/>
+      <c r="Y42" s="24"/>
     </row>
-    <row r="43" spans="2:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="T43" s="24"/>
-      <c r="U43" s="24"/>
+    <row r="43" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="X43" s="24"/>
+      <c r="Y43" s="24"/>
     </row>
-    <row r="44" spans="2:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="T44" s="24"/>
-      <c r="U44" s="24"/>
+    <row r="44" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="X44" s="24"/>
+      <c r="Y44" s="24"/>
     </row>
-    <row r="45" spans="2:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="2:21" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="2:21" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="2:25" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:25" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="2:25" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="YndaWR3aiSwmSi7G/PmgMxOOjliJrxilCxiCl/r5wArvd+pdaQsPSxpSdTqj5W+uAz+x1jfgeB3eaY6t6XrM4Q==" saltValue="4RzjfPDoa1Y6V3lY+eKnIQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" selectLockedCells="1" autoFilter="0" pivotTables="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="PBwt9+JEYjlkiRwfKHy7xOwI4p9n1mffdrLoaKYA6avPryUjvYoQx0p1kLbn75QAdFf/hB21Do9/OwxyFwBRIg==" saltValue="M6RP+xkThEPESs4iK9SW+w==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" selectLockedCells="1" autoFilter="0" pivotTables="0"/>
   <dataConsolidate/>
   <mergeCells count="7">
-    <mergeCell ref="P6:S6"/>
-    <mergeCell ref="O1:T4"/>
+    <mergeCell ref="O1:X4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="H3:I3"/>
+    <mergeCell ref="Q6:W6"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Aviso" error="Erro na inserção de dados:_x000a__x000a_'Hora Inválida'_x000a__x000a_Favor inserir uma hora válida no formato: hh:mm (ex. 12:00)" sqref="E9:H39">
@@ -7059,7 +7875,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="14" id="{33616478-990B-44FE-BB07-40117DF3ADA1}">
+          <x14:cfRule type="expression" priority="20" id="{33616478-990B-44FE-BB07-40117DF3ADA1}">
             <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C9,Config!$C$1:$D$17,2,FALSE)),FALSE,IF(VLOOKUP($C9,Config!$C$1:$D$17,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D9,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D9,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I9,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I9,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
             <x14:dxf>
               <fill>
@@ -7069,10 +7885,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B9:T9</xm:sqref>
+          <xm:sqref>B9:X9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="11" id="{D79C2469-95B2-4490-A707-5C27A171E816}">
+          <x14:cfRule type="expression" priority="17" id="{D79C2469-95B2-4490-A707-5C27A171E816}">
             <xm:f>IF(IF(ISERROR(VLOOKUP($D9,Tabelas!$A$3:$C$51,3,FALSE)),FALSE,VLOOKUP($D9,Tabelas!$A$3:$C$51,3,FALSE)="Sim"),TRUE,FALSE)</xm:f>
             <x14:dxf>
               <fill>
@@ -7085,7 +7901,7 @@
           <xm:sqref>J9 D9:F9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="17" id="{31CF979C-12F0-4F54-B477-D65B5CC060E6}">
+          <x14:cfRule type="expression" priority="23" id="{31CF979C-12F0-4F54-B477-D65B5CC060E6}">
             <xm:f>IF(IF(ISERROR(VLOOKUP($I9,Tabelas!$A$3:$C$51,3,FALSE)),FALSE,VLOOKUP($I9,Tabelas!$A$3:$C$51,3,FALSE)="Sim"),TRUE,FALSE)</xm:f>
             <x14:dxf>
               <fill>
@@ -7098,7 +7914,7 @@
           <xm:sqref>K9:M9 G9:I9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="7" id="{CF3EF681-ADA3-454F-BD4D-136E8407E816}">
+          <x14:cfRule type="expression" priority="13" id="{CF3EF681-ADA3-454F-BD4D-136E8407E816}">
             <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C7,Config!$C$1:$D$17,2,FALSE)),FALSE,IF(VLOOKUP($C7,Config!$C$1:$D$17,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
             <x14:dxf>
               <fill>
@@ -7108,10 +7924,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>P7:S7</xm:sqref>
+          <xm:sqref>Q7 S7 V7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="2" id="{9015B1FB-D320-45D4-903E-B40FCBE5CA69}">
+          <x14:cfRule type="expression" priority="8" id="{9015B1FB-D320-45D4-903E-B40FCBE5CA69}">
             <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C10,Config!$C$1:$D$17,2,FALSE)),FALSE,IF(VLOOKUP($C10,Config!$C$1:$D$17,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D10,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D10,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I10,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I10,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
             <x14:dxf>
               <fill>
@@ -7121,10 +7937,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B10:T39</xm:sqref>
+          <xm:sqref>B10:X39</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{956628B0-9BEE-401E-B2E2-0213C7CEE5C0}">
+          <x14:cfRule type="expression" priority="7" id="{956628B0-9BEE-401E-B2E2-0213C7CEE5C0}">
             <xm:f>IF(IF(ISERROR(VLOOKUP($D10,Tabelas!$A$3:$C$51,3,FALSE)),FALSE,VLOOKUP($D10,Tabelas!$A$3:$C$51,3,FALSE)="Sim"),TRUE,FALSE)</xm:f>
             <x14:dxf>
               <fill>
@@ -7137,7 +7953,7 @@
           <xm:sqref>J10:J39 D10:F39</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="3" id="{37400795-195C-4039-B9AA-275DE3D968EE}">
+          <x14:cfRule type="expression" priority="9" id="{37400795-195C-4039-B9AA-275DE3D968EE}">
             <xm:f>IF(IF(ISERROR(VLOOKUP($I10,Tabelas!$A$3:$C$51,3,FALSE)),FALSE,VLOOKUP($I10,Tabelas!$A$3:$C$51,3,FALSE)="Sim"),TRUE,FALSE)</xm:f>
             <x14:dxf>
               <fill>
@@ -7148,6 +7964,71 @@
             </x14:dxf>
           </x14:cfRule>
           <xm:sqref>K10:M39 G10:I39</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="6" id="{6833BDA1-C45D-4AD2-B5F4-CA013523FCA7}">
+            <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C7,Config!$C$1:$D$17,2,FALSE)),FALSE,IF(VLOOKUP($C7,Config!$C$1:$D$17,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFFFCC"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>O7:P7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="5" id="{ED503053-E09B-4D43-A8D9-9598E4076ED6}">
+            <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C7,Config!$C$1:$D$17,2,FALSE)),FALSE,IF(VLOOKUP($C7,Config!$C$1:$D$17,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFFFCC"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>R7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="3" id="{C09E7684-AED8-438C-B68E-2E7738ECC073}">
+            <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C7,Config!$C$1:$D$17,2,FALSE)),FALSE,IF(VLOOKUP($C7,Config!$C$1:$D$17,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFFFCC"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>W7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="2" id="{BD039133-8410-430E-A4D9-B20483016ECF}">
+            <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C7,Config!$C$1:$D$17,2,FALSE)),FALSE,IF(VLOOKUP($C7,Config!$C$1:$D$17,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFFFCC"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>U7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{18861696-7153-4870-9908-43C72D087D0E}">
+            <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C7,Config!$C$1:$D$17,2,FALSE)),FALSE,IF(VLOOKUP($C7,Config!$C$1:$D$17,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFFFCC"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>T7</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Controle de horas por período
</commit_message>
<xml_diff>
--- a/Controle de Ponto.xlsx
+++ b/Controle de Ponto.xlsx
@@ -20,6 +20,8 @@
   <definedNames>
     <definedName name="CARENCIA">Config!$D$5</definedName>
     <definedName name="JORNADA">Config!$D$7</definedName>
+    <definedName name="JORNADA_PERIODO_1">Config!$D$21</definedName>
+    <definedName name="JORNADA_PERIODO_2">Config!$D$22</definedName>
     <definedName name="LIMITE">Config!$D$3</definedName>
     <definedName name="lst_Mes">tbl_Mes[Mês]</definedName>
     <definedName name="lstEvento">tblEvento[Evento]</definedName>
@@ -95,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="109">
   <si>
     <t>Data</t>
   </si>
@@ -411,7 +413,22 @@
     <t>Hora Extra Especial (Decimal)</t>
   </si>
   <si>
-    <t>v7.3</t>
+    <t>Período</t>
+  </si>
+  <si>
+    <t>1° Período</t>
+  </si>
+  <si>
+    <t>2° Período</t>
+  </si>
+  <si>
+    <t>Qtd. Horas por Jornada</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>v7.4</t>
   </si>
 </sst>
 </file>
@@ -767,7 +784,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -905,6 +922,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="1" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -922,12 +945,6 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -968,49 +985,57 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="61">
+  <dxfs count="65">
     <dxf>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
@@ -1031,6 +1056,33 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="[h]:mm"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="167" formatCode="[h]:mm"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
@@ -1041,108 +1093,13 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD5D6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD1D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD5D6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD1D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="[h]:mm"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
     </dxf>
@@ -1274,6 +1231,90 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD5D6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD1D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD5D6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD1D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="h:mm;@"/>
@@ -1417,72 +1458,83 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tblEvento" displayName="tblEvento" ref="A2:F13" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tblEvento" displayName="tblEvento" ref="A2:F13" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
   <sortState ref="A3:F13">
     <sortCondition ref="A8"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="Evento" dataDxfId="58"/>
-    <tableColumn id="2" name="Colorir Linha" dataDxfId="57"/>
-    <tableColumn id="5" name="Colorir Período" dataDxfId="56"/>
-    <tableColumn id="6" name="Libera o Período" dataDxfId="55"/>
-    <tableColumn id="4" name="Conta hora Extra" dataDxfId="54"/>
-    <tableColumn id="3" name="Descrição" dataDxfId="53"/>
+    <tableColumn id="1" name="Evento" dataDxfId="62"/>
+    <tableColumn id="2" name="Colorir Linha" dataDxfId="61"/>
+    <tableColumn id="5" name="Colorir Período" dataDxfId="60"/>
+    <tableColumn id="6" name="Libera o Período" dataDxfId="59"/>
+    <tableColumn id="4" name="Conta hora Extra" dataDxfId="58"/>
+    <tableColumn id="3" name="Descrição" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="tblLimiteHora" displayName="tblLimiteHora" ref="H2:J4" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="tblLimiteHora" displayName="tblLimiteHora" ref="H2:J4" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
   <autoFilter ref="H2:J4"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Limite de horas" dataDxfId="50"/>
-    <tableColumn id="3" name="Limite" dataDxfId="49"/>
-    <tableColumn id="2" name="h" dataDxfId="48"/>
+    <tableColumn id="1" name="Limite de horas" dataDxfId="54"/>
+    <tableColumn id="3" name="Limite" dataDxfId="53"/>
+    <tableColumn id="2" name="h" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="tbl_Mes" displayName="tbl_Mes" ref="L2:L14" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="tbl_Mes" displayName="tbl_Mes" ref="L2:L14" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
   <autoFilter ref="L2:L14"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Mês" dataDxfId="45"/>
+    <tableColumn id="1" name="Mês" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tblDiaUtil" displayName="tblDiaUtil" ref="B10:E17" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tblDiaUtil" displayName="tblDiaUtil" ref="B10:E17" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
   <tableColumns count="4">
-    <tableColumn id="1" name="Dia da Semana" dataDxfId="42"/>
-    <tableColumn id="4" name="Abreviatura" dataDxfId="41"/>
-    <tableColumn id="2" name="É dia util?" dataDxfId="40"/>
-    <tableColumn id="3" name="Jornada Diferenciada?" dataDxfId="39"/>
+    <tableColumn id="1" name="Dia da Semana" dataDxfId="46"/>
+    <tableColumn id="4" name="Abreviatura" dataDxfId="45"/>
+    <tableColumn id="2" name="É dia util?" dataDxfId="44"/>
+    <tableColumn id="3" name="Jornada Diferenciada?" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblHoras" displayName="tblHoras" ref="B8:X39" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="tblDiaUtil7" displayName="tblDiaUtil7" ref="B20:D22" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <tableColumns count="3">
+    <tableColumn id="1" name="Período" dataDxfId="0"/>
+    <tableColumn id="4" name="Abreviatura" dataDxfId="3"/>
+    <tableColumn id="2" name="Qtd. Horas por Jornada" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblHoras" displayName="tblHoras" ref="B8:X39" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
   <tableColumns count="23">
-    <tableColumn id="1" name="Data" dataDxfId="36">
+    <tableColumn id="1" name="Data" dataDxfId="28">
       <calculatedColumnFormula>IF(B8&lt;&gt;"",IF(DAY(B8+1)=1,"",B8+1),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Dia" dataDxfId="35">
+    <tableColumn id="2" name="Dia" dataDxfId="27">
       <calculatedColumnFormula>TEXT(tblHoras[[#This Row],[Data]],"ddd")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Evento _x000a_(1º Período)" dataDxfId="34"/>
-    <tableColumn id="4" name="Entrada - 1" dataDxfId="33"/>
-    <tableColumn id="5" name="Saída - 1 (Almoço)" dataDxfId="32"/>
-    <tableColumn id="6" name="Entrada - 2 (Almoço)" dataDxfId="31"/>
-    <tableColumn id="7" name="Saída - 2" dataDxfId="30"/>
-    <tableColumn id="13" name="Evento _x000a_(2º Período)" dataDxfId="29"/>
-    <tableColumn id="15" name="Horas Trabalhadas (1º Período)" dataDxfId="28">
+    <tableColumn id="3" name="Evento _x000a_(1º Período)" dataDxfId="26"/>
+    <tableColumn id="4" name="Entrada - 1" dataDxfId="25"/>
+    <tableColumn id="5" name="Saída - 1 (Almoço)" dataDxfId="24"/>
+    <tableColumn id="6" name="Entrada - 2 (Almoço)" dataDxfId="23"/>
+    <tableColumn id="7" name="Saída - 2" dataDxfId="22"/>
+    <tableColumn id="13" name="Evento _x000a_(2º Período)" dataDxfId="21"/>
+    <tableColumn id="15" name="Horas Trabalhadas (1º Período)" dataDxfId="20">
       <calculatedColumnFormula>IF($B$6&lt;&gt;"",IF(AND(tblHoras[[#This Row],[Evento 
 (1º Período)]]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[[#This Row],[Evento 
 (1º Período)]],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[[#This Row],[Evento 
@@ -1499,7 +1551,7 @@
                           0)),
                     0)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Horas Trabalhadas (2º Período)" dataDxfId="27">
+    <tableColumn id="16" name="Horas Trabalhadas (2º Período)" dataDxfId="19">
       <calculatedColumnFormula>IF($B$6&lt;&gt;"",IF(AND(tblHoras[[#This Row],[Evento 
 (2º Período)]]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[[#This Row],[Evento 
 (2º Período)]],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[[#This Row],[Evento 
@@ -1516,10 +1568,10 @@
                          0)),
        0)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Horas Trabalhadas" dataDxfId="26">
+    <tableColumn id="8" name="Horas Trabalhadas" dataDxfId="18">
       <calculatedColumnFormula>tblHoras[[#This Row],[Horas Trabalhadas (1º Período)]]+tblHoras[[#This Row],[Horas Trabalhadas (2º Período)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Jornada Diária" dataDxfId="25">
+    <tableColumn id="17" name="Jornada Diária" dataDxfId="17">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Data]]&lt;&gt;"",
         IF(
 AND(VLOOKUP(TEXT(tblHoras[[#This Row],[Data]],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[[#This Row],[Evento 
@@ -1531,7 +1583,7 @@
               ""),
          "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Horas Trabalhadas Além Jornada" dataDxfId="24">
+    <tableColumn id="11" name="Horas Trabalhadas Além Jornada" dataDxfId="16">
       <calculatedColumnFormula>IF(OR(tblHoras[[#This Row],[Horas Trabalhadas (1º Período)]]&lt;&gt;0,tblHoras[[#This Row],[Horas Trabalhadas (2º Período)]]&lt;&gt;0),
         IF(ISNUMBER(tblHoras[[#This Row],[Jornada Diária]]),
               IF(tblHoras[[#This Row],[Jornada Diária]]&gt;(tblHoras[[#This Row],[Horas Trabalhadas (2º Período)]]+tblHoras[[#This Row],[Horas Trabalhadas (1º Período)]]),
@@ -1554,7 +1606,7 @@
 (2º Período)]],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
 )))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Saldo de Horas" dataDxfId="23">
+    <tableColumn id="18" name="Saldo de Horas" dataDxfId="15">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&gt;0,
         IF(tblHoras[[#This Row],[Jornada Diária]]&lt;&gt;"",
               IF(HOUR(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]])&gt;=VLOOKUP(LIMITE,tblLimiteHora[],Tabelas!$I$1,FALSE),
@@ -1563,23 +1615,23 @@
               tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]),
         0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="Saldo de Horas (Decimal)" dataDxfId="22">
+    <tableColumn id="20" name="Saldo de Horas (Decimal)" dataDxfId="14">
       <calculatedColumnFormula>tblHoras[[#This Row],[Saldo de Horas]]*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="Atrasos_x000a_(horas)" dataDxfId="21">
+    <tableColumn id="19" name="Atrasos_x000a_(horas)" dataDxfId="13">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&lt;0,IF(OR(tblHoras[[#This Row],[Evento 
 (1º Período)]]="",tblHoras[[#This Row],[Evento 
 (2º Período)]]=""),tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]],""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Atrasos (Decimal)" dataDxfId="2">
+    <tableColumn id="21" name="Atrasos (Decimal)" dataDxfId="12">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Faltas_x000a_(dias)" dataDxfId="20">
+    <tableColumn id="14" name="Faltas_x000a_(dias)" dataDxfId="11">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Jornada Diária]]&lt;&gt;"",IF((N(tblHoras[[#This Row],[Jornada Diária]])-ABS(N(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]])))=0,1,""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Hora Extra Normal" dataDxfId="5">
+    <tableColumn id="10" name="Hora Extra Normal" dataDxfId="10">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[[#This Row],[Data]],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[[#This Row],[Evento 
 (1º Período)]]&lt;&gt;"",IF(VLOOKUP(tblHoras[[#This Row],[Evento 
@@ -1588,10 +1640,10 @@
 (2º Período)]],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
 tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]],""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="Hora Extra Normal (Decimal)" dataDxfId="1">
+    <tableColumn id="22" name="Hora Extra Normal (Decimal)" dataDxfId="9">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Hora Extra _x000a_Especial" dataDxfId="4">
+    <tableColumn id="9" name="Hora Extra _x000a_Especial" dataDxfId="8">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[[#This Row],[Data]],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[[#This Row],[Evento 
 (1º Período)]]&lt;&gt;"",IF(VLOOKUP(tblHoras[[#This Row],[Evento 
@@ -1600,12 +1652,12 @@
 (2º Período)]],tblEvento[],Tabelas!$E$1,FALSE)="Sim",TRUE,FALSE),FALSE)),
 tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]],""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="Hora Extra Especial (Decimal)" dataDxfId="0">
+    <tableColumn id="23" name="Hora Extra Especial (Decimal)" dataDxfId="7">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Informação" dataDxfId="3">
+    <tableColumn id="12" name="Informação" dataDxfId="6">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Evento 
 (1º Período)]]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[[#This Row],[Evento 
 (1º Período)]],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[[#This Row],[Evento 
@@ -2248,9 +2300,9 @@
   <sheetPr codeName="plnConfig">
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B1:E17"/>
+  <dimension ref="B1:H27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -2261,15 +2313,17 @@
     <col min="3" max="3" width="18" style="5" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" style="5" customWidth="1"/>
     <col min="5" max="5" width="15" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="5"/>
+    <col min="6" max="6" width="9.140625" style="5"/>
+    <col min="7" max="7" width="3.5703125" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="52"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="54"/>
     </row>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="19" t="s">
@@ -2302,12 +2356,12 @@
       </c>
     </row>
     <row r="9" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="55"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="57"/>
     </row>
     <row r="10" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
@@ -2395,7 +2449,7 @@
       </c>
       <c r="E16" s="40"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="21" t="s">
         <v>40</v>
       </c>
@@ -2407,29 +2461,134 @@
       </c>
       <c r="E17" s="40"/>
     </row>
+    <row r="19" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="56"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="73" t="s">
+        <v>107</v>
+      </c>
+      <c r="F19" s="72">
+        <f>SUM(tblDiaUtil7[Qtd. Horas por Jornada])</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G19" s="5">
+        <f>IF(F19&gt;0,IF(F19=JORNADA,1,0),"")</f>
+        <v>1</v>
+      </c>
+      <c r="H19" s="74" t="str">
+        <f>IF(G19=0,"A quantidade de horas por período deve ser igual à jornada diária","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E20" s="9"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="71">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E21" s="40"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="71">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E22" s="40"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="21"/>
+      <c r="C23" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="22"/>
+      <c r="E23" s="40"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="40"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="40"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="40"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="40"/>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Ha7W5bxf1w1NgOJx04/fWLYR6pTAAF2CzVEX6sDJmxy04fCR8Uagfk8h+nnBtz3f+WOjx+7F1pkoGAjGUmStKA==" saltValue="1E1mlKU/3LZ+W9vV+cF3MA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="2">
+  <sheetProtection algorithmName="SHA-512" hashValue="9+MX/+Zq1SYuuJA2+APjigl5LM+/jyjLSaudMfNfRCLZmq4MLwZ4xMW8yxfGfTCtzoG5vjKtC/QsIWYwqDXv/w==" saltValue="45qhRGdImc2pB4p1/dSFcw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B19:D19"/>
   </mergeCells>
   <conditionalFormatting sqref="D7">
-    <cfRule type="timePeriod" dxfId="19" priority="3" timePeriod="lastMonth">
+    <cfRule type="timePeriod" dxfId="1" priority="4" timePeriod="lastMonth">
       <formula>AND(MONTH(D7)=MONTH(EDATE(TODAY(),0-1)),YEAR(D7)=YEAR(EDATE(TODAY(),0-1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <conditionalFormatting sqref="G19">
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0.5" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3">
       <formula1>lstLimiteHora</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11:D17">
       <formula1>"Sim,Não"</formula1>
     </dataValidation>
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7 D5 D21:D22 F19">
+      <formula1>0</formula1>
+      <formula2>0.999305555555556</formula2>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2603,15 +2762,15 @@
       <c r="N6" s="24"/>
       <c r="O6" s="24"/>
       <c r="P6" s="24"/>
-      <c r="Q6" s="56" t="s">
+      <c r="Q6" s="69" t="s">
         <v>95</v>
       </c>
-      <c r="R6" s="57"/>
-      <c r="S6" s="57"/>
-      <c r="T6" s="57"/>
-      <c r="U6" s="57"/>
-      <c r="V6" s="57"/>
-      <c r="W6" s="57"/>
+      <c r="R6" s="70"/>
+      <c r="S6" s="70"/>
+      <c r="T6" s="70"/>
+      <c r="U6" s="70"/>
+      <c r="V6" s="70"/>
+      <c r="W6" s="70"/>
       <c r="X6" s="24"/>
     </row>
     <row r="7" spans="2:29" x14ac:dyDescent="0.25">
@@ -2639,7 +2798,7 @@
         <f>O39</f>
         <v>0</v>
       </c>
-      <c r="P7" s="69">
+      <c r="P7" s="50">
         <f>P39</f>
         <v>0</v>
       </c>
@@ -2648,7 +2807,7 @@
 (horas)])</f>
         <v>0</v>
       </c>
-      <c r="R7" s="69">
+      <c r="R7" s="50">
         <f>SUM(tblHoras[Atrasos (Decimal)])</f>
         <v>0</v>
       </c>
@@ -2661,13 +2820,13 @@
         <f>SUM(tblHoras[Hora Extra Normal])</f>
         <v>0</v>
       </c>
-      <c r="U7" s="69"/>
+      <c r="U7" s="50"/>
       <c r="V7" s="47">
         <f>SUM(tblHoras[Hora Extra 
 Especial])</f>
         <v>0</v>
       </c>
-      <c r="W7" s="69">
+      <c r="W7" s="50">
         <f>SUM(tblHoras[Hora Extra Especial (Decimal)])</f>
         <v>0</v>
       </c>
@@ -2765,7 +2924,7 @@
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",JORNADA_PERIODO_1,JORNADA/2),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -2783,7 +2942,7 @@
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",JORNADA_PERIODO_2,JORNADA/2),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -2847,7 +3006,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])</f>
         <v>0</v>
       </c>
-      <c r="P9" s="70">
+      <c r="P9" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -2857,7 +3016,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R9" s="70" t="str">
+      <c r="R9" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -2877,7 +3036,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U9" s="70" t="str">
+      <c r="U9" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -2891,7 +3050,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W9" s="70" t="str">
+      <c r="W9" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -3012,7 +3171,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O9</f>
         <v>0</v>
       </c>
-      <c r="P10" s="70">
+      <c r="P10" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -3022,7 +3181,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R10" s="70" t="str">
+      <c r="R10" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -3042,7 +3201,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U10" s="70" t="str">
+      <c r="U10" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -3056,7 +3215,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W10" s="70" t="str">
+      <c r="W10" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -3176,7 +3335,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O10</f>
         <v>0</v>
       </c>
-      <c r="P11" s="70">
+      <c r="P11" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -3186,7 +3345,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R11" s="70" t="str">
+      <c r="R11" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -3206,7 +3365,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U11" s="70" t="str">
+      <c r="U11" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -3220,7 +3379,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W11" s="70" t="str">
+      <c r="W11" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -3339,7 +3498,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O11</f>
         <v>0</v>
       </c>
-      <c r="P12" s="70">
+      <c r="P12" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -3349,7 +3508,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R12" s="70" t="str">
+      <c r="R12" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -3369,7 +3528,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U12" s="70" t="str">
+      <c r="U12" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -3383,7 +3542,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W12" s="70" t="str">
+      <c r="W12" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -3502,7 +3661,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O12</f>
         <v>0</v>
       </c>
-      <c r="P13" s="70">
+      <c r="P13" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -3512,7 +3671,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R13" s="70" t="str">
+      <c r="R13" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -3532,7 +3691,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U13" s="70" t="str">
+      <c r="U13" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -3546,7 +3705,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W13" s="70" t="str">
+      <c r="W13" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -3665,7 +3824,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O13</f>
         <v>0</v>
       </c>
-      <c r="P14" s="70">
+      <c r="P14" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -3675,7 +3834,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R14" s="70" t="str">
+      <c r="R14" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -3695,7 +3854,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U14" s="70" t="str">
+      <c r="U14" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -3709,7 +3868,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W14" s="70" t="str">
+      <c r="W14" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -3830,7 +3989,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O14</f>
         <v>0</v>
       </c>
-      <c r="P15" s="70">
+      <c r="P15" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -3840,7 +3999,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R15" s="70" t="str">
+      <c r="R15" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -3860,7 +4019,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U15" s="70" t="str">
+      <c r="U15" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -3874,7 +4033,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W15" s="70" t="str">
+      <c r="W15" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -3994,7 +4153,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O15</f>
         <v>0</v>
       </c>
-      <c r="P16" s="70">
+      <c r="P16" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -4004,7 +4163,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R16" s="70" t="str">
+      <c r="R16" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -4024,7 +4183,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U16" s="70" t="str">
+      <c r="U16" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -4038,7 +4197,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W16" s="70" t="str">
+      <c r="W16" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -4157,7 +4316,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O16</f>
         <v>0</v>
       </c>
-      <c r="P17" s="70">
+      <c r="P17" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -4167,7 +4326,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R17" s="70" t="str">
+      <c r="R17" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -4187,7 +4346,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U17" s="70" t="str">
+      <c r="U17" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -4201,7 +4360,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W17" s="70" t="str">
+      <c r="W17" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -4320,7 +4479,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O17</f>
         <v>0</v>
       </c>
-      <c r="P18" s="70">
+      <c r="P18" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -4330,7 +4489,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R18" s="70" t="str">
+      <c r="R18" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -4350,7 +4509,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U18" s="70" t="str">
+      <c r="U18" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -4364,7 +4523,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W18" s="70" t="str">
+      <c r="W18" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -4483,7 +4642,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O18</f>
         <v>0</v>
       </c>
-      <c r="P19" s="70">
+      <c r="P19" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -4493,7 +4652,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R19" s="70" t="str">
+      <c r="R19" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -4513,7 +4672,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U19" s="70" t="str">
+      <c r="U19" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -4527,7 +4686,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W19" s="70" t="str">
+      <c r="W19" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -4646,7 +4805,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O19</f>
         <v>0</v>
       </c>
-      <c r="P20" s="70">
+      <c r="P20" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -4656,7 +4815,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R20" s="70" t="str">
+      <c r="R20" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -4676,7 +4835,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U20" s="70" t="str">
+      <c r="U20" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -4690,7 +4849,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W20" s="70" t="str">
+      <c r="W20" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -4809,7 +4968,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O20</f>
         <v>0</v>
       </c>
-      <c r="P21" s="70">
+      <c r="P21" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -4819,7 +4978,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R21" s="70" t="str">
+      <c r="R21" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -4839,7 +4998,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U21" s="70" t="str">
+      <c r="U21" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -4853,7 +5012,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W21" s="70" t="str">
+      <c r="W21" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -4972,7 +5131,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O21</f>
         <v>0</v>
       </c>
-      <c r="P22" s="70">
+      <c r="P22" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -4982,7 +5141,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R22" s="70" t="str">
+      <c r="R22" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -5002,7 +5161,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U22" s="70" t="str">
+      <c r="U22" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -5016,7 +5175,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W22" s="70" t="str">
+      <c r="W22" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -5135,7 +5294,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O22</f>
         <v>0</v>
       </c>
-      <c r="P23" s="70">
+      <c r="P23" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -5145,7 +5304,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R23" s="70" t="str">
+      <c r="R23" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -5165,7 +5324,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U23" s="70" t="str">
+      <c r="U23" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -5179,7 +5338,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W23" s="70" t="str">
+      <c r="W23" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -5298,7 +5457,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O23</f>
         <v>0</v>
       </c>
-      <c r="P24" s="70">
+      <c r="P24" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -5308,7 +5467,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R24" s="70" t="str">
+      <c r="R24" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -5328,7 +5487,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U24" s="70" t="str">
+      <c r="U24" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -5342,7 +5501,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W24" s="70" t="str">
+      <c r="W24" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -5461,7 +5620,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O24</f>
         <v>0</v>
       </c>
-      <c r="P25" s="70">
+      <c r="P25" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -5471,7 +5630,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R25" s="70" t="str">
+      <c r="R25" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -5491,7 +5650,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U25" s="70" t="str">
+      <c r="U25" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -5505,7 +5664,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W25" s="70" t="str">
+      <c r="W25" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -5624,7 +5783,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O25</f>
         <v>0</v>
       </c>
-      <c r="P26" s="70">
+      <c r="P26" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -5634,7 +5793,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R26" s="70" t="str">
+      <c r="R26" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -5654,7 +5813,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U26" s="70" t="str">
+      <c r="U26" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -5668,7 +5827,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W26" s="70" t="str">
+      <c r="W26" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -5787,7 +5946,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O26</f>
         <v>0</v>
       </c>
-      <c r="P27" s="70">
+      <c r="P27" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -5797,7 +5956,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R27" s="70" t="str">
+      <c r="R27" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -5817,7 +5976,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U27" s="70" t="str">
+      <c r="U27" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -5831,7 +5990,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W27" s="70" t="str">
+      <c r="W27" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -5950,7 +6109,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O27</f>
         <v>0</v>
       </c>
-      <c r="P28" s="70">
+      <c r="P28" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -5960,7 +6119,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R28" s="70" t="str">
+      <c r="R28" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -5980,7 +6139,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U28" s="70" t="str">
+      <c r="U28" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -5994,7 +6153,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W28" s="70" t="str">
+      <c r="W28" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -6113,7 +6272,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O28</f>
         <v>0</v>
       </c>
-      <c r="P29" s="70">
+      <c r="P29" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -6123,7 +6282,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R29" s="70" t="str">
+      <c r="R29" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -6143,7 +6302,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U29" s="70" t="str">
+      <c r="U29" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -6157,7 +6316,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W29" s="70" t="str">
+      <c r="W29" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -6276,7 +6435,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O29</f>
         <v>0</v>
       </c>
-      <c r="P30" s="70">
+      <c r="P30" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -6286,7 +6445,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R30" s="70" t="str">
+      <c r="R30" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -6306,7 +6465,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U30" s="70" t="str">
+      <c r="U30" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -6320,7 +6479,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W30" s="70" t="str">
+      <c r="W30" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -6439,7 +6598,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O30</f>
         <v>0</v>
       </c>
-      <c r="P31" s="70">
+      <c r="P31" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -6449,7 +6608,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R31" s="70" t="str">
+      <c r="R31" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -6469,7 +6628,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U31" s="70" t="str">
+      <c r="U31" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -6483,7 +6642,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W31" s="70" t="str">
+      <c r="W31" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -6602,7 +6761,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O31</f>
         <v>0</v>
       </c>
-      <c r="P32" s="70">
+      <c r="P32" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -6612,7 +6771,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R32" s="70" t="str">
+      <c r="R32" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -6632,7 +6791,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U32" s="70" t="str">
+      <c r="U32" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -6646,7 +6805,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W32" s="70" t="str">
+      <c r="W32" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -6765,7 +6924,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O32</f>
         <v>0</v>
       </c>
-      <c r="P33" s="70">
+      <c r="P33" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -6775,7 +6934,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R33" s="70" t="str">
+      <c r="R33" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -6795,7 +6954,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U33" s="70" t="str">
+      <c r="U33" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -6809,7 +6968,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W33" s="70" t="str">
+      <c r="W33" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -6928,7 +7087,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O33</f>
         <v>0</v>
       </c>
-      <c r="P34" s="70">
+      <c r="P34" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -6938,7 +7097,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R34" s="70" t="str">
+      <c r="R34" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -6958,7 +7117,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U34" s="70" t="str">
+      <c r="U34" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -6972,7 +7131,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W34" s="70" t="str">
+      <c r="W34" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -7091,7 +7250,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O34</f>
         <v>0</v>
       </c>
-      <c r="P35" s="70">
+      <c r="P35" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -7101,7 +7260,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R35" s="70" t="str">
+      <c r="R35" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -7121,7 +7280,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U35" s="70" t="str">
+      <c r="U35" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -7135,7 +7294,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W35" s="70" t="str">
+      <c r="W35" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -7254,7 +7413,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O35</f>
         <v>0</v>
       </c>
-      <c r="P36" s="70">
+      <c r="P36" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -7264,7 +7423,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R36" s="70" t="str">
+      <c r="R36" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -7284,7 +7443,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U36" s="70" t="str">
+      <c r="U36" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -7298,7 +7457,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W36" s="70" t="str">
+      <c r="W36" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -7417,7 +7576,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O36</f>
         <v>0</v>
       </c>
-      <c r="P37" s="70">
+      <c r="P37" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -7427,7 +7586,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R37" s="70" t="str">
+      <c r="R37" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -7447,7 +7606,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U37" s="70" t="str">
+      <c r="U37" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -7461,7 +7620,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W37" s="70" t="str">
+      <c r="W37" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -7580,7 +7739,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O37</f>
         <v>0</v>
       </c>
-      <c r="P38" s="70">
+      <c r="P38" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -7590,7 +7749,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R38" s="70" t="str">
+      <c r="R38" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -7610,7 +7769,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U38" s="70" t="str">
+      <c r="U38" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -7624,7 +7783,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W38" s="70" t="str">
+      <c r="W38" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -7743,7 +7902,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O38</f>
         <v>0</v>
       </c>
-      <c r="P39" s="70">
+      <c r="P39" s="51">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -7753,7 +7912,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R39" s="70" t="str">
+      <c r="R39" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -7773,7 +7932,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U39" s="70" t="str">
+      <c r="U39" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -7787,7 +7946,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W39" s="70" t="str">
+      <c r="W39" s="51" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -7810,7 +7969,7 @@
     </row>
     <row r="41" spans="2:25" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="X41" s="36" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="Y41" s="24"/>
     </row>
@@ -7830,7 +7989,7 @@
     <row r="46" spans="2:25" x14ac:dyDescent="0.25"/>
     <row r="47" spans="2:25" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="PBwt9+JEYjlkiRwfKHy7xOwI4p9n1mffdrLoaKYA6avPryUjvYoQx0p1kLbn75QAdFf/hB21Do9/OwxyFwBRIg==" saltValue="M6RP+xkThEPESs4iK9SW+w==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" selectLockedCells="1" autoFilter="0" pivotTables="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="g+BR4CBRf3bhgxyB9ax6zrXmtiNmb/Uvh/3gU32lkGvl3+ZXgKtceCtWizZ9WUgUP5GgkMWtQYrTBLqw2ELTZg==" saltValue="ndc5HYslQsI1wlkfwYIsVQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" selectLockedCells="1" autoFilter="0" pivotTables="0"/>
   <dataConsolidate/>
   <mergeCells count="7">
     <mergeCell ref="O1:X4"/>

</xml_diff>

<commit_message>
Correção na formatação de campos
</commit_message>
<xml_diff>
--- a/Controle de Ponto.xlsx
+++ b/Controle de Ponto.xlsx
@@ -784,7 +784,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -848,14 +848,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -912,9 +904,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="167" fontId="1" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -928,6 +917,17 @@
     <xf numFmtId="4" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -949,14 +949,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -968,14 +960,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -991,17 +975,25 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1009,33 +1001,51 @@
   </cellStyles>
   <dxfs count="65">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="h:mm;@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="166" formatCode="h:mm;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
+      <numFmt numFmtId="166" formatCode="h:mm;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
@@ -1164,23 +1174,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="h:mm;@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="h:mm;@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -1188,36 +1181,6 @@
       <numFmt numFmtId="166" formatCode="h:mm;@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="h:mm;@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="h:mm;@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="h:mm;@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[$-416]d\-mmm;@"/>
@@ -1317,6 +1280,26 @@
       </fill>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="166" formatCode="h:mm;@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
@@ -1340,6 +1323,16 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1497,44 +1490,44 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tblDiaUtil" displayName="tblDiaUtil" ref="B10:E17" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tblDiaUtil" displayName="tblDiaUtil" ref="B10:E17" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <tableColumns count="4">
-    <tableColumn id="1" name="Dia da Semana" dataDxfId="46"/>
-    <tableColumn id="4" name="Abreviatura" dataDxfId="45"/>
-    <tableColumn id="2" name="É dia util?" dataDxfId="44"/>
-    <tableColumn id="3" name="Jornada Diferenciada?" dataDxfId="43"/>
+    <tableColumn id="1" name="Dia da Semana" dataDxfId="45"/>
+    <tableColumn id="4" name="Abreviatura" dataDxfId="44"/>
+    <tableColumn id="2" name="É dia util?" dataDxfId="43"/>
+    <tableColumn id="3" name="Jornada Diferenciada?" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="tblDiaUtil7" displayName="tblDiaUtil7" ref="B20:D22" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="tblDiaUtil7" displayName="tblDiaUtil7" ref="B20:D22" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <tableColumns count="3">
-    <tableColumn id="1" name="Período" dataDxfId="0"/>
-    <tableColumn id="4" name="Abreviatura" dataDxfId="3"/>
-    <tableColumn id="2" name="Qtd. Horas por Jornada" dataDxfId="2"/>
+    <tableColumn id="1" name="Período" dataDxfId="39"/>
+    <tableColumn id="4" name="Abreviatura" dataDxfId="38"/>
+    <tableColumn id="2" name="Qtd. Horas por Jornada" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblHoras" displayName="tblHoras" ref="B8:X39" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblHoras" displayName="tblHoras" ref="B8:X39" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <tableColumns count="23">
-    <tableColumn id="1" name="Data" dataDxfId="28">
+    <tableColumn id="1" name="Data" dataDxfId="22">
       <calculatedColumnFormula>IF(B8&lt;&gt;"",IF(DAY(B8+1)=1,"",B8+1),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Dia" dataDxfId="27">
+    <tableColumn id="2" name="Dia" dataDxfId="5">
       <calculatedColumnFormula>TEXT(tblHoras[[#This Row],[Data]],"ddd")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Evento _x000a_(1º Período)" dataDxfId="26"/>
-    <tableColumn id="4" name="Entrada - 1" dataDxfId="25"/>
-    <tableColumn id="5" name="Saída - 1 (Almoço)" dataDxfId="24"/>
-    <tableColumn id="6" name="Entrada - 2 (Almoço)" dataDxfId="23"/>
-    <tableColumn id="7" name="Saída - 2" dataDxfId="22"/>
-    <tableColumn id="13" name="Evento _x000a_(2º Período)" dataDxfId="21"/>
-    <tableColumn id="15" name="Horas Trabalhadas (1º Período)" dataDxfId="20">
+    <tableColumn id="3" name="Evento _x000a_(1º Período)" dataDxfId="3"/>
+    <tableColumn id="4" name="Entrada - 1" dataDxfId="4"/>
+    <tableColumn id="5" name="Saída - 1 (Almoço)" dataDxfId="21"/>
+    <tableColumn id="6" name="Entrada - 2 (Almoço)" dataDxfId="20"/>
+    <tableColumn id="7" name="Saída - 2" dataDxfId="2"/>
+    <tableColumn id="13" name="Evento _x000a_(2º Período)" dataDxfId="0"/>
+    <tableColumn id="15" name="Horas Trabalhadas (1º Período)" dataDxfId="1">
       <calculatedColumnFormula>IF($B$6&lt;&gt;"",IF(AND(tblHoras[[#This Row],[Evento 
 (1º Período)]]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[[#This Row],[Evento 
 (1º Período)]],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[[#This Row],[Evento 
@@ -2026,30 +2019,30 @@
       <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="37"/>
+      <c r="E3" s="35"/>
       <c r="F3" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="38" t="str">
+      <c r="H3" s="36" t="str">
         <f>tblLimiteHora[[#This Row],[Limite]]&amp;"h diárias"</f>
         <v>2h diárias</v>
       </c>
-      <c r="I3" s="39">
+      <c r="I3" s="37">
         <v>2</v>
       </c>
       <c r="J3" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="L3" s="32" t="s">
+      <c r="L3" s="30" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2057,16 +2050,16 @@
       <c r="A4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="37"/>
+      <c r="E4" s="35"/>
       <c r="F4" s="23" t="s">
         <v>9</v>
       </c>
@@ -2079,7 +2072,7 @@
       <c r="J4" s="13">
         <v>0</v>
       </c>
-      <c r="L4" s="32" t="s">
+      <c r="L4" s="30" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2087,20 +2080,20 @@
       <c r="A5" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="37"/>
+      <c r="E5" s="35"/>
       <c r="F5" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="L5" s="32" t="s">
+      <c r="L5" s="30" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2108,20 +2101,20 @@
       <c r="A6" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="37"/>
+      <c r="E6" s="35"/>
       <c r="F6" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="L6" s="32" t="s">
+      <c r="L6" s="30" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2129,20 +2122,20 @@
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="37"/>
+      <c r="E7" s="35"/>
       <c r="F7" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="32" t="s">
+      <c r="L7" s="30" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2150,20 +2143,20 @@
       <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="37"/>
+      <c r="E8" s="35"/>
       <c r="F8" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="L8" s="32" t="s">
+      <c r="L8" s="30" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2171,20 +2164,20 @@
       <c r="A9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37" t="s">
+      <c r="D9" s="35"/>
+      <c r="E9" s="35" t="s">
         <v>30</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="L9" s="32" t="s">
+      <c r="L9" s="30" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2192,20 +2185,20 @@
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37" t="s">
+      <c r="D10" s="35"/>
+      <c r="E10" s="35" t="s">
         <v>30</v>
       </c>
       <c r="F10" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="L10" s="32" t="s">
+      <c r="L10" s="30" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2213,20 +2206,20 @@
       <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="37"/>
+      <c r="E11" s="35"/>
       <c r="F11" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="L11" s="32" t="s">
+      <c r="L11" s="30" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2234,20 +2227,20 @@
       <c r="A12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="37"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="L12" s="32" t="s">
+      <c r="L12" s="30" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2255,25 +2248,25 @@
       <c r="A13" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="37"/>
+      <c r="E13" s="35"/>
       <c r="F13" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="L13" s="32" t="s">
+      <c r="L13" s="30" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L14" s="32" t="s">
+      <c r="L14" s="30" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2319,17 +2312,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="55"/>
     </row>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="34"/>
+      <c r="C3" s="32"/>
       <c r="D3" s="2" t="s">
         <v>18</v>
       </c>
@@ -2338,8 +2331,8 @@
       <c r="B5" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="28">
+      <c r="C5" s="32"/>
+      <c r="D5" s="26">
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="E5" s="20" t="s">
@@ -2350,18 +2343,18 @@
       <c r="B7" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="34"/>
+      <c r="C7" s="32"/>
       <c r="D7" s="3">
         <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="58"/>
     </row>
     <row r="10" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
@@ -2387,7 +2380,7 @@
       <c r="D11" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="40"/>
+      <c r="E11" s="38"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="21" t="s">
@@ -2399,7 +2392,7 @@
       <c r="D12" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="40"/>
+      <c r="E12" s="38"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="21" t="s">
@@ -2411,7 +2404,7 @@
       <c r="D13" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="40"/>
+      <c r="E13" s="38"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="21" t="s">
@@ -2423,7 +2416,7 @@
       <c r="D14" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="40"/>
+      <c r="E14" s="38"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="21" t="s">
@@ -2435,7 +2428,7 @@
       <c r="D15" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="40"/>
+      <c r="E15" s="38"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="21" t="s">
@@ -2447,7 +2440,7 @@
       <c r="D16" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="40"/>
+      <c r="E16" s="38"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="21" t="s">
@@ -2459,18 +2452,18 @@
       <c r="D17" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="40"/>
+      <c r="E17" s="38"/>
     </row>
     <row r="19" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="55" t="s">
+      <c r="B19" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="56"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="73" t="s">
+      <c r="C19" s="57"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="F19" s="72">
+      <c r="F19" s="50">
         <f>SUM(tblDiaUtil7[Qtd. Horas por Jornada])</f>
         <v>0.33333333333333331</v>
       </c>
@@ -2478,7 +2471,7 @@
         <f>IF(F19&gt;0,IF(F19=JORNADA,1,0),"")</f>
         <v>1</v>
       </c>
-      <c r="H19" s="74" t="str">
+      <c r="H19" s="52" t="str">
         <f>IF(G19=0,"A quantidade de horas por período deve ser igual à jornada diária","")</f>
         <v/>
       </c>
@@ -2502,10 +2495,10 @@
       <c r="C21" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="71">
+      <c r="D21" s="49">
         <v>0.16666666666666666</v>
       </c>
-      <c r="E21" s="40"/>
+      <c r="E21" s="38"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="21" t="s">
@@ -2514,10 +2507,10 @@
       <c r="C22" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="D22" s="71">
+      <c r="D22" s="49">
         <v>0.16666666666666666</v>
       </c>
-      <c r="E22" s="40"/>
+      <c r="E22" s="38"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="21"/>
@@ -2525,31 +2518,31 @@
         <v>80</v>
       </c>
       <c r="D23" s="22"/>
-      <c r="E23" s="40"/>
+      <c r="E23" s="38"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="21"/>
       <c r="C24" s="21"/>
       <c r="D24" s="22"/>
-      <c r="E24" s="40"/>
+      <c r="E24" s="38"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
       <c r="D25" s="22"/>
-      <c r="E25" s="40"/>
+      <c r="E25" s="38"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="21"/>
       <c r="C26" s="21"/>
       <c r="D26" s="22"/>
-      <c r="E26" s="40"/>
+      <c r="E26" s="38"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
       <c r="D27" s="22"/>
-      <c r="E27" s="40"/>
+      <c r="E27" s="38"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="9+MX/+Zq1SYuuJA2+APjigl5LM+/jyjLSaudMfNfRCLZmq4MLwZ4xMW8yxfGfTCtzoG5vjKtC/QsIWYwqDXv/w==" saltValue="45qhRGdImc2pB4p1/dSFcw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0" pivotTables="0"/>
@@ -2559,7 +2552,7 @@
     <mergeCell ref="B19:D19"/>
   </mergeCells>
   <conditionalFormatting sqref="D7">
-    <cfRule type="timePeriod" dxfId="1" priority="4" timePeriod="lastMonth">
+    <cfRule type="timePeriod" dxfId="48" priority="4" timePeriod="lastMonth">
       <formula>AND(MONTH(D7)=MONTH(EDATE(TODAY(),0-1)),YEAR(D7)=YEAR(EDATE(TODAY(),0-1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2636,10 +2629,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="O1" s="58" t="str">
+      <c r="O1" s="59" t="str">
         <f>"*Limite de horas: " &amp; LIMITE &amp; "; e 
 *Contabiliza a partir de " &amp; TEXT(CARENCIA, "hh:mm") &amp; " hora(s) (para mais ou para menos);
 *Caso tenha Atestado em um dos períodos, o que ultrapassar de 4:00 horas de trabalho contabiliza hora positiva."</f>
@@ -2647,130 +2640,130 @@
 *Contabiliza a partir de 00:10 hora(s) (para mais ou para menos);
 *Caso tenha Atestado em um dos períodos, o que ultrapassar de 4:00 horas de trabalho contabiliza hora positiva.</v>
       </c>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
-      <c r="T1" s="58"/>
-      <c r="U1" s="58"/>
-      <c r="V1" s="58"/>
-      <c r="W1" s="58"/>
-      <c r="X1" s="58"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
     </row>
     <row r="2" spans="2:29" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="6"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
       <c r="N2" s="24"/>
-      <c r="O2" s="58"/>
-      <c r="P2" s="58"/>
-      <c r="Q2" s="58"/>
-      <c r="R2" s="58"/>
-      <c r="S2" s="58"/>
-      <c r="T2" s="58"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="58"/>
-      <c r="W2" s="58"/>
-      <c r="X2" s="58"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
+      <c r="R2" s="59"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="59"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="59"/>
     </row>
     <row r="3" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="H3" s="67" t="s">
+      <c r="H3" s="64" t="s">
         <v>97</v>
       </c>
-      <c r="I3" s="68"/>
+      <c r="I3" s="65"/>
       <c r="N3" s="24"/>
-      <c r="O3" s="58"/>
-      <c r="P3" s="58"/>
-      <c r="Q3" s="58"/>
-      <c r="R3" s="58"/>
-      <c r="S3" s="58"/>
-      <c r="T3" s="58"/>
-      <c r="U3" s="58"/>
-      <c r="V3" s="58"/>
-      <c r="W3" s="58"/>
-      <c r="X3" s="58"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
+      <c r="R3" s="59"/>
+      <c r="S3" s="59"/>
+      <c r="T3" s="59"/>
+      <c r="U3" s="59"/>
+      <c r="V3" s="59"/>
+      <c r="W3" s="59"/>
+      <c r="X3" s="59"/>
     </row>
     <row r="4" spans="2:29" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="60"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="71"/>
       <c r="N4" s="24"/>
-      <c r="O4" s="58"/>
-      <c r="P4" s="58"/>
-      <c r="Q4" s="58"/>
-      <c r="R4" s="58"/>
-      <c r="S4" s="58"/>
-      <c r="T4" s="58"/>
-      <c r="U4" s="58"/>
-      <c r="V4" s="58"/>
-      <c r="W4" s="58"/>
-      <c r="X4" s="58"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="59"/>
+      <c r="Q4" s="59"/>
+      <c r="R4" s="59"/>
+      <c r="S4" s="59"/>
+      <c r="T4" s="59"/>
+      <c r="U4" s="59"/>
+      <c r="V4" s="59"/>
+      <c r="W4" s="59"/>
+      <c r="X4" s="59"/>
     </row>
     <row r="5" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="30" t="s">
+      <c r="C5" s="61"/>
+      <c r="D5" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="44" t="s">
+      <c r="E5" s="42" t="s">
         <v>88</v>
       </c>
       <c r="G5" s="7"/>
       <c r="N5" s="24"/>
       <c r="O5" s="24"/>
       <c r="P5" s="24"/>
-      <c r="Q5" s="35" t="s">
+      <c r="Q5" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="R5" s="35" t="s">
+      <c r="R5" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="S5" s="35" t="s">
+      <c r="S5" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="T5" s="35" t="s">
+      <c r="T5" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="U5" s="35" t="s">
+      <c r="U5" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="V5" s="35" t="s">
+      <c r="V5" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="W5" s="35" t="s">
+      <c r="W5" s="33" t="s">
         <v>76</v>
       </c>
       <c r="X5" s="24"/>
     </row>
     <row r="6" spans="2:29" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="63"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="33" t="str">
+      <c r="B6" s="62"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="31" t="str">
         <f>IF(ISERROR(DATEVALUE(IF(E6&lt;&gt;"",E6,1)&amp;"-"&amp;B6&amp;"-"&amp;D6)),"",DATEVALUE(IF(E6&lt;&gt;"",E6,1)&amp;"-"&amp;B6&amp;"-"&amp;D6))</f>
         <v/>
       </c>
       <c r="N6" s="24"/>
       <c r="O6" s="24"/>
       <c r="P6" s="24"/>
-      <c r="Q6" s="69" t="s">
+      <c r="Q6" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="R6" s="70"/>
-      <c r="S6" s="70"/>
-      <c r="T6" s="70"/>
-      <c r="U6" s="70"/>
-      <c r="V6" s="70"/>
-      <c r="W6" s="70"/>
+      <c r="R6" s="67"/>
+      <c r="S6" s="67"/>
+      <c r="T6" s="67"/>
+      <c r="U6" s="67"/>
+      <c r="V6" s="67"/>
+      <c r="W6" s="67"/>
       <c r="X6" s="24"/>
     </row>
     <row r="7" spans="2:29" x14ac:dyDescent="0.25">
@@ -2779,54 +2772,54 @@
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
-      <c r="J7" s="35" t="s">
+      <c r="J7" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="K7" s="35" t="s">
+      <c r="K7" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="L7" s="35" t="s">
+      <c r="L7" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="M7" s="35" t="s">
+      <c r="M7" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="N7" s="35" t="s">
+      <c r="N7" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="O7" s="47">
+      <c r="O7" s="44">
         <f>O39</f>
         <v>0</v>
       </c>
-      <c r="P7" s="50">
+      <c r="P7" s="47">
         <f>P39</f>
         <v>0</v>
       </c>
-      <c r="Q7" s="47">
+      <c r="Q7" s="44">
         <f>SUM(tblHoras[Atrasos
 (horas)])</f>
         <v>0</v>
       </c>
-      <c r="R7" s="50">
+      <c r="R7" s="47">
         <f>SUM(tblHoras[Atrasos (Decimal)])</f>
         <v>0</v>
       </c>
-      <c r="S7" s="48">
+      <c r="S7" s="45">
         <f>SUM(tblHoras[Faltas
 (dias)])</f>
         <v>0</v>
       </c>
-      <c r="T7" s="47">
+      <c r="T7" s="44">
         <f>SUM(tblHoras[Hora Extra Normal])</f>
         <v>0</v>
       </c>
-      <c r="U7" s="50"/>
-      <c r="V7" s="47">
+      <c r="U7" s="47"/>
+      <c r="V7" s="44">
         <f>SUM(tblHoras[Hora Extra 
 Especial])</f>
         <v>0</v>
       </c>
-      <c r="W7" s="50">
+      <c r="W7" s="47">
         <f>SUM(tblHoras[Hora Extra Especial (Decimal)])</f>
         <v>0</v>
       </c>
@@ -2902,7 +2895,7 @@
       <c r="X8" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="AA8" s="27"/>
+      <c r="AA8" s="25"/>
     </row>
     <row r="9" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="str">
@@ -2913,12 +2906,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D9" s="26"/>
+      <c r="D9" s="72"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="25"/>
+      <c r="I9" s="72"/>
       <c r="J9" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -3006,7 +2999,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])</f>
         <v>0</v>
       </c>
-      <c r="P9" s="51">
+      <c r="P9" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -3016,7 +3009,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R9" s="51" t="str">
+      <c r="R9" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -3036,7 +3029,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U9" s="51" t="str">
+      <c r="U9" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -3050,7 +3043,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W9" s="51" t="str">
+      <c r="W9" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -3078,12 +3071,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D10" s="26"/>
+      <c r="D10" s="72"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="25"/>
+      <c r="I10" s="72"/>
       <c r="J10" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -3171,7 +3164,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O9</f>
         <v>0</v>
       </c>
-      <c r="P10" s="51">
+      <c r="P10" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -3181,7 +3174,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R10" s="51" t="str">
+      <c r="R10" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -3201,7 +3194,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U10" s="51" t="str">
+      <c r="U10" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -3215,7 +3208,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W10" s="51" t="str">
+      <c r="W10" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -3242,12 +3235,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D11" s="26"/>
+      <c r="D11" s="72"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="25"/>
+      <c r="I11" s="72"/>
       <c r="J11" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -3335,7 +3328,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O10</f>
         <v>0</v>
       </c>
-      <c r="P11" s="51">
+      <c r="P11" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -3345,7 +3338,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R11" s="51" t="str">
+      <c r="R11" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -3365,7 +3358,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U11" s="51" t="str">
+      <c r="U11" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -3379,7 +3372,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W11" s="51" t="str">
+      <c r="W11" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -3405,12 +3398,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D12" s="26"/>
+      <c r="D12" s="72"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="25"/>
+      <c r="I12" s="72"/>
       <c r="J12" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -3498,7 +3491,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O11</f>
         <v>0</v>
       </c>
-      <c r="P12" s="51">
+      <c r="P12" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -3508,7 +3501,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R12" s="51" t="str">
+      <c r="R12" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -3528,7 +3521,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U12" s="51" t="str">
+      <c r="U12" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -3542,7 +3535,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W12" s="51" t="str">
+      <c r="W12" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -3568,12 +3561,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D13" s="26"/>
+      <c r="D13" s="72"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="25"/>
+      <c r="I13" s="72"/>
       <c r="J13" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -3661,7 +3654,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O12</f>
         <v>0</v>
       </c>
-      <c r="P13" s="51">
+      <c r="P13" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -3671,7 +3664,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R13" s="51" t="str">
+      <c r="R13" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -3691,7 +3684,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U13" s="51" t="str">
+      <c r="U13" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -3705,7 +3698,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W13" s="51" t="str">
+      <c r="W13" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -3731,12 +3724,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D14" s="26"/>
+      <c r="D14" s="72"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="25"/>
+      <c r="I14" s="72"/>
       <c r="J14" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -3824,7 +3817,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O13</f>
         <v>0</v>
       </c>
-      <c r="P14" s="51">
+      <c r="P14" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -3834,7 +3827,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R14" s="51" t="str">
+      <c r="R14" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -3854,7 +3847,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U14" s="51" t="str">
+      <c r="U14" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -3868,7 +3861,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W14" s="51" t="str">
+      <c r="W14" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -3896,12 +3889,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D15" s="26"/>
+      <c r="D15" s="72"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="25"/>
+      <c r="I15" s="72"/>
       <c r="J15" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -3989,7 +3982,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O14</f>
         <v>0</v>
       </c>
-      <c r="P15" s="51">
+      <c r="P15" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -3999,7 +3992,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R15" s="51" t="str">
+      <c r="R15" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -4019,7 +4012,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U15" s="51" t="str">
+      <c r="U15" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -4033,7 +4026,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W15" s="51" t="str">
+      <c r="W15" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -4060,12 +4053,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D16" s="26"/>
+      <c r="D16" s="72"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="25"/>
+      <c r="I16" s="72"/>
       <c r="J16" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -4153,7 +4146,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O15</f>
         <v>0</v>
       </c>
-      <c r="P16" s="51">
+      <c r="P16" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -4163,7 +4156,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R16" s="51" t="str">
+      <c r="R16" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -4183,7 +4176,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U16" s="51" t="str">
+      <c r="U16" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -4197,7 +4190,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W16" s="51" t="str">
+      <c r="W16" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -4223,12 +4216,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D17" s="26"/>
+      <c r="D17" s="72"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="25"/>
+      <c r="I17" s="72"/>
       <c r="J17" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -4316,7 +4309,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O16</f>
         <v>0</v>
       </c>
-      <c r="P17" s="51">
+      <c r="P17" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -4326,7 +4319,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R17" s="51" t="str">
+      <c r="R17" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -4346,7 +4339,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U17" s="51" t="str">
+      <c r="U17" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -4360,7 +4353,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W17" s="51" t="str">
+      <c r="W17" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -4386,12 +4379,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D18" s="26"/>
+      <c r="D18" s="72"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="25"/>
+      <c r="I18" s="72"/>
       <c r="J18" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -4479,7 +4472,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O17</f>
         <v>0</v>
       </c>
-      <c r="P18" s="51">
+      <c r="P18" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -4489,7 +4482,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R18" s="51" t="str">
+      <c r="R18" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -4509,7 +4502,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U18" s="51" t="str">
+      <c r="U18" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -4523,7 +4516,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W18" s="51" t="str">
+      <c r="W18" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -4549,12 +4542,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D19" s="26"/>
+      <c r="D19" s="72"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="25"/>
+      <c r="I19" s="72"/>
       <c r="J19" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -4642,7 +4635,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O18</f>
         <v>0</v>
       </c>
-      <c r="P19" s="51">
+      <c r="P19" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -4652,7 +4645,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R19" s="51" t="str">
+      <c r="R19" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -4672,7 +4665,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U19" s="51" t="str">
+      <c r="U19" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -4686,7 +4679,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W19" s="51" t="str">
+      <c r="W19" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -4712,12 +4705,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D20" s="26"/>
+      <c r="D20" s="72"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="25"/>
+      <c r="I20" s="72"/>
       <c r="J20" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -4805,7 +4798,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O19</f>
         <v>0</v>
       </c>
-      <c r="P20" s="51">
+      <c r="P20" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -4815,7 +4808,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R20" s="51" t="str">
+      <c r="R20" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -4835,7 +4828,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U20" s="51" t="str">
+      <c r="U20" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -4849,7 +4842,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W20" s="51" t="str">
+      <c r="W20" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -4875,12 +4868,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D21" s="26"/>
+      <c r="D21" s="72"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-      <c r="I21" s="25"/>
+      <c r="I21" s="72"/>
       <c r="J21" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -4968,7 +4961,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O20</f>
         <v>0</v>
       </c>
-      <c r="P21" s="51">
+      <c r="P21" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -4978,7 +4971,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R21" s="51" t="str">
+      <c r="R21" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -4998,7 +4991,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U21" s="51" t="str">
+      <c r="U21" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -5012,7 +5005,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W21" s="51" t="str">
+      <c r="W21" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -5038,12 +5031,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D22" s="26"/>
+      <c r="D22" s="72"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-      <c r="I22" s="25"/>
+      <c r="I22" s="72"/>
       <c r="J22" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -5131,7 +5124,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O21</f>
         <v>0</v>
       </c>
-      <c r="P22" s="51">
+      <c r="P22" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -5141,7 +5134,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R22" s="51" t="str">
+      <c r="R22" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -5161,7 +5154,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U22" s="51" t="str">
+      <c r="U22" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -5175,7 +5168,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W22" s="51" t="str">
+      <c r="W22" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -5201,12 +5194,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D23" s="26"/>
+      <c r="D23" s="72"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="25"/>
+      <c r="I23" s="72"/>
       <c r="J23" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -5294,7 +5287,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O22</f>
         <v>0</v>
       </c>
-      <c r="P23" s="51">
+      <c r="P23" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -5304,7 +5297,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R23" s="51" t="str">
+      <c r="R23" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -5324,7 +5317,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U23" s="51" t="str">
+      <c r="U23" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -5338,7 +5331,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W23" s="51" t="str">
+      <c r="W23" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -5364,12 +5357,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D24" s="26"/>
+      <c r="D24" s="72"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-      <c r="I24" s="25"/>
+      <c r="I24" s="72"/>
       <c r="J24" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -5457,7 +5450,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O23</f>
         <v>0</v>
       </c>
-      <c r="P24" s="51">
+      <c r="P24" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -5467,7 +5460,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R24" s="51" t="str">
+      <c r="R24" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -5487,7 +5480,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U24" s="51" t="str">
+      <c r="U24" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -5501,7 +5494,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W24" s="51" t="str">
+      <c r="W24" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -5527,12 +5520,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D25" s="26"/>
+      <c r="D25" s="72"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="I25" s="25"/>
+      <c r="I25" s="72"/>
       <c r="J25" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -5620,7 +5613,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O24</f>
         <v>0</v>
       </c>
-      <c r="P25" s="51">
+      <c r="P25" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -5630,7 +5623,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R25" s="51" t="str">
+      <c r="R25" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -5650,7 +5643,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U25" s="51" t="str">
+      <c r="U25" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -5664,7 +5657,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W25" s="51" t="str">
+      <c r="W25" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -5690,12 +5683,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D26" s="26"/>
+      <c r="D26" s="72"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
-      <c r="I26" s="25"/>
+      <c r="I26" s="72"/>
       <c r="J26" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -5783,7 +5776,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O25</f>
         <v>0</v>
       </c>
-      <c r="P26" s="51">
+      <c r="P26" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -5793,7 +5786,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R26" s="51" t="str">
+      <c r="R26" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -5813,7 +5806,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U26" s="51" t="str">
+      <c r="U26" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -5827,7 +5820,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W26" s="51" t="str">
+      <c r="W26" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -5853,12 +5846,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D27" s="26"/>
+      <c r="D27" s="72"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
-      <c r="I27" s="25"/>
+      <c r="I27" s="72"/>
       <c r="J27" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -5946,7 +5939,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O26</f>
         <v>0</v>
       </c>
-      <c r="P27" s="51">
+      <c r="P27" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -5956,7 +5949,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R27" s="51" t="str">
+      <c r="R27" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -5976,7 +5969,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U27" s="51" t="str">
+      <c r="U27" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -5990,7 +5983,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W27" s="51" t="str">
+      <c r="W27" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -6016,12 +6009,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D28" s="26"/>
+      <c r="D28" s="72"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-      <c r="I28" s="25"/>
+      <c r="I28" s="72"/>
       <c r="J28" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -6109,7 +6102,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O27</f>
         <v>0</v>
       </c>
-      <c r="P28" s="51">
+      <c r="P28" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -6119,7 +6112,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R28" s="51" t="str">
+      <c r="R28" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -6139,7 +6132,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U28" s="51" t="str">
+      <c r="U28" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -6153,7 +6146,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W28" s="51" t="str">
+      <c r="W28" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -6179,12 +6172,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D29" s="26"/>
+      <c r="D29" s="72"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
-      <c r="I29" s="25"/>
+      <c r="I29" s="72"/>
       <c r="J29" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -6272,7 +6265,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O28</f>
         <v>0</v>
       </c>
-      <c r="P29" s="51">
+      <c r="P29" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -6282,7 +6275,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R29" s="51" t="str">
+      <c r="R29" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -6302,7 +6295,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U29" s="51" t="str">
+      <c r="U29" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -6316,7 +6309,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W29" s="51" t="str">
+      <c r="W29" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -6342,12 +6335,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D30" s="26"/>
+      <c r="D30" s="72"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
-      <c r="I30" s="25"/>
+      <c r="I30" s="72"/>
       <c r="J30" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -6435,7 +6428,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O29</f>
         <v>0</v>
       </c>
-      <c r="P30" s="51">
+      <c r="P30" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -6445,7 +6438,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R30" s="51" t="str">
+      <c r="R30" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -6465,7 +6458,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U30" s="51" t="str">
+      <c r="U30" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -6479,7 +6472,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W30" s="51" t="str">
+      <c r="W30" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -6505,12 +6498,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D31" s="26"/>
+      <c r="D31" s="72"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
-      <c r="I31" s="25"/>
+      <c r="I31" s="72"/>
       <c r="J31" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -6598,7 +6591,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O30</f>
         <v>0</v>
       </c>
-      <c r="P31" s="51">
+      <c r="P31" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -6608,7 +6601,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R31" s="51" t="str">
+      <c r="R31" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -6628,7 +6621,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U31" s="51" t="str">
+      <c r="U31" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -6642,7 +6635,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W31" s="51" t="str">
+      <c r="W31" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -6668,12 +6661,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D32" s="26"/>
+      <c r="D32" s="72"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
-      <c r="I32" s="25"/>
+      <c r="I32" s="72"/>
       <c r="J32" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -6761,7 +6754,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O31</f>
         <v>0</v>
       </c>
-      <c r="P32" s="51">
+      <c r="P32" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -6771,7 +6764,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R32" s="51" t="str">
+      <c r="R32" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -6791,7 +6784,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U32" s="51" t="str">
+      <c r="U32" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -6805,7 +6798,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W32" s="51" t="str">
+      <c r="W32" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -6831,12 +6824,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D33" s="26"/>
+      <c r="D33" s="72"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
-      <c r="I33" s="25"/>
+      <c r="I33" s="72"/>
       <c r="J33" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -6924,7 +6917,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O32</f>
         <v>0</v>
       </c>
-      <c r="P33" s="51">
+      <c r="P33" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -6934,7 +6927,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R33" s="51" t="str">
+      <c r="R33" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -6954,7 +6947,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U33" s="51" t="str">
+      <c r="U33" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -6968,7 +6961,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W33" s="51" t="str">
+      <c r="W33" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -6994,12 +6987,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D34" s="26"/>
+      <c r="D34" s="72"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
-      <c r="I34" s="25"/>
+      <c r="I34" s="72"/>
       <c r="J34" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -7087,7 +7080,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O33</f>
         <v>0</v>
       </c>
-      <c r="P34" s="51">
+      <c r="P34" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -7097,7 +7090,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R34" s="51" t="str">
+      <c r="R34" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -7117,7 +7110,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U34" s="51" t="str">
+      <c r="U34" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -7131,7 +7124,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W34" s="51" t="str">
+      <c r="W34" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -7157,12 +7150,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D35" s="26"/>
+      <c r="D35" s="72"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
-      <c r="I35" s="25"/>
+      <c r="I35" s="72"/>
       <c r="J35" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -7250,7 +7243,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O34</f>
         <v>0</v>
       </c>
-      <c r="P35" s="51">
+      <c r="P35" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -7260,7 +7253,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R35" s="51" t="str">
+      <c r="R35" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -7280,7 +7273,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U35" s="51" t="str">
+      <c r="U35" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -7294,7 +7287,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W35" s="51" t="str">
+      <c r="W35" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -7320,12 +7313,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D36" s="26"/>
+      <c r="D36" s="72"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
-      <c r="I36" s="25"/>
+      <c r="I36" s="72"/>
       <c r="J36" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -7413,7 +7406,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O35</f>
         <v>0</v>
       </c>
-      <c r="P36" s="51">
+      <c r="P36" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -7423,7 +7416,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R36" s="51" t="str">
+      <c r="R36" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -7443,7 +7436,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U36" s="51" t="str">
+      <c r="U36" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -7457,7 +7450,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W36" s="51" t="str">
+      <c r="W36" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -7483,12 +7476,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D37" s="26"/>
+      <c r="D37" s="72"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
-      <c r="I37" s="25"/>
+      <c r="I37" s="72"/>
       <c r="J37" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -7576,7 +7569,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O36</f>
         <v>0</v>
       </c>
-      <c r="P37" s="51">
+      <c r="P37" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -7586,7 +7579,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R37" s="51" t="str">
+      <c r="R37" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -7606,7 +7599,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U37" s="51" t="str">
+      <c r="U37" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -7620,7 +7613,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W37" s="51" t="str">
+      <c r="W37" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -7646,12 +7639,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D38" s="26"/>
+      <c r="D38" s="72"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
-      <c r="I38" s="25"/>
+      <c r="I38" s="72"/>
       <c r="J38" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -7739,7 +7732,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O37</f>
         <v>0</v>
       </c>
-      <c r="P38" s="51">
+      <c r="P38" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -7749,7 +7742,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R38" s="51" t="str">
+      <c r="R38" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -7769,7 +7762,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U38" s="51" t="str">
+      <c r="U38" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -7783,7 +7776,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W38" s="51" t="str">
+      <c r="W38" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -7809,12 +7802,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D39" s="26"/>
+      <c r="D39" s="72"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
-      <c r="I39" s="25"/>
+      <c r="I39" s="72"/>
       <c r="J39" s="4">
         <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -7902,7 +7895,7 @@
         tblHoras[Horas Trabalhadas Além Jornada])+O38</f>
         <v>0</v>
       </c>
-      <c r="P39" s="51">
+      <c r="P39" s="48">
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
@@ -7912,7 +7905,7 @@
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R39" s="51" t="str">
+      <c r="R39" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
@@ -7932,7 +7925,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U39" s="51" t="str">
+      <c r="U39" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
@@ -7946,7 +7939,7 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W39" s="51" t="str">
+      <c r="W39" s="48" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
@@ -7968,7 +7961,7 @@
       <c r="Y40" s="24"/>
     </row>
     <row r="41" spans="2:25" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="X41" s="36" t="s">
+      <c r="X41" s="34" t="s">
         <v>108</v>
       </c>
       <c r="Y41" s="24"/>
@@ -8208,44 +8201,44 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="41"/>
+    <col min="1" max="16384" width="9.140625" style="39"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
     </row>
     <row r="5" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B5" s="42"/>
-      <c r="C5" s="42" t="s">
+      <c r="B5" s="40"/>
+      <c r="C5" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
     </row>
     <row r="6" spans="2:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="B6" s="42"/>
-      <c r="C6" s="49" t="s">
+      <c r="B6" s="40"/>
+      <c r="C6" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="42"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="40"/>
     </row>
     <row r="7" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>

</xml_diff>

<commit_message>
Alterações da jornada diferenciada por dia de semana e correções da planilha anual
</commit_message>
<xml_diff>
--- a/Controle de Ponto.xlsx
+++ b/Controle de Ponto.xlsx
@@ -5,7 +5,7 @@
   <workbookPr date1904="1" codeName="EstaPasta_de_trabalho" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\Controle de Ponto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ExcelGuru-ControlePonto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,8 +20,8 @@
   <definedNames>
     <definedName name="CARENCIA">Config!$D$5</definedName>
     <definedName name="JORNADA">Config!$D$7</definedName>
-    <definedName name="JORNADA_PERIODO_1">Config!$D$21</definedName>
-    <definedName name="JORNADA_PERIODO_2">Config!$D$22</definedName>
+    <definedName name="JORNADA_PERIODO_1">Config!$D$22</definedName>
+    <definedName name="JORNADA_PERIODO_2">Config!$D$23</definedName>
     <definedName name="LIMITE">Config!$D$3</definedName>
     <definedName name="lst_Mes">tbl_Mes[Mês]</definedName>
     <definedName name="lstEvento">tblEvento[Evento]</definedName>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="112">
   <si>
     <t>Data</t>
   </si>
@@ -429,6 +429,15 @@
   </si>
   <si>
     <t>v7.4</t>
+  </si>
+  <si>
+    <t>1º Período</t>
+  </si>
+  <si>
+    <t>2º Período</t>
+  </si>
+  <si>
+    <t>Total Jornada</t>
   </si>
 </sst>
 </file>
@@ -600,7 +609,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -779,12 +788,98 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="6"/>
+      </top>
+      <bottom style="medium">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color theme="5"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="6"/>
+      </top>
+      <bottom style="medium">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color theme="5"/>
+      </right>
+      <top style="medium">
+        <color theme="6"/>
+      </top>
+      <bottom style="medium">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color theme="5"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color theme="5"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color theme="5"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color theme="5"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -928,6 +1023,47 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -946,8 +1082,25 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -955,11 +1108,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -975,79 +1132,12 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="65">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="h:mm;@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="h:mm;@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="h:mm;@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
+  <dxfs count="67">
     <dxf>
       <font>
         <i/>
@@ -1174,6 +1264,23 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="h:mm;@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -1181,6 +1288,37 @@
       <numFmt numFmtId="166" formatCode="h:mm;@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="h:mm;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="h:mm;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="h:mm;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[$-416]d\-mmm;@"/>
@@ -1302,6 +1440,62 @@
     <dxf>
       <numFmt numFmtId="166" formatCode="h:mm;@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="double">
+          <color theme="5"/>
+        </right>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="medium">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="h:mm;@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="medium">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="h:mm;@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="double">
+          <color theme="5"/>
+        </left>
+        <right/>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="medium">
+          <color auto="1"/>
+        </horizontal>
+      </border>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1451,58 +1645,62 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tblEvento" displayName="tblEvento" ref="A2:F13" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tblEvento" displayName="tblEvento" ref="A2:F13" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
   <sortState ref="A3:F13">
     <sortCondition ref="A8"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="Evento" dataDxfId="62"/>
-    <tableColumn id="2" name="Colorir Linha" dataDxfId="61"/>
-    <tableColumn id="5" name="Colorir Período" dataDxfId="60"/>
-    <tableColumn id="6" name="Libera o Período" dataDxfId="59"/>
-    <tableColumn id="4" name="Conta hora Extra" dataDxfId="58"/>
-    <tableColumn id="3" name="Descrição" dataDxfId="57"/>
+    <tableColumn id="1" name="Evento" dataDxfId="64"/>
+    <tableColumn id="2" name="Colorir Linha" dataDxfId="63"/>
+    <tableColumn id="5" name="Colorir Período" dataDxfId="62"/>
+    <tableColumn id="6" name="Libera o Período" dataDxfId="61"/>
+    <tableColumn id="4" name="Conta hora Extra" dataDxfId="60"/>
+    <tableColumn id="3" name="Descrição" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="tblLimiteHora" displayName="tblLimiteHora" ref="H2:J4" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="tblLimiteHora" displayName="tblLimiteHora" ref="H2:J4" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
   <autoFilter ref="H2:J4"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Limite de horas" dataDxfId="54"/>
-    <tableColumn id="3" name="Limite" dataDxfId="53"/>
-    <tableColumn id="2" name="h" dataDxfId="52"/>
+    <tableColumn id="1" name="Limite de horas" dataDxfId="56"/>
+    <tableColumn id="3" name="Limite" dataDxfId="55"/>
+    <tableColumn id="2" name="h" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="tbl_Mes" displayName="tbl_Mes" ref="L2:L14" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="tbl_Mes" displayName="tbl_Mes" ref="L2:L14" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <autoFilter ref="L2:L14"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Mês" dataDxfId="49"/>
+    <tableColumn id="1" name="Mês" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tblDiaUtil" displayName="tblDiaUtil" ref="B10:E17" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
-  <tableColumns count="4">
-    <tableColumn id="1" name="Dia da Semana" dataDxfId="45"/>
-    <tableColumn id="4" name="Abreviatura" dataDxfId="44"/>
-    <tableColumn id="2" name="É dia util?" dataDxfId="43"/>
-    <tableColumn id="3" name="Jornada Diferenciada?" dataDxfId="42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tblDiaUtil" displayName="tblDiaUtil" ref="B11:G18" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
+  <tableColumns count="6">
+    <tableColumn id="1" name="Dia da Semana" dataDxfId="47"/>
+    <tableColumn id="4" name="Abreviatura" dataDxfId="46"/>
+    <tableColumn id="2" name="É dia util?" dataDxfId="45"/>
+    <tableColumn id="3" name="1º Período" dataDxfId="44"/>
+    <tableColumn id="5" name="2º Período" dataDxfId="43"/>
+    <tableColumn id="6" name="Total Jornada" dataDxfId="42">
+      <calculatedColumnFormula>IF((tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]])&gt;0,tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]],"")</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="tblDiaUtil7" displayName="tblDiaUtil7" ref="B20:D22" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="tblDiaUtil7" displayName="tblDiaUtil7" ref="B21:D23" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <tableColumns count="3">
     <tableColumn id="1" name="Período" dataDxfId="39"/>
     <tableColumn id="4" name="Abreviatura" dataDxfId="38"/>
@@ -1518,53 +1716,59 @@
     <tableColumn id="1" name="Data" dataDxfId="22">
       <calculatedColumnFormula>IF(B8&lt;&gt;"",IF(DAY(B8+1)=1,"",B8+1),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Dia" dataDxfId="5">
+    <tableColumn id="2" name="Dia" dataDxfId="21">
       <calculatedColumnFormula>TEXT(tblHoras[[#This Row],[Data]],"ddd")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Evento _x000a_(1º Período)" dataDxfId="3"/>
-    <tableColumn id="4" name="Entrada - 1" dataDxfId="4"/>
-    <tableColumn id="5" name="Saída - 1 (Almoço)" dataDxfId="21"/>
-    <tableColumn id="6" name="Entrada - 2 (Almoço)" dataDxfId="20"/>
-    <tableColumn id="7" name="Saída - 2" dataDxfId="2"/>
-    <tableColumn id="13" name="Evento _x000a_(2º Período)" dataDxfId="0"/>
-    <tableColumn id="15" name="Horas Trabalhadas (1º Período)" dataDxfId="1">
-      <calculatedColumnFormula>IF($B$6&lt;&gt;"",IF(AND(tblHoras[[#This Row],[Evento 
-(1º Período)]]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[[#This Row],[Evento 
-(1º Período)]],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[[#This Row],[Evento 
-(1º Período)]],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
-        IF(AND(ISNUMBER(tblHoras[[#This Row],[Saída - 1 (Almoço)]]),ISNUMBER(tblHoras[[#This Row],[Entrada - 1]])),
-              IF(OR(AND(tblHoras[[#This Row],[Evento 
-(1º Período)]]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[[#This Row],[Evento 
-(1º Período)]],tblEvento[],Tabelas!$E$1,FALSE)),FALSE,VLOOKUP(tblHoras[[#This Row],[Evento 
-(1º Período)]],tblEvento[],Tabelas!$E$1,FALSE)="Sim")),IF(VLOOKUP(TEXT(tblHoras[[#This Row],[Data]],"dddd"),tblDiaUtil[],2,FALSE)="Não",TRUE,FALSE)),
-                   tblHoras[[#This Row],[Saída - 1 (Almoço)]]-tblHoras[[#This Row],[Entrada - 1]],
-                   IF(OR(HOUR(tblHoras[[#This Row],[Saída - 1 (Almoço)]]-tblHoras[[#This Row],[Entrada - 1]])&gt;0,ROUND(tblHoras[[#This Row],[Saída - 1 (Almoço)]]-tblHoras[[#This Row],[Entrada - 1]],6)&gt;ROUND(CARENCIA,6)),
-                          tblHoras[[#This Row],[Saída - 1 (Almoço)]]-tblHoras[[#This Row],[Entrada - 1]],
+    <tableColumn id="3" name="Evento _x000a_(1º Período)" dataDxfId="20"/>
+    <tableColumn id="4" name="Entrada - 1" dataDxfId="19"/>
+    <tableColumn id="5" name="Saída - 1 (Almoço)" dataDxfId="18"/>
+    <tableColumn id="6" name="Entrada - 2 (Almoço)" dataDxfId="17"/>
+    <tableColumn id="7" name="Saída - 2" dataDxfId="16"/>
+    <tableColumn id="13" name="Evento _x000a_(2º Período)" dataDxfId="15"/>
+    <tableColumn id="15" name="Horas Trabalhadas (1º Período)" dataDxfId="14">
+      <calculatedColumnFormula>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
+(1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
+        IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
+              IF(OR(AND(tblHoras[Evento 
+(1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[],Tabelas!$E$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim")),IF(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],2,FALSE)="Não",TRUE,FALSE)),
+                   tblHoras[Saída - 1 (Almoço)]-tblHoras[Entrada - 1],
+                   IF(OR(HOUR(tblHoras[Saída - 1 (Almoço)]-tblHoras[Entrada - 1])&gt;0,ROUND(tblHoras[Saída - 1 (Almoço)]-tblHoras[Entrada - 1],6)&gt;ROUND(CARENCIA,6)),
+                          tblHoras[Saída - 1 (Almoço)]-tblHoras[Entrada - 1],
                           0)),
                     0)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Horas Trabalhadas (2º Período)" dataDxfId="19">
-      <calculatedColumnFormula>IF($B$6&lt;&gt;"",IF(AND(tblHoras[[#This Row],[Evento 
-(2º Período)]]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[[#This Row],[Evento 
-(2º Período)]],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[[#This Row],[Evento 
-(2º Período)]],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
-        IF(AND(ISNUMBER(tblHoras[[#This Row],[Saída - 2]]),ISNUMBER(tblHoras[[#This Row],[Entrada - 2 (Almoço)]])),
-              IF(OR(AND(tblHoras[[#This Row],[Evento 
-(2º Período)]]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[[#This Row],[Evento 
-(2º Período)]],tblEvento[],Tabelas!$E$1,FALSE)),FALSE,VLOOKUP(tblHoras[[#This Row],[Evento 
-(2º Período)]],tblEvento[],Tabelas!$E$1,FALSE)="Sim")),IF(VLOOKUP(TEXT(tblHoras[[#This Row],[Data]],"dddd"),tblDiaUtil[],2,FALSE)="Não",TRUE,FALSE)),
-                   tblHoras[[#This Row],[Saída - 2]]-tblHoras[[#This Row],[Entrada - 2 (Almoço)]],
-                   IF(OR(HOUR(tblHoras[[#This Row],[Saída - 2]]-tblHoras[[#This Row],[Entrada - 2 (Almoço)]])&gt;0,MINUTE(tblHoras[[#This Row],[Saída - 2]]-tblHoras[[#This Row],[Entrada - 2 (Almoço)]])&gt;CARENCIA),
-                         tblHoras[[#This Row],[Saída - 2]]-tblHoras[[#This Row],[Entrada - 2 (Almoço)]],
+    <tableColumn id="16" name="Horas Trabalhadas (2º Período)" dataDxfId="13">
+      <calculatedColumnFormula>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
+(2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
+        IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
+              IF(OR(AND(tblHoras[Evento 
+(2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[],Tabelas!$E$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim")),IF(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],2,FALSE)="Não",TRUE,FALSE)),
+                   tblHoras[Saída - 2]-tblHoras[Entrada - 2 (Almoço)],
+                   IF(OR(HOUR(tblHoras[Saída - 2]-tblHoras[Entrada - 2 (Almoço)])&gt;0,MINUTE(tblHoras[Saída - 2]-tblHoras[Entrada - 2 (Almoço)])&gt;CARENCIA),
+                         tblHoras[Saída - 2]-tblHoras[Entrada - 2 (Almoço)],
                          0)),
        0)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Horas Trabalhadas" dataDxfId="18">
+    <tableColumn id="8" name="Horas Trabalhadas" dataDxfId="12">
       <calculatedColumnFormula>tblHoras[[#This Row],[Horas Trabalhadas (1º Período)]]+tblHoras[[#This Row],[Horas Trabalhadas (2º Período)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Jornada Diária" dataDxfId="17">
+    <tableColumn id="17" name="Jornada Diária" dataDxfId="11">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Data]]&lt;&gt;"",
         IF(
 AND(VLOOKUP(TEXT(tblHoras[[#This Row],[Data]],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[[#This Row],[Evento 
@@ -1572,11 +1776,11 @@
 (1º Período)]],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[[#This Row],[Evento 
 (2º Período)]]&lt;&gt;"",IF(VLOOKUP(tblHoras[[#This Row],[Evento 
 (2º Período)]],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[[#This Row],[Dia]],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[[#This Row],[Dia]],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[[#This Row],[Dia]],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[[#This Row],[Dia]],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Horas Trabalhadas Além Jornada" dataDxfId="16">
+    <tableColumn id="11" name="Horas Trabalhadas Além Jornada" dataDxfId="10">
       <calculatedColumnFormula>IF(OR(tblHoras[[#This Row],[Horas Trabalhadas (1º Período)]]&lt;&gt;0,tblHoras[[#This Row],[Horas Trabalhadas (2º Período)]]&lt;&gt;0),
         IF(ISNUMBER(tblHoras[[#This Row],[Jornada Diária]]),
               IF(tblHoras[[#This Row],[Jornada Diária]]&gt;(tblHoras[[#This Row],[Horas Trabalhadas (2º Período)]]+tblHoras[[#This Row],[Horas Trabalhadas (1º Período)]]),
@@ -1599,7 +1803,7 @@
 (2º Período)]],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
 )))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Saldo de Horas" dataDxfId="15">
+    <tableColumn id="18" name="Saldo de Horas" dataDxfId="9">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&gt;0,
         IF(tblHoras[[#This Row],[Jornada Diária]]&lt;&gt;"",
               IF(HOUR(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]])&gt;=VLOOKUP(LIMITE,tblLimiteHora[],Tabelas!$I$1,FALSE),
@@ -1608,23 +1812,23 @@
               tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]),
         0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="Saldo de Horas (Decimal)" dataDxfId="14">
+    <tableColumn id="20" name="Saldo de Horas (Decimal)" dataDxfId="8">
       <calculatedColumnFormula>tblHoras[[#This Row],[Saldo de Horas]]*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="Atrasos_x000a_(horas)" dataDxfId="13">
+    <tableColumn id="19" name="Atrasos_x000a_(horas)" dataDxfId="7">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&lt;0,IF(OR(tblHoras[[#This Row],[Evento 
 (1º Período)]]="",tblHoras[[#This Row],[Evento 
 (2º Período)]]=""),tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]],""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Atrasos (Decimal)" dataDxfId="12">
+    <tableColumn id="21" name="Atrasos (Decimal)" dataDxfId="6">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Faltas_x000a_(dias)" dataDxfId="11">
+    <tableColumn id="14" name="Faltas_x000a_(dias)" dataDxfId="5">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Jornada Diária]]&lt;&gt;"",IF((N(tblHoras[[#This Row],[Jornada Diária]])-ABS(N(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]])))=0,1,""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Hora Extra Normal" dataDxfId="10">
+    <tableColumn id="10" name="Hora Extra Normal" dataDxfId="4">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[[#This Row],[Data]],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[[#This Row],[Evento 
 (1º Período)]]&lt;&gt;"",IF(VLOOKUP(tblHoras[[#This Row],[Evento 
@@ -1633,10 +1837,10 @@
 (2º Período)]],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
 tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]],""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="Hora Extra Normal (Decimal)" dataDxfId="9">
+    <tableColumn id="22" name="Hora Extra Normal (Decimal)" dataDxfId="3">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Hora Extra _x000a_Especial" dataDxfId="8">
+    <tableColumn id="9" name="Hora Extra _x000a_Especial" dataDxfId="2">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[[#This Row],[Data]],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[[#This Row],[Evento 
 (1º Período)]]&lt;&gt;"",IF(VLOOKUP(tblHoras[[#This Row],[Evento 
@@ -1645,12 +1849,12 @@
 (2º Período)]],tblEvento[],Tabelas!$E$1,FALSE)="Sim",TRUE,FALSE),FALSE)),
 tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]],""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="Hora Extra Especial (Decimal)" dataDxfId="7">
+    <tableColumn id="23" name="Hora Extra Especial (Decimal)" dataDxfId="1">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Informação" dataDxfId="6">
+    <tableColumn id="12" name="Informação" dataDxfId="0">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Evento 
 (1º Período)]]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[[#This Row],[Evento 
 (1º Período)]],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[[#This Row],[Evento 
@@ -2293,7 +2497,7 @@
   <sheetPr codeName="plnConfig">
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B1:H27"/>
+  <dimension ref="B1:H28"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
@@ -2305,20 +2509,18 @@
     <col min="2" max="2" width="18" style="5" customWidth="1"/>
     <col min="3" max="3" width="18" style="5" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="15" style="5" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="5"/>
-    <col min="7" max="7" width="3.5703125" style="5" customWidth="1"/>
+    <col min="5" max="7" width="12.7109375" style="5" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="53" t="s">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="55"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="67"/>
     </row>
-    <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="19" t="s">
         <v>19</v>
       </c>
@@ -2327,7 +2529,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="19" t="s">
         <v>32</v>
       </c>
@@ -2339,7 +2541,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="19" t="s">
         <v>37</v>
       </c>
@@ -2348,164 +2550,206 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="56" t="s">
+    <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="58"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
     </row>
-    <row r="10" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
+    <row r="10" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="53"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="71" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="72"/>
+      <c r="G10" s="73"/>
+    </row>
+    <row r="11" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C11" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D11" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>77</v>
+      <c r="E11" s="58" t="s">
+        <v>109</v>
+      </c>
+      <c r="F11" s="56" t="s">
+        <v>110</v>
+      </c>
+      <c r="G11" s="59" t="s">
+        <v>111</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="21" t="s">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C12" s="21" t="s">
         <v>78</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="38"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>79</v>
       </c>
       <c r="D12" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="38"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="61" t="str">
+        <f>IF((tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]])&gt;0,tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]],"")</f>
+        <v/>
+      </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D13" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="38"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="61" t="str">
+        <f>IF((tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]])&gt;0,tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]],"")</f>
+        <v/>
+      </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D14" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="38"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="61" t="str">
+        <f>IF((tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]])&gt;0,tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]],"")</f>
+        <v/>
+      </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="38"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="61" t="str">
+        <f>IF((tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]])&gt;0,tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]],"")</f>
+        <v/>
+      </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="21" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="38"/>
+        <v>30</v>
+      </c>
+      <c r="E16" s="60"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="61" t="str">
+        <f>IF((tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]])&gt;0,tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]],"")</f>
+        <v/>
+      </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D17" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="38"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="61" t="str">
+        <f>IF((tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]])&gt;0,tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]],"")</f>
+        <v/>
+      </c>
     </row>
-    <row r="19" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="56" t="s">
+    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="62"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="64" t="str">
+        <f>IF((tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]])&gt;0,tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="57"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="51" t="s">
+      <c r="C20" s="69"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="F19" s="50">
+      <c r="F20" s="50">
         <f>SUM(tblDiaUtil7[Qtd. Horas por Jornada])</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="G19" s="5">
-        <f>IF(F19&gt;0,IF(F19=JORNADA,1,0),"")</f>
+      <c r="G20" s="5">
+        <f>IF(F20&gt;0,IF(F20=JORNADA,1,0),"")</f>
         <v>1</v>
       </c>
-      <c r="H19" s="52" t="str">
-        <f>IF(G19=0,"A quantidade de horas por período deve ser igual à jornada diária","")</f>
+      <c r="H20" s="52" t="str">
+        <f>IF(G20=0,"A quantidade de horas por período deve ser igual à jornada diária","")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="9" t="s">
+    <row r="21" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C21" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D21" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="E20" s="9"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" s="49">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="E21" s="38"/>
+      <c r="E21" s="9"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D22" s="49">
         <v>0.16666666666666666</v>
@@ -2513,16 +2757,22 @@
       <c r="E22" s="38"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="21"/>
+      <c r="B23" s="21" t="s">
+        <v>105</v>
+      </c>
       <c r="C23" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="D23" s="22"/>
+        <v>79</v>
+      </c>
+      <c r="D23" s="49">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="E23" s="38"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
+      <c r="C24" s="21" t="s">
+        <v>80</v>
+      </c>
       <c r="D24" s="22"/>
       <c r="E24" s="38"/>
     </row>
@@ -2544,19 +2794,26 @@
       <c r="D27" s="22"/>
       <c r="E27" s="38"/>
     </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="38"/>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="9+MX/+Zq1SYuuJA2+APjigl5LM+/jyjLSaudMfNfRCLZmq4MLwZ4xMW8yxfGfTCtzoG5vjKtC/QsIWYwqDXv/w==" saltValue="45qhRGdImc2pB4p1/dSFcw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="3">
+  <sheetProtection algorithmName="SHA-512" hashValue="RnrvVp3tEDNTp8mdQPd60H5d7VLLpthwUsDdotXw3PsqfeHCjHQiw1zsv7QBUMP6fz7QFEcMcfCCQ4D2lR3Ing==" saltValue="ziJzkLVU3wAeLs4y4La38Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="4">
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="E10:G10"/>
   </mergeCells>
   <conditionalFormatting sqref="D7">
-    <cfRule type="timePeriod" dxfId="48" priority="4" timePeriod="lastMonth">
+    <cfRule type="timePeriod" dxfId="50" priority="4" timePeriod="lastMonth">
       <formula>AND(MONTH(D7)=MONTH(EDATE(TODAY(),0-1)),YEAR(D7)=YEAR(EDATE(TODAY(),0-1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G19">
+  <conditionalFormatting sqref="G20">
     <cfRule type="iconSet" priority="1">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -2569,10 +2826,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3">
       <formula1>lstLimiteHora</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11:D17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12:D18">
       <formula1>"Sim,Não"</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7 D5 D21:D22 F19">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7 D5 D22:D23 F20">
       <formula1>0</formula1>
       <formula2>0.999305555555556</formula2>
     </dataValidation>
@@ -2595,7 +2852,7 @@
   <dimension ref="A1:AG47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="8" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection activeCell="H10" sqref="H10"/>
       <selection pane="topRight" activeCell="H10" sqref="H10"/>
       <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
@@ -2632,7 +2889,7 @@
       <c r="G1" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="O1" s="59" t="str">
+      <c r="O1" s="74" t="str">
         <f>"*Limite de horas: " &amp; LIMITE &amp; "; e 
 *Contabiliza a partir de " &amp; TEXT(CARENCIA, "hh:mm") &amp; " hora(s) (para mais ou para menos);
 *Caso tenha Atestado em um dos períodos, o que ultrapassar de 4:00 horas de trabalho contabiliza hora positiva."</f>
@@ -2640,76 +2897,76 @@
 *Contabiliza a partir de 00:10 hora(s) (para mais ou para menos);
 *Caso tenha Atestado em um dos períodos, o que ultrapassar de 4:00 horas de trabalho contabiliza hora positiva.</v>
       </c>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
-      <c r="S1" s="59"/>
-      <c r="T1" s="59"/>
-      <c r="U1" s="59"/>
-      <c r="V1" s="59"/>
-      <c r="W1" s="59"/>
-      <c r="X1" s="59"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+      <c r="S1" s="74"/>
+      <c r="T1" s="74"/>
+      <c r="U1" s="74"/>
+      <c r="V1" s="74"/>
+      <c r="W1" s="74"/>
+      <c r="X1" s="74"/>
     </row>
     <row r="2" spans="2:29" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="6"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
       <c r="N2" s="24"/>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
-      <c r="Q2" s="59"/>
-      <c r="R2" s="59"/>
-      <c r="S2" s="59"/>
-      <c r="T2" s="59"/>
-      <c r="U2" s="59"/>
-      <c r="V2" s="59"/>
-      <c r="W2" s="59"/>
-      <c r="X2" s="59"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="74"/>
+      <c r="S2" s="74"/>
+      <c r="T2" s="74"/>
+      <c r="U2" s="74"/>
+      <c r="V2" s="74"/>
+      <c r="W2" s="74"/>
+      <c r="X2" s="74"/>
     </row>
     <row r="3" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
       <c r="G3" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="H3" s="64" t="s">
+      <c r="H3" s="82" t="s">
         <v>97</v>
       </c>
-      <c r="I3" s="65"/>
+      <c r="I3" s="83"/>
       <c r="N3" s="24"/>
-      <c r="O3" s="59"/>
-      <c r="P3" s="59"/>
-      <c r="Q3" s="59"/>
-      <c r="R3" s="59"/>
-      <c r="S3" s="59"/>
-      <c r="T3" s="59"/>
-      <c r="U3" s="59"/>
-      <c r="V3" s="59"/>
-      <c r="W3" s="59"/>
-      <c r="X3" s="59"/>
+      <c r="O3" s="74"/>
+      <c r="P3" s="74"/>
+      <c r="Q3" s="74"/>
+      <c r="R3" s="74"/>
+      <c r="S3" s="74"/>
+      <c r="T3" s="74"/>
+      <c r="U3" s="74"/>
+      <c r="V3" s="74"/>
+      <c r="W3" s="74"/>
+      <c r="X3" s="74"/>
     </row>
     <row r="4" spans="2:29" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="71"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="76"/>
       <c r="N4" s="24"/>
-      <c r="O4" s="59"/>
-      <c r="P4" s="59"/>
-      <c r="Q4" s="59"/>
-      <c r="R4" s="59"/>
-      <c r="S4" s="59"/>
-      <c r="T4" s="59"/>
-      <c r="U4" s="59"/>
-      <c r="V4" s="59"/>
-      <c r="W4" s="59"/>
-      <c r="X4" s="59"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="74"/>
+      <c r="Q4" s="74"/>
+      <c r="R4" s="74"/>
+      <c r="S4" s="74"/>
+      <c r="T4" s="74"/>
+      <c r="U4" s="74"/>
+      <c r="V4" s="74"/>
+      <c r="W4" s="74"/>
+      <c r="X4" s="74"/>
     </row>
     <row r="5" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="77" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="61"/>
+      <c r="C5" s="78"/>
       <c r="D5" s="28" t="s">
         <v>62</v>
       </c>
@@ -2744,8 +3001,8 @@
       <c r="X5" s="24"/>
     </row>
     <row r="6" spans="2:29" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="62"/>
-      <c r="C6" s="63"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="79"/>
       <c r="D6" s="29"/>
       <c r="E6" s="29"/>
       <c r="F6" s="31" t="str">
@@ -2755,15 +3012,15 @@
       <c r="N6" s="24"/>
       <c r="O6" s="24"/>
       <c r="P6" s="24"/>
-      <c r="Q6" s="66" t="s">
+      <c r="Q6" s="84" t="s">
         <v>95</v>
       </c>
-      <c r="R6" s="67"/>
-      <c r="S6" s="67"/>
-      <c r="T6" s="67"/>
-      <c r="U6" s="67"/>
-      <c r="V6" s="67"/>
-      <c r="W6" s="67"/>
+      <c r="R6" s="85"/>
+      <c r="S6" s="85"/>
+      <c r="T6" s="85"/>
+      <c r="U6" s="85"/>
+      <c r="V6" s="85"/>
+      <c r="W6" s="85"/>
       <c r="X6" s="24"/>
     </row>
     <row r="7" spans="2:29" x14ac:dyDescent="0.25">
@@ -2906,18 +3163,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D9" s="72"/>
+      <c r="D9" s="55"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="72"/>
+      <c r="I9" s="55"/>
       <c r="J9" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        IF(JORNADA_PERIODO_1&lt;&gt;"",JORNADA_PERIODO_1,JORNADA/2),
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -2931,11 +3191,14 @@
         <v>0</v>
       </c>
       <c r="K9" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        IF(JORNADA_PERIODO_2&lt;&gt;"",JORNADA_PERIODO_2,JORNADA/2),
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -2960,7 +3223,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -3071,18 +3334,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D10" s="72"/>
+      <c r="D10" s="55"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="72"/>
+      <c r="I10" s="55"/>
       <c r="J10" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -3096,11 +3362,14 @@
         <v>0</v>
       </c>
       <c r="K10" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -3125,7 +3394,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -3235,18 +3504,23 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D11" s="72"/>
+      <c r="D11" s="55" t="s">
+        <v>24</v>
+      </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="72"/>
+      <c r="I11" s="55"/>
       <c r="J11" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -3260,11 +3534,14 @@
         <v>0</v>
       </c>
       <c r="K11" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -3289,7 +3566,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -3386,7 +3663,7 @@
 (2º Período)]&lt;&gt;tblHoras[Evento 
 (1º Período)])," - " &amp; VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")</f>
-        <v/>
+        <v xml:space="preserve"> - Atestado Médico</v>
       </c>
     </row>
     <row r="12" spans="2:29" x14ac:dyDescent="0.25">
@@ -3398,18 +3675,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D12" s="72"/>
+      <c r="D12" s="55"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="72"/>
+      <c r="I12" s="55"/>
       <c r="J12" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -3423,11 +3703,14 @@
         <v>0</v>
       </c>
       <c r="K12" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -3452,7 +3735,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -3561,18 +3844,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D13" s="72"/>
+      <c r="D13" s="55"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="72"/>
+      <c r="I13" s="55"/>
       <c r="J13" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -3586,11 +3872,14 @@
         <v>0</v>
       </c>
       <c r="K13" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -3615,7 +3904,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -3724,18 +4013,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D14" s="72"/>
+      <c r="D14" s="55"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="72"/>
+      <c r="I14" s="55"/>
       <c r="J14" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -3749,11 +4041,14 @@
         <v>0</v>
       </c>
       <c r="K14" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -3778,7 +4073,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -3889,18 +4184,23 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D15" s="72"/>
+      <c r="D15" s="55" t="s">
+        <v>24</v>
+      </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="72"/>
+      <c r="I15" s="55"/>
       <c r="J15" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -3914,11 +4214,14 @@
         <v>0</v>
       </c>
       <c r="K15" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -3943,7 +4246,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -4040,7 +4343,7 @@
 (2º Período)]&lt;&gt;tblHoras[Evento 
 (1º Período)])," - " &amp; VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")</f>
-        <v/>
+        <v xml:space="preserve"> - Atestado Médico</v>
       </c>
       <c r="AB15" s="17"/>
     </row>
@@ -4053,18 +4356,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D16" s="72"/>
+      <c r="D16" s="55"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="72"/>
+      <c r="I16" s="55"/>
       <c r="J16" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -4078,11 +4384,14 @@
         <v>0</v>
       </c>
       <c r="K16" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -4107,7 +4416,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -4216,18 +4525,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D17" s="72"/>
+      <c r="D17" s="55"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="72"/>
+      <c r="I17" s="55"/>
       <c r="J17" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -4241,11 +4553,14 @@
         <v>0</v>
       </c>
       <c r="K17" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -4270,7 +4585,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -4379,18 +4694,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D18" s="72"/>
+      <c r="D18" s="55"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="72"/>
+      <c r="I18" s="55"/>
       <c r="J18" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -4404,11 +4722,14 @@
         <v>0</v>
       </c>
       <c r="K18" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -4433,7 +4754,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -4542,18 +4863,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D19" s="72"/>
+      <c r="D19" s="55"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="72"/>
+      <c r="I19" s="55"/>
       <c r="J19" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -4567,11 +4891,14 @@
         <v>0</v>
       </c>
       <c r="K19" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -4596,7 +4923,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -4705,18 +5032,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D20" s="72"/>
+      <c r="D20" s="55"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="72"/>
+      <c r="I20" s="55"/>
       <c r="J20" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -4730,11 +5060,14 @@
         <v>0</v>
       </c>
       <c r="K20" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -4759,7 +5092,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -4868,18 +5201,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D21" s="72"/>
+      <c r="D21" s="55"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-      <c r="I21" s="72"/>
+      <c r="I21" s="55"/>
       <c r="J21" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -4893,11 +5229,14 @@
         <v>0</v>
       </c>
       <c r="K21" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -4922,7 +5261,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -5031,18 +5370,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D22" s="72"/>
+      <c r="D22" s="55"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-      <c r="I22" s="72"/>
+      <c r="I22" s="55"/>
       <c r="J22" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -5056,11 +5398,14 @@
         <v>0</v>
       </c>
       <c r="K22" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -5085,7 +5430,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -5194,18 +5539,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D23" s="72"/>
+      <c r="D23" s="55"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="72"/>
+      <c r="I23" s="55"/>
       <c r="J23" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -5219,11 +5567,14 @@
         <v>0</v>
       </c>
       <c r="K23" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -5248,7 +5599,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -5357,18 +5708,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D24" s="72"/>
+      <c r="D24" s="55"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-      <c r="I24" s="72"/>
+      <c r="I24" s="55"/>
       <c r="J24" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -5382,11 +5736,14 @@
         <v>0</v>
       </c>
       <c r="K24" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -5411,7 +5768,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -5520,18 +5877,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D25" s="72"/>
+      <c r="D25" s="55"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="I25" s="72"/>
+      <c r="I25" s="55"/>
       <c r="J25" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -5545,11 +5905,14 @@
         <v>0</v>
       </c>
       <c r="K25" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -5574,7 +5937,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -5683,18 +6046,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D26" s="72"/>
+      <c r="D26" s="55"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
-      <c r="I26" s="72"/>
+      <c r="I26" s="55"/>
       <c r="J26" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -5708,11 +6074,14 @@
         <v>0</v>
       </c>
       <c r="K26" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -5737,7 +6106,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -5846,18 +6215,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D27" s="72"/>
+      <c r="D27" s="55"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
-      <c r="I27" s="72"/>
+      <c r="I27" s="55"/>
       <c r="J27" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -5871,11 +6243,14 @@
         <v>0</v>
       </c>
       <c r="K27" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -5900,7 +6275,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -6009,18 +6384,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D28" s="72"/>
+      <c r="D28" s="55"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-      <c r="I28" s="72"/>
+      <c r="I28" s="55"/>
       <c r="J28" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -6034,11 +6412,14 @@
         <v>0</v>
       </c>
       <c r="K28" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -6063,7 +6444,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -6172,18 +6553,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D29" s="72"/>
+      <c r="D29" s="55"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
-      <c r="I29" s="72"/>
+      <c r="I29" s="55"/>
       <c r="J29" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -6197,11 +6581,14 @@
         <v>0</v>
       </c>
       <c r="K29" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -6226,7 +6613,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -6335,18 +6722,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D30" s="72"/>
+      <c r="D30" s="55"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
-      <c r="I30" s="72"/>
+      <c r="I30" s="55"/>
       <c r="J30" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -6360,11 +6750,14 @@
         <v>0</v>
       </c>
       <c r="K30" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -6389,7 +6782,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -6498,18 +6891,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D31" s="72"/>
+      <c r="D31" s="55"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
-      <c r="I31" s="72"/>
+      <c r="I31" s="55"/>
       <c r="J31" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -6523,11 +6919,14 @@
         <v>0</v>
       </c>
       <c r="K31" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -6552,7 +6951,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -6661,18 +7060,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D32" s="72"/>
+      <c r="D32" s="55"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
-      <c r="I32" s="72"/>
+      <c r="I32" s="55"/>
       <c r="J32" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -6686,11 +7088,14 @@
         <v>0</v>
       </c>
       <c r="K32" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -6715,7 +7120,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -6824,18 +7229,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D33" s="72"/>
+      <c r="D33" s="55"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
-      <c r="I33" s="72"/>
+      <c r="I33" s="55"/>
       <c r="J33" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -6849,11 +7257,14 @@
         <v>0</v>
       </c>
       <c r="K33" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -6878,7 +7289,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -6987,18 +7398,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D34" s="72"/>
+      <c r="D34" s="55"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
-      <c r="I34" s="72"/>
+      <c r="I34" s="55"/>
       <c r="J34" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -7012,11 +7426,14 @@
         <v>0</v>
       </c>
       <c r="K34" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -7041,7 +7458,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -7150,18 +7567,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D35" s="72"/>
+      <c r="D35" s="55"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
-      <c r="I35" s="72"/>
+      <c r="I35" s="55"/>
       <c r="J35" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -7175,11 +7595,14 @@
         <v>0</v>
       </c>
       <c r="K35" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -7204,7 +7627,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -7313,18 +7736,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D36" s="72"/>
+      <c r="D36" s="55"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
-      <c r="I36" s="72"/>
+      <c r="I36" s="55"/>
       <c r="J36" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -7338,11 +7764,14 @@
         <v>0</v>
       </c>
       <c r="K36" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -7367,7 +7796,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -7476,18 +7905,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D37" s="72"/>
+      <c r="D37" s="55"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
-      <c r="I37" s="72"/>
+      <c r="I37" s="55"/>
       <c r="J37" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -7501,11 +7933,14 @@
         <v>0</v>
       </c>
       <c r="K37" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -7530,7 +7965,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -7639,18 +8074,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D38" s="72"/>
+      <c r="D38" s="55"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
-      <c r="I38" s="72"/>
+      <c r="I38" s="55"/>
       <c r="J38" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -7664,11 +8102,14 @@
         <v>0</v>
       </c>
       <c r="K38" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -7693,7 +8134,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -7802,18 +8243,21 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D39" s="72"/>
+      <c r="D39" s="55"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
-      <c r="I39" s="72"/>
+      <c r="I39" s="55"/>
       <c r="J39" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_1&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 1 (Almoço)]),ISNUMBER(tblHoras[Entrada - 1])),
               IF(OR(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -7827,11 +8271,14 @@
         <v>0</v>
       </c>
       <c r="K39" s="4">
-        <f>IF($B$6&lt;&gt;"",IF(AND(tblHoras[Evento 
+        <f>IF($B$6&lt;&gt;"",
+IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)),FALSE,VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$D$1,FALSE)="Sim")),
-        JORNADA/2,
+        IF(JORNADA_PERIODO_2&lt;&gt;"",
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),
+IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA/2)),
         IF(AND(ISNUMBER(tblHoras[Saída - 2]),ISNUMBER(tblHoras[Entrada - 2 (Almoço)])),
               IF(OR(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -7856,7 +8303,7 @@
 (1º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE),IF(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
-              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Jornada Diferenciada?]],3,FALSE),JORNADA),
+              IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&gt;0,VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA),
               ""),
          "")</f>
         <v/>
@@ -7982,7 +8429,7 @@
     <row r="46" spans="2:25" x14ac:dyDescent="0.25"/>
     <row r="47" spans="2:25" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="g+BR4CBRf3bhgxyB9ax6zrXmtiNmb/Uvh/3gU32lkGvl3+ZXgKtceCtWizZ9WUgUP5GgkMWtQYrTBLqw2ELTZg==" saltValue="ndc5HYslQsI1wlkfwYIsVQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" selectLockedCells="1" autoFilter="0" pivotTables="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="OOVCGaV0KvgMtSubE9+IxtCvpWHDxM1nF/FFfZQC6EK7aVhssExT1uDR7c3jvHiTwH0/pgXbt1pPAPaPR3GWtA==" saltValue="3RvzvNj7lxdnD5M1Jj4JHQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" selectLockedCells="1" autoFilter="0" pivotTables="0"/>
   <dataConsolidate/>
   <mergeCells count="7">
     <mergeCell ref="O1:X4"/>
@@ -8028,7 +8475,7 @@
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="20" id="{33616478-990B-44FE-BB07-40117DF3ADA1}">
-            <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C9,Config!$C$1:$D$17,2,FALSE)),FALSE,IF(VLOOKUP($C9,Config!$C$1:$D$17,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D9,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D9,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I9,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I9,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
+            <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)),FALSE,IF(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -8037,7 +8484,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B9:X9</xm:sqref>
+          <xm:sqref>B9:X9 S7 V7 J10:X39</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="17" id="{D79C2469-95B2-4490-A707-5C27A171E816}">
@@ -8050,7 +8497,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>J9 D9:F9</xm:sqref>
+          <xm:sqref>D9:F9 J9:J39</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="23" id="{31CF979C-12F0-4F54-B477-D65B5CC060E6}">
@@ -8063,11 +8510,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>K9:M9 G9:I9</xm:sqref>
+          <xm:sqref>K9:M9 G9:I9 K10:K39</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="13" id="{CF3EF681-ADA3-454F-BD4D-136E8407E816}">
-            <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C7,Config!$C$1:$D$17,2,FALSE)),FALSE,IF(VLOOKUP($C7,Config!$C$1:$D$17,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
+            <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)),FALSE,IF(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -8076,11 +8523,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>Q7 S7 V7</xm:sqref>
+          <xm:sqref>Q7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="8" id="{9015B1FB-D320-45D4-903E-B40FCBE5CA69}">
-            <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C10,Config!$C$1:$D$17,2,FALSE)),FALSE,IF(VLOOKUP($C10,Config!$C$1:$D$17,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D10,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D10,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I10,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I10,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
+            <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C10,Config!$C$1:$D$18,2,FALSE)),FALSE,IF(VLOOKUP($C10,Config!$C$1:$D$18,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D10,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D10,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I10,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I10,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -8089,7 +8536,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B10:X39</xm:sqref>
+          <xm:sqref>B10:I39</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="7" id="{956628B0-9BEE-401E-B2E2-0213C7CEE5C0}">
@@ -8102,7 +8549,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>J10:J39 D10:F39</xm:sqref>
+          <xm:sqref>D10:F39</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="9" id="{37400795-195C-4039-B9AA-275DE3D968EE}">
@@ -8115,11 +8562,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>K10:M39 G10:I39</xm:sqref>
+          <xm:sqref>L10:M39 G10:I39</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="6" id="{6833BDA1-C45D-4AD2-B5F4-CA013523FCA7}">
-            <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C7,Config!$C$1:$D$17,2,FALSE)),FALSE,IF(VLOOKUP($C7,Config!$C$1:$D$17,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
+            <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)),FALSE,IF(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -8132,7 +8579,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="5" id="{ED503053-E09B-4D43-A8D9-9598E4076ED6}">
-            <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C7,Config!$C$1:$D$17,2,FALSE)),FALSE,IF(VLOOKUP($C7,Config!$C$1:$D$17,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
+            <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)),FALSE,IF(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -8145,7 +8592,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="3" id="{C09E7684-AED8-438C-B68E-2E7738ECC073}">
-            <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C7,Config!$C$1:$D$17,2,FALSE)),FALSE,IF(VLOOKUP($C7,Config!$C$1:$D$17,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
+            <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)),FALSE,IF(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -8158,7 +8605,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="2" id="{BD039133-8410-430E-A4D9-B20483016ECF}">
-            <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C7,Config!$C$1:$D$17,2,FALSE)),FALSE,IF(VLOOKUP($C7,Config!$C$1:$D$17,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
+            <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)),FALSE,IF(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -8171,7 +8618,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="1" id="{18861696-7153-4870-9908-43C72D087D0E}">
-            <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C7,Config!$C$1:$D$17,2,FALSE)),FALSE,IF(VLOOKUP($C7,Config!$C$1:$D$17,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
+            <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)),FALSE,IF(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>

</xml_diff>

<commit_message>
Correção no saldo de horas para eventos com desconto
</commit_message>
<xml_diff>
--- a/Controle de Ponto.xlsx
+++ b/Controle de Ponto.xlsx
@@ -20,8 +20,8 @@
   <definedNames>
     <definedName name="CARENCIA">Config!$D$5</definedName>
     <definedName name="JORNADA">Config!$D$7</definedName>
-    <definedName name="JORNADA_PERIODO_1">Config!$D$22</definedName>
-    <definedName name="JORNADA_PERIODO_2">Config!$D$23</definedName>
+    <definedName name="JORNADA_PERIODO_1">Config!$D$23</definedName>
+    <definedName name="JORNADA_PERIODO_2">Config!$D$24</definedName>
     <definedName name="LIMITE">Config!$D$3</definedName>
     <definedName name="lst_Mes">tbl_Mes[Mês]</definedName>
     <definedName name="lstEvento">tblEvento[Evento]</definedName>
@@ -1018,7 +1018,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1058,6 +1057,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1128,8 +1130,8 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1138,35 +1140,101 @@
   </cellStyles>
   <dxfs count="67">
     <dxf>
-      <numFmt numFmtId="166" formatCode="h:mm;@"/>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="h:mm;@"/>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="h:mm;@"/>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD5D6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD1D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD5D6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD1D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="[h]:mm"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
     </dxf>
@@ -1257,7 +1325,35 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="[h]:mm"/>
+      <numFmt numFmtId="166" formatCode="h:mm;@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="h:mm;@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="h:mm;@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
     </dxf>
@@ -1331,90 +1427,6 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD5D6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD1D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD5D6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD1D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1516,16 +1528,6 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1683,14 +1685,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tblDiaUtil" displayName="tblDiaUtil" ref="B11:G18" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tblDiaUtil" displayName="tblDiaUtil" ref="B11:G18" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
   <tableColumns count="6">
-    <tableColumn id="1" name="Dia da Semana" dataDxfId="47"/>
-    <tableColumn id="4" name="Abreviatura" dataDxfId="46"/>
-    <tableColumn id="2" name="É dia util?" dataDxfId="45"/>
-    <tableColumn id="3" name="1º Período" dataDxfId="44"/>
-    <tableColumn id="5" name="2º Período" dataDxfId="43"/>
-    <tableColumn id="6" name="Total Jornada" dataDxfId="42">
+    <tableColumn id="1" name="Dia da Semana" dataDxfId="48"/>
+    <tableColumn id="4" name="Abreviatura" dataDxfId="47"/>
+    <tableColumn id="2" name="É dia util?" dataDxfId="46"/>
+    <tableColumn id="3" name="1º Período" dataDxfId="45"/>
+    <tableColumn id="5" name="2º Período" dataDxfId="44"/>
+    <tableColumn id="6" name="Total Jornada" dataDxfId="43">
       <calculatedColumnFormula>IF((tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]])&gt;0,tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]],"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1699,32 +1701,32 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="tblDiaUtil7" displayName="tblDiaUtil7" ref="B21:D23" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="tblDiaUtil7" displayName="tblDiaUtil7" ref="B22:D24" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <tableColumns count="3">
-    <tableColumn id="1" name="Período" dataDxfId="39"/>
-    <tableColumn id="4" name="Abreviatura" dataDxfId="38"/>
-    <tableColumn id="2" name="Qtd. Horas por Jornada" dataDxfId="37"/>
+    <tableColumn id="1" name="Período" dataDxfId="40"/>
+    <tableColumn id="4" name="Abreviatura" dataDxfId="39"/>
+    <tableColumn id="2" name="Qtd. Horas por Jornada" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblHoras" displayName="tblHoras" ref="B8:X39" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblHoras" displayName="tblHoras" ref="B8:X39" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
   <tableColumns count="23">
-    <tableColumn id="1" name="Data" dataDxfId="22">
+    <tableColumn id="1" name="Data" dataDxfId="35">
       <calculatedColumnFormula>IF(B8&lt;&gt;"",IF(DAY(B8+1)=1,"",B8+1),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Dia" dataDxfId="21">
+    <tableColumn id="2" name="Dia" dataDxfId="34">
       <calculatedColumnFormula>TEXT(tblHoras[[#This Row],[Data]],"ddd")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Evento _x000a_(1º Período)" dataDxfId="20"/>
-    <tableColumn id="4" name="Entrada - 1" dataDxfId="19"/>
-    <tableColumn id="5" name="Saída - 1 (Almoço)" dataDxfId="18"/>
-    <tableColumn id="6" name="Entrada - 2 (Almoço)" dataDxfId="17"/>
-    <tableColumn id="7" name="Saída - 2" dataDxfId="16"/>
-    <tableColumn id="13" name="Evento _x000a_(2º Período)" dataDxfId="15"/>
-    <tableColumn id="15" name="Horas Trabalhadas (1º Período)" dataDxfId="1">
+    <tableColumn id="3" name="Evento _x000a_(1º Período)" dataDxfId="33"/>
+    <tableColumn id="4" name="Entrada - 1" dataDxfId="32"/>
+    <tableColumn id="5" name="Saída - 1 (Almoço)" dataDxfId="31"/>
+    <tableColumn id="6" name="Entrada - 2 (Almoço)" dataDxfId="30"/>
+    <tableColumn id="7" name="Saída - 2" dataDxfId="29"/>
+    <tableColumn id="13" name="Evento _x000a_(2º Período)" dataDxfId="28"/>
+    <tableColumn id="15" name="Horas Trabalhadas (1º Período)" dataDxfId="27">
       <calculatedColumnFormula>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -1744,7 +1746,7 @@
                           0)),
                     0)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Horas Trabalhadas (2º Período)" dataDxfId="0">
+    <tableColumn id="16" name="Horas Trabalhadas (2º Período)" dataDxfId="26">
       <calculatedColumnFormula>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -1764,10 +1766,10 @@
                          0)),
        0)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Horas Trabalhadas" dataDxfId="14">
+    <tableColumn id="8" name="Horas Trabalhadas" dataDxfId="25">
       <calculatedColumnFormula>tblHoras[[#This Row],[Horas Trabalhadas (1º Período)]]+tblHoras[[#This Row],[Horas Trabalhadas (2º Período)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Jornada Diária" dataDxfId="2">
+    <tableColumn id="17" name="Jornada Diária" dataDxfId="24">
       <calculatedColumnFormula>IF(tblHoras[Data]&lt;&gt;"",
         IF(
 AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
@@ -1780,29 +1782,34 @@
          "")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" name="Horas Trabalhadas Além Jornada" dataDxfId="13">
-      <calculatedColumnFormula>IF(OR(tblHoras[[#This Row],[Horas Trabalhadas (1º Período)]]&lt;&gt;0,tblHoras[[#This Row],[Horas Trabalhadas (2º Período)]]&lt;&gt;0),
-        IF(ISNUMBER(tblHoras[[#This Row],[Jornada Diária]]),
-              IF(tblHoras[[#This Row],[Jornada Diária]]&gt;(tblHoras[[#This Row],[Horas Trabalhadas (2º Período)]]+tblHoras[[#This Row],[Horas Trabalhadas (1º Período)]]),
-                     IF(ROUND((tblHoras[[#This Row],[Jornada Diária]]-(tblHoras[[#This Row],[Horas Trabalhadas (2º Período)]]+tblHoras[[#This Row],[Horas Trabalhadas (1º Período)]])),6)&gt;ROUND(CARENCIA,6),
-                           -tblHoras[[#This Row],[Jornada Diária]]+(tblHoras[[#This Row],[Horas Trabalhadas (2º Período)]]+tblHoras[[#This Row],[Horas Trabalhadas (1º Período)]]),
+      <calculatedColumnFormula>IF(OR(tblHoras[Horas Trabalhadas (1º Período)]&lt;&gt;0,tblHoras[Horas Trabalhadas (2º Período)]&lt;&gt;0),
+        IF(ISNUMBER(tblHoras[Jornada Diária]),
+              IF(tblHoras[Jornada Diária]&gt;(tblHoras[Horas Trabalhadas (2º Período)]+tblHoras[Horas Trabalhadas (1º Período)]),
+                     IF(ROUND((tblHoras[Jornada Diária]-(tblHoras[Horas Trabalhadas (2º Período)]+tblHoras[Horas Trabalhadas (1º Período)])),6)&gt;ROUND(CARENCIA,6),
+                           -tblHoras[Jornada Diária]+(tblHoras[Horas Trabalhadas (2º Período)]+tblHoras[Horas Trabalhadas (1º Período)]),
                            0),
-                      IF(ROUND((tblHoras[[#This Row],[Jornada Diária]]-(tblHoras[[#This Row],[Horas Trabalhadas (2º Período)]]+tblHoras[[#This Row],[Horas Trabalhadas (1º Período)]])),6)&lt;ROUND(-CARENCIA,6),
-                           -tblHoras[[#This Row],[Jornada Diária]]+(tblHoras[[#This Row],[Horas Trabalhadas (2º Período)]]+tblHoras[[#This Row],[Horas Trabalhadas (1º Período)]]),
+                      IF(ROUND((tblHoras[Jornada Diária]-(tblHoras[Horas Trabalhadas (2º Período)]+tblHoras[Horas Trabalhadas (1º Período)])),6)&lt;ROUND(-CARENCIA,6),
+                           -tblHoras[Jornada Diária]+(tblHoras[Horas Trabalhadas (2º Período)]+tblHoras[Horas Trabalhadas (1º Período)]),
                            0)),
-              tblHoras[[#This Row],[Horas Trabalhadas (2º Período)]]+tblHoras[[#This Row],[Horas Trabalhadas (1º Período)]]),
-         IF(AND(IF(ISERROR(VLOOKUP(tblHoras[[#This Row],[Evento 
-(1º Período)]],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[[#This Row],[Evento 
-(1º Período)]],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[[#This Row],[Evento 
-(2º Período)]],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[[#This Row],[Evento 
-(2º Período)]],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[[#This Row],[Evento 
-(1º Período)]],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[[#This Row],[Evento 
-(1º Período)]],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[[#This Row],[Evento 
-(2º Período)]],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[[#This Row],[Evento 
-(2º Período)]],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</calculatedColumnFormula>
+              tblHoras[Horas Trabalhadas (2º Período)]+tblHoras[Horas Trabalhadas (1º Período)]),
+         IF(AND(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Saldo de Horas" dataDxfId="12">
+    <tableColumn id="18" name="Saldo de Horas" dataDxfId="23">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&gt;0,
         IF(tblHoras[[#This Row],[Jornada Diária]]&lt;&gt;"",
               IF(HOUR(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]])&gt;=VLOOKUP(LIMITE,tblLimiteHora[],Tabelas!$I$1,FALSE),
@@ -1811,23 +1818,23 @@
               tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]),
         0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="Saldo de Horas (Decimal)" dataDxfId="11">
+    <tableColumn id="20" name="Saldo de Horas (Decimal)" dataDxfId="22">
       <calculatedColumnFormula>tblHoras[[#This Row],[Saldo de Horas]]*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="Atrasos_x000a_(horas)" dataDxfId="10">
+    <tableColumn id="19" name="Atrasos_x000a_(horas)" dataDxfId="21">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&lt;0,IF(OR(tblHoras[[#This Row],[Evento 
 (1º Período)]]="",tblHoras[[#This Row],[Evento 
 (2º Período)]]=""),tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]],""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Atrasos (Decimal)" dataDxfId="9">
+    <tableColumn id="21" name="Atrasos (Decimal)" dataDxfId="20">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Faltas_x000a_(dias)" dataDxfId="8">
+    <tableColumn id="14" name="Faltas_x000a_(dias)" dataDxfId="19">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Jornada Diária]]&lt;&gt;"",IF((N(tblHoras[[#This Row],[Jornada Diária]])-ABS(N(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]])))=0,1,""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Hora Extra Normal" dataDxfId="7">
+    <tableColumn id="10" name="Hora Extra Normal" dataDxfId="18">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[[#This Row],[Data]],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[[#This Row],[Evento 
 (1º Período)]]&lt;&gt;"",IF(VLOOKUP(tblHoras[[#This Row],[Evento 
@@ -1836,10 +1843,10 @@
 (2º Período)]],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
 tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]],""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="Hora Extra Normal (Decimal)" dataDxfId="6">
+    <tableColumn id="22" name="Hora Extra Normal (Decimal)" dataDxfId="17">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Hora Extra _x000a_Especial" dataDxfId="5">
+    <tableColumn id="9" name="Hora Extra _x000a_Especial" dataDxfId="16">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[[#This Row],[Data]],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[[#This Row],[Evento 
 (1º Período)]]&lt;&gt;"",IF(VLOOKUP(tblHoras[[#This Row],[Evento 
@@ -1848,12 +1855,12 @@
 (2º Período)]],tblEvento[],Tabelas!$E$1,FALSE)="Sim",TRUE,FALSE),FALSE)),
 tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]],""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="Hora Extra Especial (Decimal)" dataDxfId="4">
+    <tableColumn id="23" name="Hora Extra Especial (Decimal)" dataDxfId="15">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Informação" dataDxfId="3">
+    <tableColumn id="12" name="Informação" dataDxfId="14">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Evento 
 (1º Período)]]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[[#This Row],[Evento 
 (1º Período)]],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[[#This Row],[Evento 
@@ -2496,10 +2503,10 @@
   <sheetPr codeName="plnConfig">
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B1:H28"/>
+  <dimension ref="B1:G29"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2560,9 +2567,9 @@
       <c r="G9" s="68"/>
     </row>
     <row r="10" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
       <c r="E10" s="70" t="s">
         <v>77</v>
       </c>
@@ -2579,13 +2586,13 @@
       <c r="D11" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="57" t="s">
+      <c r="E11" s="56" t="s">
         <v>109</v>
       </c>
-      <c r="F11" s="55" t="s">
+      <c r="F11" s="54" t="s">
         <v>110</v>
       </c>
-      <c r="G11" s="58" t="s">
+      <c r="G11" s="57" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2599,9 +2606,9 @@
       <c r="D12" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="59"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="60" t="str">
+      <c r="E12" s="58"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="59" t="str">
         <f>IF((tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]])&gt;0,tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]],"")</f>
         <v/>
       </c>
@@ -2616,9 +2623,9 @@
       <c r="D13" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="59"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="60" t="str">
+      <c r="E13" s="58"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="59" t="str">
         <f>IF((tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]])&gt;0,tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]],"")</f>
         <v/>
       </c>
@@ -2633,9 +2640,9 @@
       <c r="D14" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="59"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="60" t="str">
+      <c r="E14" s="58"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="59" t="str">
         <f>IF((tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]])&gt;0,tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]],"")</f>
         <v/>
       </c>
@@ -2650,9 +2657,9 @@
       <c r="D15" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="59"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="60" t="str">
+      <c r="E15" s="58"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="59" t="str">
         <f>IF((tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]])&gt;0,tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]],"")</f>
         <v/>
       </c>
@@ -2667,14 +2674,14 @@
       <c r="D16" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="59"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="60" t="str">
+      <c r="E16" s="58"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="59" t="str">
         <f>IF((tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]])&gt;0,tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]],"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="21" t="s">
         <v>39</v>
       </c>
@@ -2684,14 +2691,14 @@
       <c r="D17" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="59"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="60" t="str">
+      <c r="E17" s="58"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="59" t="str">
         <f>IF((tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]])&gt;0,tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]],"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="21" t="s">
         <v>40</v>
       </c>
@@ -2701,118 +2708,120 @@
       <c r="D18" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="61"/>
-      <c r="F18" s="62"/>
-      <c r="G18" s="63" t="str">
+      <c r="E18" s="60"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="62" t="str">
         <f>IF((tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]])&gt;0,tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]],"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="67" t="s">
+    <row r="19" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="85" t="str">
+        <f>IF(G21=0,"A quantidade de horas por período deve ser igual à jornada diária","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="68"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="50" t="s">
+      <c r="C21" s="68"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="F20" s="49">
+      <c r="F21" s="49">
         <f>SUM(tblDiaUtil7[Qtd. Horas por Jornada])</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="G20" s="5">
-        <f>IF(F20&gt;0,IF(F20=JORNADA,1,0),"")</f>
+      <c r="G21" s="5">
+        <f>IF(F21&gt;0,IF(F21=JORNADA,1,0),"")</f>
         <v>1</v>
       </c>
-      <c r="H20" s="51" t="str">
-        <f>IF(G20=0,"A quantidade de horas por período deve ser igual à jornada diária","")</f>
-        <v/>
-      </c>
     </row>
-    <row r="21" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="9" t="s">
+    <row r="22" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C22" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D22" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="E21" s="9"/>
+      <c r="E22" s="9"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="21" t="s">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C23" s="21" t="s">
         <v>78</v>
-      </c>
-      <c r="D22" s="48">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="E22" s="85"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="C23" s="21" t="s">
-        <v>79</v>
       </c>
       <c r="D23" s="48">
         <v>0.16666666666666666</v>
       </c>
-      <c r="E23" s="85"/>
+      <c r="E23" s="63"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="21"/>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="21" t="s">
+        <v>105</v>
+      </c>
       <c r="C24" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="48">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E24" s="63"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="21"/>
+      <c r="C25" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="21"/>
-      <c r="E24" s="85"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="63"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="85"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="21"/>
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
-      <c r="E26" s="85"/>
+      <c r="E26" s="63"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
       <c r="D27" s="21"/>
-      <c r="E27" s="85"/>
+      <c r="E27" s="63"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="21"/>
       <c r="C28" s="21"/>
       <c r="D28" s="21"/>
-      <c r="E28" s="85"/>
+      <c r="E28" s="63"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="63"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="DV6P2w6S2Px8igwAks4XwyWALpetOIoer10E/w9JExO7VL9FVk2lNyuSjtXj5rOIgeD7r6A1Ix8EJJEZkR1Zsg==" saltValue="jeleglo0aEbh6c+KM2KWVQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0" pivotTables="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="/HBlOI4uQUqg/9nO7C/ktqXANaFpWNQ4VHt3dQbJIUn/YEPsTgXS4RWZdvTE+ovsirrBGMNAfKTU50a6Iz9CNQ==" saltValue="mRnOdzsIZTNBzc/JMi0l4A==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" selectLockedCells="1" autoFilter="0" pivotTables="0"/>
   <mergeCells count="4">
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="E10:G10"/>
   </mergeCells>
   <conditionalFormatting sqref="D7">
-    <cfRule type="timePeriod" dxfId="50" priority="4" timePeriod="lastMonth">
+    <cfRule type="timePeriod" dxfId="12" priority="4" timePeriod="lastMonth">
       <formula>AND(MONTH(D7)=MONTH(EDATE(TODAY(),0-1)),YEAR(D7)=YEAR(EDATE(TODAY(),0-1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G20">
+  <conditionalFormatting sqref="G21">
     <cfRule type="iconSet" priority="1">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -2828,7 +2837,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12:D18">
       <formula1>"Sim,Não"</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7 D5 D22:D23 F20">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7 D5 D23:D24 F21">
       <formula1>0</formula1>
       <formula2>0.999305555555556</formula2>
     </dataValidation>
@@ -2946,7 +2955,7 @@
     </row>
     <row r="4" spans="2:29" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6"/>
-      <c r="G4" s="53"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="74"/>
       <c r="I4" s="75"/>
       <c r="N4" s="24"/>
@@ -3162,12 +3171,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D9" s="54"/>
+      <c r="D9" s="53"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="54"/>
+      <c r="I9" s="53"/>
       <c r="J9" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -3242,13 +3251,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-tblHoras[[#This Row],[Jornada Diária]], IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-tblHoras[[#This Row],[Jornada Diária]]/2,0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O9" s="14">
@@ -3333,12 +3347,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D10" s="54"/>
+      <c r="D10" s="53"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="54"/>
+      <c r="I10" s="53"/>
       <c r="J10" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -3413,13 +3427,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O10" s="14">
@@ -3503,12 +3522,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D11" s="54"/>
+      <c r="D11" s="53"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="54"/>
+      <c r="I11" s="53"/>
       <c r="J11" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -3583,13 +3602,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O11" s="14">
@@ -3672,12 +3696,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D12" s="54"/>
+      <c r="D12" s="53"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="54"/>
+      <c r="I12" s="53"/>
       <c r="J12" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -3752,13 +3776,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O12" s="14">
@@ -3841,12 +3870,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D13" s="54"/>
+      <c r="D13" s="53"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="54"/>
+      <c r="I13" s="53"/>
       <c r="J13" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -3921,13 +3950,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O13" s="14">
@@ -4010,12 +4044,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D14" s="54"/>
+      <c r="D14" s="53"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="54"/>
+      <c r="I14" s="53"/>
       <c r="J14" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -4090,13 +4124,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O14" s="14">
@@ -4181,12 +4220,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D15" s="54"/>
+      <c r="D15" s="53"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="54"/>
+      <c r="I15" s="53"/>
       <c r="J15" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -4261,13 +4300,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O15" s="14">
@@ -4351,12 +4395,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D16" s="54"/>
+      <c r="D16" s="53"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="54"/>
+      <c r="I16" s="53"/>
       <c r="J16" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -4431,13 +4475,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O16" s="14">
@@ -4520,12 +4569,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D17" s="54"/>
+      <c r="D17" s="53"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="54"/>
+      <c r="I17" s="53"/>
       <c r="J17" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -4600,13 +4649,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O17" s="14">
@@ -4689,12 +4743,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D18" s="54"/>
+      <c r="D18" s="53"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="54"/>
+      <c r="I18" s="53"/>
       <c r="J18" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -4769,13 +4823,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O18" s="14">
@@ -4858,12 +4917,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D19" s="54"/>
+      <c r="D19" s="53"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="54"/>
+      <c r="I19" s="53"/>
       <c r="J19" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -4938,13 +4997,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O19" s="14">
@@ -5027,12 +5091,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D20" s="54"/>
+      <c r="D20" s="53"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="54"/>
+      <c r="I20" s="53"/>
       <c r="J20" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -5107,13 +5171,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O20" s="14">
@@ -5196,12 +5265,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D21" s="54"/>
+      <c r="D21" s="53"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-      <c r="I21" s="54"/>
+      <c r="I21" s="53"/>
       <c r="J21" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -5276,13 +5345,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O21" s="14">
@@ -5365,12 +5439,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D22" s="54"/>
+      <c r="D22" s="53"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-      <c r="I22" s="54"/>
+      <c r="I22" s="53"/>
       <c r="J22" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -5445,13 +5519,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O22" s="14">
@@ -5534,12 +5613,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D23" s="54"/>
+      <c r="D23" s="53"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="54"/>
+      <c r="I23" s="53"/>
       <c r="J23" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -5614,13 +5693,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O23" s="14">
@@ -5703,12 +5787,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D24" s="54"/>
+      <c r="D24" s="53"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-      <c r="I24" s="54"/>
+      <c r="I24" s="53"/>
       <c r="J24" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -5783,13 +5867,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O24" s="14">
@@ -5872,12 +5961,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D25" s="54"/>
+      <c r="D25" s="53"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="I25" s="54"/>
+      <c r="I25" s="53"/>
       <c r="J25" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -5952,13 +6041,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O25" s="14">
@@ -6041,12 +6135,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D26" s="54"/>
+      <c r="D26" s="53"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
-      <c r="I26" s="54"/>
+      <c r="I26" s="53"/>
       <c r="J26" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -6121,13 +6215,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O26" s="14">
@@ -6210,12 +6309,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D27" s="54"/>
+      <c r="D27" s="53"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
-      <c r="I27" s="54"/>
+      <c r="I27" s="53"/>
       <c r="J27" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -6290,13 +6389,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O27" s="14">
@@ -6379,12 +6483,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D28" s="54"/>
+      <c r="D28" s="53"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-      <c r="I28" s="54"/>
+      <c r="I28" s="53"/>
       <c r="J28" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -6459,13 +6563,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O28" s="14">
@@ -6548,12 +6657,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D29" s="54"/>
+      <c r="D29" s="53"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
-      <c r="I29" s="54"/>
+      <c r="I29" s="53"/>
       <c r="J29" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -6628,13 +6737,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O29" s="14">
@@ -6717,12 +6831,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D30" s="54"/>
+      <c r="D30" s="53"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
-      <c r="I30" s="54"/>
+      <c r="I30" s="53"/>
       <c r="J30" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -6797,13 +6911,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O30" s="14">
@@ -6886,12 +7005,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D31" s="54"/>
+      <c r="D31" s="53"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
-      <c r="I31" s="54"/>
+      <c r="I31" s="53"/>
       <c r="J31" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -6966,13 +7085,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O31" s="14">
@@ -7055,12 +7179,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D32" s="54"/>
+      <c r="D32" s="53"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
-      <c r="I32" s="54"/>
+      <c r="I32" s="53"/>
       <c r="J32" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -7135,13 +7259,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O32" s="14">
@@ -7224,12 +7353,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D33" s="54"/>
+      <c r="D33" s="53"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
-      <c r="I33" s="54"/>
+      <c r="I33" s="53"/>
       <c r="J33" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -7304,13 +7433,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O33" s="14">
@@ -7393,12 +7527,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D34" s="54"/>
+      <c r="D34" s="53"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
-      <c r="I34" s="54"/>
+      <c r="I34" s="53"/>
       <c r="J34" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -7473,13 +7607,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O34" s="14">
@@ -7562,12 +7701,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D35" s="54"/>
+      <c r="D35" s="53"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
-      <c r="I35" s="54"/>
+      <c r="I35" s="53"/>
       <c r="J35" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -7642,13 +7781,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O35" s="14">
@@ -7731,12 +7875,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D36" s="54"/>
+      <c r="D36" s="53"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
-      <c r="I36" s="54"/>
+      <c r="I36" s="53"/>
       <c r="J36" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -7811,13 +7955,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O36" s="14">
@@ -7900,12 +8049,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D37" s="54"/>
+      <c r="D37" s="53"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
-      <c r="I37" s="54"/>
+      <c r="I37" s="53"/>
       <c r="J37" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -7980,13 +8129,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O37" s="14">
@@ -8069,12 +8223,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D38" s="54"/>
+      <c r="D38" s="53"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
-      <c r="I38" s="54"/>
+      <c r="I38" s="53"/>
       <c r="J38" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -8149,13 +8303,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O38" s="14">
@@ -8238,12 +8397,12 @@
         <f>TEXT(tblHoras[Data],"ddd")</f>
         <v/>
       </c>
-      <c r="D39" s="54"/>
+      <c r="D39" s="53"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
-      <c r="I39" s="54"/>
+      <c r="I39" s="53"/>
       <c r="J39" s="4">
         <f>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
@@ -8318,13 +8477,18 @@
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"8:00", IF(OR(
-IF(ISERROR(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[Total Jornada]],5,FALSE),JORNADA),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,
+IF(VLOOKUP(tblHoras[Evento 
+(1º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)
+),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[1º Período]],3,FALSE),JORNADA_PERIODO_1),
+IF(IF(ISERROR(VLOOKUP(tblHoras[Evento 
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)),FALSE,IF(VLOOKUP(tblHoras[Evento 
-(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE))),-"4:00",0
-)))</f>
+(2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
+-IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</f>
         <v>0</v>
       </c>
       <c r="O39" s="14">
@@ -8424,7 +8588,7 @@
     <row r="46" spans="2:25" x14ac:dyDescent="0.25"/>
     <row r="47" spans="2:25" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="AHxmuBj3/3b1LbTCw724C/woZxEGofRL9br3/lyEA9Tg7/8vuSuM7oDKItX5bYNqNp6ZhOrTM9sr8JJCWEyWMQ==" saltValue="94YOl7twiM5HMTR34JufiQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" selectLockedCells="1" autoFilter="0" pivotTables="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="bBIJ5VKH8eRPD0Nk6AoCBIAJy949a0nruGdg/IfyAUyli4uaivzHwMGe1yKt7zfjsf2LQtKJwt/uv3052sgG8A==" saltValue="8oOuV34fHmvfn2tlV7CO0Q==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" selectLockedCells="1" autoFilter="0" pivotTables="0"/>
   <dataConsolidate/>
   <mergeCells count="7">
     <mergeCell ref="O1:X4"/>
@@ -8435,7 +8599,7 @@
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="Q6:W6"/>
   </mergeCells>
-  <dataValidations count="5">
+  <dataValidations xWindow="263" yWindow="440" count="5">
     <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Aviso" error="Erro na inserção de dados:_x000a__x000a_'Hora Inválida'_x000a__x000a_Favor inserir uma hora válida no formato: hh:mm (ex. 12:00)" sqref="E9:H39">
       <formula1>0</formula1>
       <formula2>0.999305555555556</formula2>

</xml_diff>

<commit_message>
Correção cálulo de hora diferenciada na semana
</commit_message>
<xml_diff>
--- a/Controle de Ponto.xlsx
+++ b/Controle de Ponto.xlsx
@@ -1062,6 +1062,9 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1130,114 +1133,12 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="67">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD5D6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD1D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD5D6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD1D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="[h]:mm"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
     <dxf>
       <font>
         <i/>
@@ -1316,6 +1217,11 @@
           <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="[h]:mm"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
     </dxf>
@@ -1429,6 +1335,90 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD5D6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD1D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD5D6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD1D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -1528,6 +1518,16 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1685,14 +1685,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tblDiaUtil" displayName="tblDiaUtil" ref="B11:G18" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tblDiaUtil" displayName="tblDiaUtil" ref="B11:G18" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
   <tableColumns count="6">
-    <tableColumn id="1" name="Dia da Semana" dataDxfId="48"/>
-    <tableColumn id="4" name="Abreviatura" dataDxfId="47"/>
-    <tableColumn id="2" name="É dia util?" dataDxfId="46"/>
-    <tableColumn id="3" name="1º Período" dataDxfId="45"/>
-    <tableColumn id="5" name="2º Período" dataDxfId="44"/>
-    <tableColumn id="6" name="Total Jornada" dataDxfId="43">
+    <tableColumn id="1" name="Dia da Semana" dataDxfId="47"/>
+    <tableColumn id="4" name="Abreviatura" dataDxfId="46"/>
+    <tableColumn id="2" name="É dia util?" dataDxfId="45"/>
+    <tableColumn id="3" name="1º Período" dataDxfId="44"/>
+    <tableColumn id="5" name="2º Período" dataDxfId="43"/>
+    <tableColumn id="6" name="Total Jornada" dataDxfId="42">
       <calculatedColumnFormula>IF((tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]])&gt;0,tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]],"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1701,32 +1701,32 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="tblDiaUtil7" displayName="tblDiaUtil7" ref="B22:D24" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="tblDiaUtil7" displayName="tblDiaUtil7" ref="B22:D24" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <tableColumns count="3">
-    <tableColumn id="1" name="Período" dataDxfId="40"/>
-    <tableColumn id="4" name="Abreviatura" dataDxfId="39"/>
-    <tableColumn id="2" name="Qtd. Horas por Jornada" dataDxfId="38"/>
+    <tableColumn id="1" name="Período" dataDxfId="39"/>
+    <tableColumn id="4" name="Abreviatura" dataDxfId="38"/>
+    <tableColumn id="2" name="Qtd. Horas por Jornada" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblHoras" displayName="tblHoras" ref="B8:X39" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblHoras" displayName="tblHoras" ref="B8:X39" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <tableColumns count="23">
-    <tableColumn id="1" name="Data" dataDxfId="35">
+    <tableColumn id="1" name="Data" dataDxfId="22">
       <calculatedColumnFormula>IF(B8&lt;&gt;"",IF(DAY(B8+1)=1,"",B8+1),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Dia" dataDxfId="34">
+    <tableColumn id="2" name="Dia" dataDxfId="21">
       <calculatedColumnFormula>TEXT(tblHoras[[#This Row],[Data]],"ddd")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Evento _x000a_(1º Período)" dataDxfId="33"/>
-    <tableColumn id="4" name="Entrada - 1" dataDxfId="32"/>
-    <tableColumn id="5" name="Saída - 1 (Almoço)" dataDxfId="31"/>
-    <tableColumn id="6" name="Entrada - 2 (Almoço)" dataDxfId="30"/>
-    <tableColumn id="7" name="Saída - 2" dataDxfId="29"/>
-    <tableColumn id="13" name="Evento _x000a_(2º Período)" dataDxfId="28"/>
-    <tableColumn id="15" name="Horas Trabalhadas (1º Período)" dataDxfId="27">
+    <tableColumn id="3" name="Evento _x000a_(1º Período)" dataDxfId="20"/>
+    <tableColumn id="4" name="Entrada - 1" dataDxfId="19"/>
+    <tableColumn id="5" name="Saída - 1 (Almoço)" dataDxfId="18"/>
+    <tableColumn id="6" name="Entrada - 2 (Almoço)" dataDxfId="17"/>
+    <tableColumn id="7" name="Saída - 2" dataDxfId="16"/>
+    <tableColumn id="13" name="Evento _x000a_(2º Período)" dataDxfId="15"/>
+    <tableColumn id="15" name="Horas Trabalhadas (1º Período)" dataDxfId="14">
       <calculatedColumnFormula>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -1746,7 +1746,7 @@
                           0)),
                     0)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Horas Trabalhadas (2º Período)" dataDxfId="26">
+    <tableColumn id="16" name="Horas Trabalhadas (2º Período)" dataDxfId="13">
       <calculatedColumnFormula>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -1766,10 +1766,10 @@
                          0)),
        0)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Horas Trabalhadas" dataDxfId="25">
+    <tableColumn id="8" name="Horas Trabalhadas" dataDxfId="12">
       <calculatedColumnFormula>tblHoras[[#This Row],[Horas Trabalhadas (1º Período)]]+tblHoras[[#This Row],[Horas Trabalhadas (2º Período)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Jornada Diária" dataDxfId="24">
+    <tableColumn id="17" name="Jornada Diária" dataDxfId="11">
       <calculatedColumnFormula>IF(tblHoras[Data]&lt;&gt;"",
         IF(
 AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
@@ -1781,7 +1781,7 @@
               ""),
          "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Horas Trabalhadas Além Jornada" dataDxfId="13">
+    <tableColumn id="11" name="Horas Trabalhadas Além Jornada" dataDxfId="10">
       <calculatedColumnFormula>IF(OR(tblHoras[Horas Trabalhadas (1º Período)]&lt;&gt;0,tblHoras[Horas Trabalhadas (2º Período)]&lt;&gt;0),
         IF(ISNUMBER(tblHoras[Jornada Diária]),
               IF(tblHoras[Jornada Diária]&gt;(tblHoras[Horas Trabalhadas (2º Período)]+tblHoras[Horas Trabalhadas (1º Período)]),
@@ -1809,7 +1809,7 @@
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
 -IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Saldo de Horas" dataDxfId="23">
+    <tableColumn id="18" name="Saldo de Horas" dataDxfId="9">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&gt;0,
         IF(tblHoras[[#This Row],[Jornada Diária]]&lt;&gt;"",
               IF(HOUR(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]])&gt;=VLOOKUP(LIMITE,tblLimiteHora[],Tabelas!$I$1,FALSE),
@@ -1818,23 +1818,23 @@
               tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]),
         0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="Saldo de Horas (Decimal)" dataDxfId="22">
+    <tableColumn id="20" name="Saldo de Horas (Decimal)" dataDxfId="8">
       <calculatedColumnFormula>tblHoras[[#This Row],[Saldo de Horas]]*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="Atrasos_x000a_(horas)" dataDxfId="21">
+    <tableColumn id="19" name="Atrasos_x000a_(horas)" dataDxfId="7">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&lt;0,IF(OR(tblHoras[[#This Row],[Evento 
 (1º Período)]]="",tblHoras[[#This Row],[Evento 
 (2º Período)]]=""),tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]],""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Atrasos (Decimal)" dataDxfId="20">
+    <tableColumn id="21" name="Atrasos (Decimal)" dataDxfId="6">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Faltas_x000a_(dias)" dataDxfId="19">
+    <tableColumn id="14" name="Faltas_x000a_(dias)" dataDxfId="5">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Jornada Diária]]&lt;&gt;"",IF((N(tblHoras[[#This Row],[Jornada Diária]])-ABS(N(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]])))=0,1,""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Hora Extra Normal" dataDxfId="18">
+    <tableColumn id="10" name="Hora Extra Normal" dataDxfId="4">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[[#This Row],[Data]],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[[#This Row],[Evento 
 (1º Período)]]&lt;&gt;"",IF(VLOOKUP(tblHoras[[#This Row],[Evento 
@@ -1843,10 +1843,10 @@
 (2º Período)]],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
 tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]],""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="Hora Extra Normal (Decimal)" dataDxfId="17">
+    <tableColumn id="22" name="Hora Extra Normal (Decimal)" dataDxfId="3">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Hora Extra _x000a_Especial" dataDxfId="16">
+    <tableColumn id="9" name="Hora Extra _x000a_Especial" dataDxfId="2">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[[#This Row],[Data]],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[[#This Row],[Evento 
 (1º Período)]]&lt;&gt;"",IF(VLOOKUP(tblHoras[[#This Row],[Evento 
@@ -1855,12 +1855,12 @@
 (2º Período)]],tblEvento[],Tabelas!$E$1,FALSE)="Sim",TRUE,FALSE),FALSE)),
 tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]],""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="Hora Extra Especial (Decimal)" dataDxfId="15">
+    <tableColumn id="23" name="Hora Extra Especial (Decimal)" dataDxfId="1">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Informação" dataDxfId="14">
+    <tableColumn id="12" name="Informação" dataDxfId="0">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Evento 
 (1º Período)]]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[[#This Row],[Evento 
 (1º Período)]],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[[#This Row],[Evento 
@@ -2520,11 +2520,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="67"/>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="19" t="s">
@@ -2557,24 +2557,24 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="68"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="68"/>
-      <c r="G9" s="68"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
     </row>
     <row r="10" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
       <c r="D10" s="51"/>
-      <c r="E10" s="70" t="s">
+      <c r="E10" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="F10" s="71"/>
-      <c r="G10" s="72"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="73"/>
     </row>
     <row r="11" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
@@ -2717,17 +2717,17 @@
     </row>
     <row r="19" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="85" t="str">
+      <c r="B20" s="64" t="str">
         <f>IF(G21=0,"A quantidade de horas por período deve ser igual à jornada diária","")</f>
         <v/>
       </c>
     </row>
     <row r="21" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="67" t="s">
+      <c r="B21" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="68"/>
-      <c r="D21" s="69"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="70"/>
       <c r="E21" s="50" t="s">
         <v>107</v>
       </c>
@@ -2809,7 +2809,7 @@
       <c r="E29" s="63"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="/HBlOI4uQUqg/9nO7C/ktqXANaFpWNQ4VHt3dQbJIUn/YEPsTgXS4RWZdvTE+ovsirrBGMNAfKTU50a6Iz9CNQ==" saltValue="mRnOdzsIZTNBzc/JMi0l4A==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" selectLockedCells="1" autoFilter="0" pivotTables="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="+z573ywRttFf+dAAgYaIOIBBNUJY+nMRS4tZgTgy5kbEcETtFNKi78kRmDQnXTQJulbAtd1p2J9VwkVu8+L0hg==" saltValue="oL8JWHWZGDrWh3+3Q2SaJw==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" selectLockedCells="1" autoFilter="0" pivotTables="0"/>
   <mergeCells count="4">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B21:D21"/>
@@ -2817,7 +2817,7 @@
     <mergeCell ref="E10:G10"/>
   </mergeCells>
   <conditionalFormatting sqref="D7">
-    <cfRule type="timePeriod" dxfId="12" priority="4" timePeriod="lastMonth">
+    <cfRule type="timePeriod" dxfId="50" priority="4" timePeriod="lastMonth">
       <formula>AND(MONTH(D7)=MONTH(EDATE(TODAY(),0-1)),YEAR(D7)=YEAR(EDATE(TODAY(),0-1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2830,7 +2830,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3">
       <formula1>lstLimiteHora</formula1>
     </dataValidation>
@@ -2838,6 +2838,10 @@
       <formula1>"Sim,Não"</formula1>
     </dataValidation>
     <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7 D5 D23:D24 F21">
+      <formula1>0</formula1>
+      <formula2>0.999305555555556</formula2>
+    </dataValidation>
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12:F18">
       <formula1>0</formula1>
       <formula2>0.999305555555556</formula2>
     </dataValidation>
@@ -2897,7 +2901,7 @@
       <c r="G1" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="O1" s="73" t="str">
+      <c r="O1" s="74" t="str">
         <f>"*Limite de horas: " &amp; LIMITE &amp; "; e 
 *Contabiliza a partir de " &amp; TEXT(CARENCIA, "hh:mm") &amp; " hora(s) (para mais ou para menos);
 *Caso tenha Atestado em um dos períodos, o que ultrapassar de 4:00 horas de trabalho contabiliza hora positiva."</f>
@@ -2905,76 +2909,76 @@
 *Contabiliza a partir de 00:10 hora(s) (para mais ou para menos);
 *Caso tenha Atestado em um dos períodos, o que ultrapassar de 4:00 horas de trabalho contabiliza hora positiva.</v>
       </c>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="73"/>
-      <c r="S1" s="73"/>
-      <c r="T1" s="73"/>
-      <c r="U1" s="73"/>
-      <c r="V1" s="73"/>
-      <c r="W1" s="73"/>
-      <c r="X1" s="73"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+      <c r="S1" s="74"/>
+      <c r="T1" s="74"/>
+      <c r="U1" s="74"/>
+      <c r="V1" s="74"/>
+      <c r="W1" s="74"/>
+      <c r="X1" s="74"/>
     </row>
     <row r="2" spans="2:29" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="6"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
       <c r="N2" s="24"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
-      <c r="S2" s="73"/>
-      <c r="T2" s="73"/>
-      <c r="U2" s="73"/>
-      <c r="V2" s="73"/>
-      <c r="W2" s="73"/>
-      <c r="X2" s="73"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="74"/>
+      <c r="S2" s="74"/>
+      <c r="T2" s="74"/>
+      <c r="U2" s="74"/>
+      <c r="V2" s="74"/>
+      <c r="W2" s="74"/>
+      <c r="X2" s="74"/>
     </row>
     <row r="3" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
       <c r="G3" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="H3" s="81" t="s">
+      <c r="H3" s="82" t="s">
         <v>97</v>
       </c>
-      <c r="I3" s="82"/>
+      <c r="I3" s="83"/>
       <c r="N3" s="24"/>
-      <c r="O3" s="73"/>
-      <c r="P3" s="73"/>
-      <c r="Q3" s="73"/>
-      <c r="R3" s="73"/>
-      <c r="S3" s="73"/>
-      <c r="T3" s="73"/>
-      <c r="U3" s="73"/>
-      <c r="V3" s="73"/>
-      <c r="W3" s="73"/>
-      <c r="X3" s="73"/>
+      <c r="O3" s="74"/>
+      <c r="P3" s="74"/>
+      <c r="Q3" s="74"/>
+      <c r="R3" s="74"/>
+      <c r="S3" s="74"/>
+      <c r="T3" s="74"/>
+      <c r="U3" s="74"/>
+      <c r="V3" s="74"/>
+      <c r="W3" s="74"/>
+      <c r="X3" s="74"/>
     </row>
     <row r="4" spans="2:29" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6"/>
       <c r="G4" s="52"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="76"/>
       <c r="N4" s="24"/>
-      <c r="O4" s="73"/>
-      <c r="P4" s="73"/>
-      <c r="Q4" s="73"/>
-      <c r="R4" s="73"/>
-      <c r="S4" s="73"/>
-      <c r="T4" s="73"/>
-      <c r="U4" s="73"/>
-      <c r="V4" s="73"/>
-      <c r="W4" s="73"/>
-      <c r="X4" s="73"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="74"/>
+      <c r="Q4" s="74"/>
+      <c r="R4" s="74"/>
+      <c r="S4" s="74"/>
+      <c r="T4" s="74"/>
+      <c r="U4" s="74"/>
+      <c r="V4" s="74"/>
+      <c r="W4" s="74"/>
+      <c r="X4" s="74"/>
     </row>
     <row r="5" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="76" t="s">
+      <c r="B5" s="77" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="77"/>
+      <c r="C5" s="78"/>
       <c r="D5" s="28" t="s">
         <v>62</v>
       </c>
@@ -3009,8 +3013,8 @@
       <c r="X5" s="24"/>
     </row>
     <row r="6" spans="2:29" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="74"/>
-      <c r="C6" s="78"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="79"/>
       <c r="D6" s="29"/>
       <c r="E6" s="29"/>
       <c r="F6" s="31" t="str">
@@ -3020,15 +3024,15 @@
       <c r="N6" s="24"/>
       <c r="O6" s="24"/>
       <c r="P6" s="24"/>
-      <c r="Q6" s="83" t="s">
+      <c r="Q6" s="84" t="s">
         <v>95</v>
       </c>
-      <c r="R6" s="84"/>
-      <c r="S6" s="84"/>
-      <c r="T6" s="84"/>
-      <c r="U6" s="84"/>
-      <c r="V6" s="84"/>
-      <c r="W6" s="84"/>
+      <c r="R6" s="85"/>
+      <c r="S6" s="85"/>
+      <c r="T6" s="85"/>
+      <c r="U6" s="85"/>
+      <c r="V6" s="85"/>
+      <c r="W6" s="85"/>
       <c r="X6" s="24"/>
     </row>
     <row r="7" spans="2:29" x14ac:dyDescent="0.25">
@@ -8588,7 +8592,7 @@
     <row r="46" spans="2:25" x14ac:dyDescent="0.25"/>
     <row r="47" spans="2:25" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="bBIJ5VKH8eRPD0Nk6AoCBIAJy949a0nruGdg/IfyAUyli4uaivzHwMGe1yKt7zfjsf2LQtKJwt/uv3052sgG8A==" saltValue="8oOuV34fHmvfn2tlV7CO0Q==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" selectLockedCells="1" autoFilter="0" pivotTables="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="wh/+VoYVVnak25x5YuNiGaeakyCVDleTTx/mzFqjy4I51lJuZrooeyoIHS6E9Pw2n2SxRorcnw2F9MW/h2C07w==" saltValue="1qHqpbONbfSXejfoMLEoFg==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" selectLockedCells="1" autoFilter="0" pivotTables="0"/>
   <dataConsolidate/>
   <mergeCells count="7">
     <mergeCell ref="O1:X4"/>

</xml_diff>

<commit_message>
Inserção de cálculo de Intervalo de Almoço
</commit_message>
<xml_diff>
--- a/Controle de Ponto.xlsx
+++ b/Controle de Ponto.xlsx
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="113">
   <si>
     <t>Data</t>
   </si>
@@ -438,6 +438,9 @@
   </si>
   <si>
     <t>Total Jornada</t>
+  </si>
+  <si>
+    <t>Intervalo Almoço</t>
   </si>
 </sst>
 </file>
@@ -451,7 +454,7 @@
     <numFmt numFmtId="167" formatCode="[h]:mm"/>
     <numFmt numFmtId="168" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -554,6 +557,14 @@
       <u/>
       <sz val="16"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -879,7 +890,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1133,12 +1144,142 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="67">
+  <dxfs count="71">
+    <dxf>
+      <numFmt numFmtId="167" formatCode="[h]:mm"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD5D6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD1D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD5D6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD1D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <i/>
@@ -1335,90 +1476,6 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD5D6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD1D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD5D6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD1D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -1518,16 +1575,6 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1646,53 +1693,53 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tblEvento" displayName="tblEvento" ref="A2:F13" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tblEvento" displayName="tblEvento" ref="A2:F13" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69">
   <sortState ref="A3:F13">
     <sortCondition ref="A8"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="Evento" dataDxfId="64"/>
-    <tableColumn id="2" name="Colorir Linha" dataDxfId="63"/>
-    <tableColumn id="5" name="Colorir Período" dataDxfId="62"/>
-    <tableColumn id="6" name="Libera o Período" dataDxfId="61"/>
-    <tableColumn id="4" name="Conta hora Extra" dataDxfId="60"/>
-    <tableColumn id="3" name="Descrição" dataDxfId="59"/>
+    <tableColumn id="1" name="Evento" dataDxfId="68"/>
+    <tableColumn id="2" name="Colorir Linha" dataDxfId="67"/>
+    <tableColumn id="5" name="Colorir Período" dataDxfId="66"/>
+    <tableColumn id="6" name="Libera o Período" dataDxfId="65"/>
+    <tableColumn id="4" name="Conta hora Extra" dataDxfId="64"/>
+    <tableColumn id="3" name="Descrição" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="tblLimiteHora" displayName="tblLimiteHora" ref="H2:J4" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="tblLimiteHora" displayName="tblLimiteHora" ref="H2:J4" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
   <autoFilter ref="H2:J4"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Limite de horas" dataDxfId="56"/>
-    <tableColumn id="3" name="Limite" dataDxfId="55"/>
-    <tableColumn id="2" name="h" dataDxfId="54"/>
+    <tableColumn id="1" name="Limite de horas" dataDxfId="60"/>
+    <tableColumn id="3" name="Limite" dataDxfId="59"/>
+    <tableColumn id="2" name="h" dataDxfId="58"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="tbl_Mes" displayName="tbl_Mes" ref="L2:L14" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="tbl_Mes" displayName="tbl_Mes" ref="L2:L14" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
   <autoFilter ref="L2:L14"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Mês" dataDxfId="51"/>
+    <tableColumn id="1" name="Mês" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tblDiaUtil" displayName="tblDiaUtil" ref="B11:G18" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tblDiaUtil" displayName="tblDiaUtil" ref="B11:G18" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
   <tableColumns count="6">
-    <tableColumn id="1" name="Dia da Semana" dataDxfId="47"/>
-    <tableColumn id="4" name="Abreviatura" dataDxfId="46"/>
-    <tableColumn id="2" name="É dia util?" dataDxfId="45"/>
-    <tableColumn id="3" name="1º Período" dataDxfId="44"/>
-    <tableColumn id="5" name="2º Período" dataDxfId="43"/>
-    <tableColumn id="6" name="Total Jornada" dataDxfId="42">
+    <tableColumn id="1" name="Dia da Semana" dataDxfId="52"/>
+    <tableColumn id="4" name="Abreviatura" dataDxfId="51"/>
+    <tableColumn id="2" name="É dia util?" dataDxfId="50"/>
+    <tableColumn id="3" name="1º Período" dataDxfId="49"/>
+    <tableColumn id="5" name="2º Período" dataDxfId="48"/>
+    <tableColumn id="6" name="Total Jornada" dataDxfId="47">
       <calculatedColumnFormula>IF((tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]])&gt;0,tblDiaUtil[[#This Row],[1º Período]]+tblDiaUtil[[#This Row],[2º Período]],"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1701,32 +1748,32 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="tblDiaUtil7" displayName="tblDiaUtil7" ref="B22:D24" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="tblDiaUtil7" displayName="tblDiaUtil7" ref="B22:D24" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
   <tableColumns count="3">
-    <tableColumn id="1" name="Período" dataDxfId="39"/>
-    <tableColumn id="4" name="Abreviatura" dataDxfId="38"/>
-    <tableColumn id="2" name="Qtd. Horas por Jornada" dataDxfId="37"/>
+    <tableColumn id="1" name="Período" dataDxfId="44"/>
+    <tableColumn id="4" name="Abreviatura" dataDxfId="43"/>
+    <tableColumn id="2" name="Qtd. Horas por Jornada" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblHoras" displayName="tblHoras" ref="B8:X39" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
-  <tableColumns count="23">
-    <tableColumn id="1" name="Data" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblHoras" displayName="tblHoras" ref="B8:Y39" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+  <tableColumns count="24">
+    <tableColumn id="1" name="Data" dataDxfId="39">
       <calculatedColumnFormula>IF(B8&lt;&gt;"",IF(DAY(B8+1)=1,"",B8+1),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Dia" dataDxfId="21">
+    <tableColumn id="2" name="Dia" dataDxfId="38">
       <calculatedColumnFormula>TEXT(tblHoras[[#This Row],[Data]],"ddd")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Evento _x000a_(1º Período)" dataDxfId="20"/>
-    <tableColumn id="4" name="Entrada - 1" dataDxfId="19"/>
-    <tableColumn id="5" name="Saída - 1 (Almoço)" dataDxfId="18"/>
-    <tableColumn id="6" name="Entrada - 2 (Almoço)" dataDxfId="17"/>
-    <tableColumn id="7" name="Saída - 2" dataDxfId="16"/>
-    <tableColumn id="13" name="Evento _x000a_(2º Período)" dataDxfId="15"/>
-    <tableColumn id="15" name="Horas Trabalhadas (1º Período)" dataDxfId="14">
+    <tableColumn id="3" name="Evento _x000a_(1º Período)" dataDxfId="37"/>
+    <tableColumn id="4" name="Entrada - 1" dataDxfId="36"/>
+    <tableColumn id="5" name="Saída - 1 (Almoço)" dataDxfId="35"/>
+    <tableColumn id="6" name="Entrada - 2 (Almoço)" dataDxfId="34"/>
+    <tableColumn id="7" name="Saída - 2" dataDxfId="33"/>
+    <tableColumn id="13" name="Evento _x000a_(2º Período)" dataDxfId="32"/>
+    <tableColumn id="15" name="Horas Trabalhadas (1º Período)" dataDxfId="31">
       <calculatedColumnFormula>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -1746,7 +1793,7 @@
                           0)),
                     0)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Horas Trabalhadas (2º Período)" dataDxfId="13">
+    <tableColumn id="16" name="Horas Trabalhadas (2º Período)" dataDxfId="30">
       <calculatedColumnFormula>IF($B$6&lt;&gt;"",
 IF(AND(tblHoras[Evento 
 (2º Período)]&lt;&gt;"",IF(ISERROR(VLOOKUP(tblHoras[Evento 
@@ -1766,10 +1813,10 @@
                          0)),
        0)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Horas Trabalhadas" dataDxfId="12">
+    <tableColumn id="8" name="Horas Trabalhadas" dataDxfId="29">
       <calculatedColumnFormula>tblHoras[[#This Row],[Horas Trabalhadas (1º Período)]]+tblHoras[[#This Row],[Horas Trabalhadas (2º Período)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Jornada Diária" dataDxfId="11">
+    <tableColumn id="17" name="Jornada Diária" dataDxfId="28">
       <calculatedColumnFormula>IF(tblHoras[Data]&lt;&gt;"",
         IF(
 AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
@@ -1781,7 +1828,7 @@
               ""),
          "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Horas Trabalhadas Além Jornada" dataDxfId="10">
+    <tableColumn id="11" name="Horas Trabalhadas Além Jornada" dataDxfId="27">
       <calculatedColumnFormula>IF(OR(tblHoras[Horas Trabalhadas (1º Período)]&lt;&gt;0,tblHoras[Horas Trabalhadas (2º Período)]&lt;&gt;0),
         IF(ISNUMBER(tblHoras[Jornada Diária]),
               IF(tblHoras[Jornada Diária]&gt;(tblHoras[Horas Trabalhadas (2º Período)]+tblHoras[Horas Trabalhadas (1º Período)]),
@@ -1809,7 +1856,7 @@
 (2º Período)],tblEvento[[Evento]:[Libera o Período]],4,FALSE)="Não",TRUE,FALSE)),
 -IF(VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE)&lt;&gt;"",VLOOKUP(tblHoras[Dia],tblDiaUtil[[Abreviatura]:[2º Período]],4,FALSE),JORNADA_PERIODO_2),0))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Saldo de Horas" dataDxfId="9">
+    <tableColumn id="18" name="Saldo de Horas" dataDxfId="26">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&gt;0,
         IF(tblHoras[[#This Row],[Jornada Diária]]&lt;&gt;"",
               IF(HOUR(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]])&gt;=VLOOKUP(LIMITE,tblLimiteHora[],Tabelas!$I$1,FALSE),
@@ -1818,23 +1865,26 @@
               tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]),
         0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="Saldo de Horas (Decimal)" dataDxfId="8">
+    <tableColumn id="20" name="Saldo de Horas (Decimal)" dataDxfId="25">
       <calculatedColumnFormula>tblHoras[[#This Row],[Saldo de Horas]]*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="Atrasos_x000a_(horas)" dataDxfId="7">
+    <tableColumn id="24" name="Intervalo Almoço" dataDxfId="0">
+      <calculatedColumnFormula>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="19" name="Atrasos_x000a_(horas)" dataDxfId="24">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&lt;0,IF(OR(tblHoras[[#This Row],[Evento 
 (1º Período)]]="",tblHoras[[#This Row],[Evento 
 (2º Período)]]=""),tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]],""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Atrasos (Decimal)" dataDxfId="6">
+    <tableColumn id="21" name="Atrasos (Decimal)" dataDxfId="23">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Faltas_x000a_(dias)" dataDxfId="5">
+    <tableColumn id="14" name="Faltas_x000a_(dias)" dataDxfId="22">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Jornada Diária]]&lt;&gt;"",IF((N(tblHoras[[#This Row],[Jornada Diária]])-ABS(N(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]])))=0,1,""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Hora Extra Normal" dataDxfId="4">
+    <tableColumn id="10" name="Hora Extra Normal" dataDxfId="21">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[[#This Row],[Data]],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[[#This Row],[Evento 
 (1º Período)]]&lt;&gt;"",IF(VLOOKUP(tblHoras[[#This Row],[Evento 
@@ -1843,10 +1893,10 @@
 (2º Período)]],tblEvento[],Tabelas!$E$1,FALSE)="Sim",FALSE,TRUE),TRUE)),
 tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]],""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="Hora Extra Normal (Decimal)" dataDxfId="3">
+    <tableColumn id="22" name="Hora Extra Normal (Decimal)" dataDxfId="20">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Hora Extra _x000a_Especial" dataDxfId="2">
+    <tableColumn id="9" name="Hora Extra _x000a_Especial" dataDxfId="19">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[[#This Row],[Data]],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[[#This Row],[Evento 
 (1º Período)]]&lt;&gt;"",IF(VLOOKUP(tblHoras[[#This Row],[Evento 
@@ -1855,12 +1905,12 @@
 (2º Período)]],tblEvento[],Tabelas!$E$1,FALSE)="Sim",TRUE,FALSE),FALSE)),
 tblHoras[[#This Row],[Horas Trabalhadas Além Jornada]],""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="Hora Extra Especial (Decimal)" dataDxfId="1">
+    <tableColumn id="23" name="Hora Extra Especial (Decimal)" dataDxfId="18">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Informação" dataDxfId="0">
+    <tableColumn id="12" name="Informação" dataDxfId="17">
       <calculatedColumnFormula>IF(tblHoras[[#This Row],[Evento 
 (1º Período)]]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[[#This Row],[Evento 
 (1º Período)]],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[[#This Row],[Evento 
@@ -2817,7 +2867,7 @@
     <mergeCell ref="E10:G10"/>
   </mergeCells>
   <conditionalFormatting sqref="D7">
-    <cfRule type="timePeriod" dxfId="50" priority="4" timePeriod="lastMonth">
+    <cfRule type="timePeriod" dxfId="16" priority="4" timePeriod="lastMonth">
       <formula>AND(MONTH(D7)=MONTH(EDATE(TODAY(),0-1)),YEAR(D7)=YEAR(EDATE(TODAY(),0-1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2861,14 +2911,14 @@
     <tabColor theme="4" tint="0.59999389629810485"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AG47"/>
+  <dimension ref="A1:AH47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection activeCell="H10" sqref="H10"/>
       <selection pane="topRight" activeCell="H10" sqref="H10"/>
       <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6:C6"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2880,24 +2930,25 @@
     <col min="10" max="14" width="12.7109375" style="5" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="12.7109375" style="5" customWidth="1"/>
     <col min="16" max="16" width="10.7109375" style="5" customWidth="1"/>
-    <col min="17" max="17" width="12.7109375" style="5" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" style="5" hidden="1" customWidth="1"/>
-    <col min="19" max="20" width="12.7109375" style="5" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="10.7109375" style="5" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="12.7109375" style="5" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="10.7109375" style="5" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="38.42578125" style="5" customWidth="1"/>
-    <col min="25" max="25" width="2.7109375" style="5" customWidth="1"/>
-    <col min="26" max="26" width="9.140625" style="5" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="12.42578125" style="5" hidden="1" customWidth="1"/>
-    <col min="28" max="29" width="0" style="5" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="9.140625" style="5" hidden="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" style="5" hidden="1" customWidth="1"/>
-    <col min="32" max="33" width="0" style="5" hidden="1" customWidth="1"/>
-    <col min="34" max="16384" width="9.140625" style="5" hidden="1"/>
+    <col min="17" max="17" width="10.7109375" style="5" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" style="5" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" style="5" hidden="1" customWidth="1"/>
+    <col min="20" max="21" width="12.7109375" style="5" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" style="5" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="12.7109375" style="5" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="10.7109375" style="5" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="38.42578125" style="5" customWidth="1"/>
+    <col min="26" max="26" width="2.7109375" style="5" customWidth="1"/>
+    <col min="27" max="27" width="9.140625" style="5" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="12.42578125" style="5" hidden="1" customWidth="1"/>
+    <col min="29" max="30" width="0" style="5" hidden="1" customWidth="1"/>
+    <col min="31" max="31" width="9.140625" style="5" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="12.42578125" style="5" hidden="1" customWidth="1"/>
+    <col min="33" max="34" width="0" style="5" hidden="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.140625" style="5" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G1" s="27" t="s">
         <v>58</v>
       </c>
@@ -2918,8 +2969,9 @@
       <c r="V1" s="74"/>
       <c r="W1" s="74"/>
       <c r="X1" s="74"/>
+      <c r="Y1" s="74"/>
     </row>
-    <row r="2" spans="2:29" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="6"/>
       <c r="G2" s="80"/>
       <c r="H2" s="81"/>
@@ -2935,8 +2987,9 @@
       <c r="V2" s="74"/>
       <c r="W2" s="74"/>
       <c r="X2" s="74"/>
+      <c r="Y2" s="74"/>
     </row>
-    <row r="3" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
       <c r="G3" s="42" t="s">
         <v>96</v>
@@ -2956,8 +3009,9 @@
       <c r="V3" s="74"/>
       <c r="W3" s="74"/>
       <c r="X3" s="74"/>
+      <c r="Y3" s="74"/>
     </row>
-    <row r="4" spans="2:29" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6"/>
       <c r="G4" s="52"/>
       <c r="H4" s="75"/>
@@ -2973,8 +3027,9 @@
       <c r="V4" s="74"/>
       <c r="W4" s="74"/>
       <c r="X4" s="74"/>
+      <c r="Y4" s="74"/>
     </row>
-    <row r="5" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="77" t="s">
         <v>59</v>
       </c>
@@ -3010,9 +3065,12 @@
       <c r="W5" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="X5" s="24"/>
+      <c r="X5" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y5" s="24"/>
     </row>
-    <row r="6" spans="2:29" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:30" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="75"/>
       <c r="C6" s="79"/>
       <c r="D6" s="29"/>
@@ -3033,9 +3091,10 @@
       <c r="U6" s="85"/>
       <c r="V6" s="85"/>
       <c r="W6" s="85"/>
-      <c r="X6" s="24"/>
+      <c r="X6" s="85"/>
+      <c r="Y6" s="24"/>
     </row>
-    <row r="7" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:30" x14ac:dyDescent="0.25">
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
@@ -3065,36 +3124,40 @@
         <v>0</v>
       </c>
       <c r="Q7" s="43">
+        <f>SUM(tblHoras[Intervalo Almoço])</f>
+        <v>0</v>
+      </c>
+      <c r="R7" s="43">
         <f>SUM(tblHoras[Atrasos
 (horas)])</f>
         <v>0</v>
       </c>
-      <c r="R7" s="46">
+      <c r="S7" s="46">
         <f>SUM(tblHoras[Atrasos (Decimal)])</f>
         <v>0</v>
       </c>
-      <c r="S7" s="44">
+      <c r="T7" s="44">
         <f>SUM(tblHoras[Faltas
 (dias)])</f>
         <v>0</v>
       </c>
-      <c r="T7" s="43">
+      <c r="U7" s="43">
         <f>SUM(tblHoras[Hora Extra Normal])</f>
         <v>0</v>
       </c>
-      <c r="U7" s="46"/>
-      <c r="V7" s="43">
+      <c r="V7" s="46"/>
+      <c r="W7" s="43">
         <f>SUM(tblHoras[Hora Extra 
 Especial])</f>
         <v>0</v>
       </c>
-      <c r="W7" s="46">
+      <c r="X7" s="46">
         <f>SUM(tblHoras[Hora Extra Especial (Decimal)])</f>
         <v>0</v>
       </c>
-      <c r="X7" s="24"/>
+      <c r="Y7" s="24"/>
     </row>
-    <row r="8" spans="2:29" s="9" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:30" s="9" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
         <v>0</v>
       </c>
@@ -3141,32 +3204,35 @@
         <v>99</v>
       </c>
       <c r="Q8" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="R8" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="R8" s="9" t="s">
+      <c r="S8" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="S8" s="9" t="s">
+      <c r="T8" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="T8" s="9" t="s">
+      <c r="U8" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="U8" s="9" t="s">
+      <c r="V8" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="V8" s="9" t="s">
+      <c r="W8" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="W8" s="9" t="s">
+      <c r="X8" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="X8" s="9" t="s">
+      <c r="Y8" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="AA8" s="25"/>
+      <c r="AB8" s="25"/>
     </row>
-    <row r="9" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="str">
         <f>IF(ISERROR(F6),"",F6)</f>
         <v/>
@@ -3176,7 +3242,7 @@
         <v/>
       </c>
       <c r="D9" s="53"/>
-      <c r="E9" s="1"/>
+      <c r="E9" s="86"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -3283,23 +3349,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q9" s="14" t="str">
+      <c r="Q9" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R9" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R9" s="47" t="str">
+      <c r="S9" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S9" s="14" t="str">
+      <c r="T9" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T9" s="14" t="str">
+      <c r="U9" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -3309,11 +3379,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U9" s="47" t="str">
+      <c r="V9" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V9" s="14" t="str">
+      <c r="W9" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -3323,13 +3393,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W9" s="47" t="str">
+      <c r="X9" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X9" s="15" t="str">
+      <c r="Y9" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -3339,10 +3409,10 @@
 (2º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")</f>
         <v/>
       </c>
-      <c r="Z9" s="16"/>
-      <c r="AC9" s="17"/>
+      <c r="AA9" s="16"/>
+      <c r="AD9" s="17"/>
     </row>
-    <row r="10" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="str">
         <f>IF(B9&lt;&gt;"",IF(DAY(B9+1)=IF($E$6&lt;&gt;"",$E$6,1),"",B9+1),"")</f>
         <v/>
@@ -3459,23 +3529,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q10" s="14" t="str">
+      <c r="Q10" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R10" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R10" s="47" t="str">
+      <c r="S10" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S10" s="14" t="str">
+      <c r="T10" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T10" s="14" t="str">
+      <c r="U10" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -3485,11 +3559,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U10" s="47" t="str">
+      <c r="V10" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V10" s="14" t="str">
+      <c r="W10" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -3499,13 +3573,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W10" s="47" t="str">
+      <c r="X10" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X10" s="15" t="str">
+      <c r="Y10" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -3515,9 +3589,9 @@
 (2º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")</f>
         <v/>
       </c>
-      <c r="AC10" s="17"/>
+      <c r="AD10" s="17"/>
     </row>
-    <row r="11" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="str">
         <f t="shared" ref="B11:B39" si="0">IF(B10&lt;&gt;"",IF(DAY(B10+1)=IF($E$6&lt;&gt;"",$E$6,1),"",B10+1),"")</f>
         <v/>
@@ -3634,23 +3708,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q11" s="14" t="str">
+      <c r="Q11" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R11" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R11" s="47" t="str">
+      <c r="S11" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S11" s="14" t="str">
+      <c r="T11" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T11" s="14" t="str">
+      <c r="U11" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -3660,11 +3738,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U11" s="47" t="str">
+      <c r="V11" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V11" s="14" t="str">
+      <c r="W11" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -3674,13 +3752,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W11" s="47" t="str">
+      <c r="X11" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X11" s="15" t="str">
+      <c r="Y11" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -3691,7 +3769,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3808,23 +3886,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q12" s="14" t="str">
+      <c r="Q12" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R12" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R12" s="47" t="str">
+      <c r="S12" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S12" s="14" t="str">
+      <c r="T12" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T12" s="14" t="str">
+      <c r="U12" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -3834,11 +3916,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U12" s="47" t="str">
+      <c r="V12" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V12" s="14" t="str">
+      <c r="W12" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -3848,13 +3930,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W12" s="47" t="str">
+      <c r="X12" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X12" s="15" t="str">
+      <c r="Y12" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -3865,7 +3947,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3982,23 +4064,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="14" t="str">
+      <c r="Q13" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R13" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R13" s="47" t="str">
+      <c r="S13" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S13" s="14" t="str">
+      <c r="T13" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T13" s="14" t="str">
+      <c r="U13" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -4008,11 +4094,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U13" s="47" t="str">
+      <c r="V13" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V13" s="14" t="str">
+      <c r="W13" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -4022,13 +4108,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W13" s="47" t="str">
+      <c r="X13" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X13" s="15" t="str">
+      <c r="Y13" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -4039,7 +4125,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -4156,23 +4242,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="14" t="str">
+      <c r="Q14" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R14" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R14" s="47" t="str">
+      <c r="S14" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S14" s="14" t="str">
+      <c r="T14" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T14" s="14" t="str">
+      <c r="U14" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -4182,11 +4272,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U14" s="47" t="str">
+      <c r="V14" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V14" s="14" t="str">
+      <c r="W14" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -4196,13 +4286,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W14" s="47" t="str">
+      <c r="X14" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X14" s="15" t="str">
+      <c r="Y14" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -4212,10 +4302,10 @@
 (2º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")</f>
         <v/>
       </c>
-      <c r="AB14" s="18"/>
       <c r="AC14" s="18"/>
+      <c r="AD14" s="18"/>
     </row>
-    <row r="15" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -4332,23 +4422,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q15" s="14" t="str">
+      <c r="Q15" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R15" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R15" s="47" t="str">
+      <c r="S15" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S15" s="14" t="str">
+      <c r="T15" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T15" s="14" t="str">
+      <c r="U15" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -4358,11 +4452,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U15" s="47" t="str">
+      <c r="V15" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V15" s="14" t="str">
+      <c r="W15" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -4372,13 +4466,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W15" s="47" t="str">
+      <c r="X15" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X15" s="15" t="str">
+      <c r="Y15" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -4388,9 +4482,9 @@
 (2º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")</f>
         <v/>
       </c>
-      <c r="AB15" s="17"/>
+      <c r="AC15" s="17"/>
     </row>
-    <row r="16" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -4507,23 +4601,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q16" s="14" t="str">
+      <c r="Q16" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R16" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R16" s="47" t="str">
+      <c r="S16" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S16" s="14" t="str">
+      <c r="T16" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T16" s="14" t="str">
+      <c r="U16" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -4533,11 +4631,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U16" s="47" t="str">
+      <c r="V16" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V16" s="14" t="str">
+      <c r="W16" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -4547,13 +4645,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W16" s="47" t="str">
+      <c r="X16" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X16" s="15" t="str">
+      <c r="Y16" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -4564,7 +4662,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -4681,23 +4779,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q17" s="14" t="str">
+      <c r="Q17" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R17" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R17" s="47" t="str">
+      <c r="S17" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S17" s="14" t="str">
+      <c r="T17" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T17" s="14" t="str">
+      <c r="U17" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -4707,11 +4809,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U17" s="47" t="str">
+      <c r="V17" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V17" s="14" t="str">
+      <c r="W17" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -4721,13 +4823,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W17" s="47" t="str">
+      <c r="X17" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X17" s="15" t="str">
+      <c r="Y17" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -4738,7 +4840,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B18" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -4855,23 +4957,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q18" s="14" t="str">
+      <c r="Q18" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R18" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R18" s="47" t="str">
+      <c r="S18" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S18" s="14" t="str">
+      <c r="T18" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T18" s="14" t="str">
+      <c r="U18" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -4881,11 +4987,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U18" s="47" t="str">
+      <c r="V18" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V18" s="14" t="str">
+      <c r="W18" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -4895,13 +5001,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W18" s="47" t="str">
+      <c r="X18" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X18" s="15" t="str">
+      <c r="Y18" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -4912,7 +5018,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -5029,23 +5135,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="14" t="str">
+      <c r="Q19" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R19" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R19" s="47" t="str">
+      <c r="S19" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S19" s="14" t="str">
+      <c r="T19" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T19" s="14" t="str">
+      <c r="U19" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -5055,11 +5165,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U19" s="47" t="str">
+      <c r="V19" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V19" s="14" t="str">
+      <c r="W19" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -5069,13 +5179,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W19" s="47" t="str">
+      <c r="X19" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X19" s="15" t="str">
+      <c r="Y19" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -5086,7 +5196,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B20" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -5203,23 +5313,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q20" s="14" t="str">
+      <c r="Q20" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R20" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R20" s="47" t="str">
+      <c r="S20" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S20" s="14" t="str">
+      <c r="T20" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T20" s="14" t="str">
+      <c r="U20" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -5229,11 +5343,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U20" s="47" t="str">
+      <c r="V20" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V20" s="14" t="str">
+      <c r="W20" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -5243,13 +5357,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W20" s="47" t="str">
+      <c r="X20" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X20" s="15" t="str">
+      <c r="Y20" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -5260,7 +5374,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B21" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -5377,23 +5491,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q21" s="14" t="str">
+      <c r="Q21" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R21" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R21" s="47" t="str">
+      <c r="S21" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S21" s="14" t="str">
+      <c r="T21" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T21" s="14" t="str">
+      <c r="U21" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -5403,11 +5521,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U21" s="47" t="str">
+      <c r="V21" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V21" s="14" t="str">
+      <c r="W21" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -5417,13 +5535,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W21" s="47" t="str">
+      <c r="X21" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X21" s="15" t="str">
+      <c r="Y21" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -5434,7 +5552,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -5551,23 +5669,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q22" s="14" t="str">
+      <c r="Q22" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R22" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R22" s="47" t="str">
+      <c r="S22" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S22" s="14" t="str">
+      <c r="T22" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T22" s="14" t="str">
+      <c r="U22" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -5577,11 +5699,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U22" s="47" t="str">
+      <c r="V22" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V22" s="14" t="str">
+      <c r="W22" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -5591,13 +5713,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W22" s="47" t="str">
+      <c r="X22" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X22" s="15" t="str">
+      <c r="Y22" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -5608,7 +5730,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B23" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -5725,23 +5847,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q23" s="14" t="str">
+      <c r="Q23" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R23" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R23" s="47" t="str">
+      <c r="S23" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S23" s="14" t="str">
+      <c r="T23" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T23" s="14" t="str">
+      <c r="U23" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -5751,11 +5877,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U23" s="47" t="str">
+      <c r="V23" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V23" s="14" t="str">
+      <c r="W23" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -5765,13 +5891,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W23" s="47" t="str">
+      <c r="X23" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X23" s="15" t="str">
+      <c r="Y23" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -5782,7 +5908,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B24" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -5899,23 +6025,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q24" s="14" t="str">
+      <c r="Q24" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R24" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R24" s="47" t="str">
+      <c r="S24" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S24" s="14" t="str">
+      <c r="T24" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T24" s="14" t="str">
+      <c r="U24" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -5925,11 +6055,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U24" s="47" t="str">
+      <c r="V24" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V24" s="14" t="str">
+      <c r="W24" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -5939,13 +6069,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W24" s="47" t="str">
+      <c r="X24" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X24" s="15" t="str">
+      <c r="Y24" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -5956,7 +6086,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B25" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6073,23 +6203,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q25" s="14" t="str">
+      <c r="Q25" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R25" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R25" s="47" t="str">
+      <c r="S25" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S25" s="14" t="str">
+      <c r="T25" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T25" s="14" t="str">
+      <c r="U25" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -6099,11 +6233,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U25" s="47" t="str">
+      <c r="V25" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V25" s="14" t="str">
+      <c r="W25" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -6113,13 +6247,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W25" s="47" t="str">
+      <c r="X25" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X25" s="15" t="str">
+      <c r="Y25" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -6130,7 +6264,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B26" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6247,23 +6381,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q26" s="14" t="str">
+      <c r="Q26" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R26" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R26" s="47" t="str">
+      <c r="S26" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S26" s="14" t="str">
+      <c r="T26" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T26" s="14" t="str">
+      <c r="U26" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -6273,11 +6411,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U26" s="47" t="str">
+      <c r="V26" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V26" s="14" t="str">
+      <c r="W26" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -6287,13 +6425,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W26" s="47" t="str">
+      <c r="X26" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X26" s="15" t="str">
+      <c r="Y26" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -6304,7 +6442,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B27" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6421,23 +6559,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q27" s="14" t="str">
+      <c r="Q27" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R27" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R27" s="47" t="str">
+      <c r="S27" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S27" s="14" t="str">
+      <c r="T27" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T27" s="14" t="str">
+      <c r="U27" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -6447,11 +6589,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U27" s="47" t="str">
+      <c r="V27" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V27" s="14" t="str">
+      <c r="W27" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -6461,13 +6603,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W27" s="47" t="str">
+      <c r="X27" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X27" s="15" t="str">
+      <c r="Y27" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -6478,7 +6620,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B28" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6595,23 +6737,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q28" s="14" t="str">
+      <c r="Q28" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R28" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R28" s="47" t="str">
+      <c r="S28" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S28" s="14" t="str">
+      <c r="T28" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T28" s="14" t="str">
+      <c r="U28" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -6621,11 +6767,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U28" s="47" t="str">
+      <c r="V28" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V28" s="14" t="str">
+      <c r="W28" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -6635,13 +6781,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W28" s="47" t="str">
+      <c r="X28" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X28" s="15" t="str">
+      <c r="Y28" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -6652,7 +6798,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B29" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6769,23 +6915,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q29" s="14" t="str">
+      <c r="Q29" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R29" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R29" s="47" t="str">
+      <c r="S29" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S29" s="14" t="str">
+      <c r="T29" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T29" s="14" t="str">
+      <c r="U29" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -6795,11 +6945,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U29" s="47" t="str">
+      <c r="V29" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V29" s="14" t="str">
+      <c r="W29" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -6809,13 +6959,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W29" s="47" t="str">
+      <c r="X29" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X29" s="15" t="str">
+      <c r="Y29" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -6826,7 +6976,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B30" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6943,23 +7093,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q30" s="14" t="str">
+      <c r="Q30" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R30" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R30" s="47" t="str">
+      <c r="S30" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S30" s="14" t="str">
+      <c r="T30" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T30" s="14" t="str">
+      <c r="U30" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -6969,11 +7123,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U30" s="47" t="str">
+      <c r="V30" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V30" s="14" t="str">
+      <c r="W30" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -6983,13 +7137,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W30" s="47" t="str">
+      <c r="X30" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X30" s="15" t="str">
+      <c r="Y30" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -7000,7 +7154,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B31" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -7117,23 +7271,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q31" s="14" t="str">
+      <c r="Q31" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R31" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R31" s="47" t="str">
+      <c r="S31" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S31" s="14" t="str">
+      <c r="T31" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T31" s="14" t="str">
+      <c r="U31" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -7143,11 +7301,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U31" s="47" t="str">
+      <c r="V31" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V31" s="14" t="str">
+      <c r="W31" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -7157,13 +7315,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W31" s="47" t="str">
+      <c r="X31" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X31" s="15" t="str">
+      <c r="Y31" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -7174,7 +7332,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B32" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -7291,23 +7449,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q32" s="14" t="str">
+      <c r="Q32" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R32" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R32" s="47" t="str">
+      <c r="S32" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S32" s="14" t="str">
+      <c r="T32" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T32" s="14" t="str">
+      <c r="U32" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -7317,11 +7479,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U32" s="47" t="str">
+      <c r="V32" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V32" s="14" t="str">
+      <c r="W32" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -7331,13 +7493,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W32" s="47" t="str">
+      <c r="X32" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X32" s="15" t="str">
+      <c r="Y32" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -7348,7 +7510,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B33" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -7465,23 +7627,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q33" s="14" t="str">
+      <c r="Q33" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R33" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R33" s="47" t="str">
+      <c r="S33" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S33" s="14" t="str">
+      <c r="T33" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T33" s="14" t="str">
+      <c r="U33" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -7491,11 +7657,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U33" s="47" t="str">
+      <c r="V33" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V33" s="14" t="str">
+      <c r="W33" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -7505,13 +7671,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W33" s="47" t="str">
+      <c r="X33" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X33" s="15" t="str">
+      <c r="Y33" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -7522,7 +7688,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B34" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -7639,23 +7805,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q34" s="14" t="str">
+      <c r="Q34" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R34" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R34" s="47" t="str">
+      <c r="S34" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S34" s="14" t="str">
+      <c r="T34" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T34" s="14" t="str">
+      <c r="U34" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -7665,11 +7835,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U34" s="47" t="str">
+      <c r="V34" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V34" s="14" t="str">
+      <c r="W34" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -7679,13 +7849,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W34" s="47" t="str">
+      <c r="X34" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X34" s="15" t="str">
+      <c r="Y34" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -7696,7 +7866,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B35" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -7813,23 +7983,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q35" s="14" t="str">
+      <c r="Q35" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R35" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R35" s="47" t="str">
+      <c r="S35" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S35" s="14" t="str">
+      <c r="T35" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T35" s="14" t="str">
+      <c r="U35" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -7839,11 +8013,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U35" s="47" t="str">
+      <c r="V35" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V35" s="14" t="str">
+      <c r="W35" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -7853,13 +8027,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W35" s="47" t="str">
+      <c r="X35" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X35" s="15" t="str">
+      <c r="Y35" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -7870,7 +8044,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B36" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -7987,23 +8161,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q36" s="14" t="str">
+      <c r="Q36" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R36" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R36" s="47" t="str">
+      <c r="S36" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S36" s="14" t="str">
+      <c r="T36" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T36" s="14" t="str">
+      <c r="U36" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -8013,11 +8191,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U36" s="47" t="str">
+      <c r="V36" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V36" s="14" t="str">
+      <c r="W36" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -8027,13 +8205,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W36" s="47" t="str">
+      <c r="X36" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X36" s="15" t="str">
+      <c r="Y36" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -8044,7 +8222,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B37" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -8161,23 +8339,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q37" s="14" t="str">
+      <c r="Q37" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R37" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R37" s="47" t="str">
+      <c r="S37" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S37" s="14" t="str">
+      <c r="T37" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T37" s="14" t="str">
+      <c r="U37" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -8187,11 +8369,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U37" s="47" t="str">
+      <c r="V37" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V37" s="14" t="str">
+      <c r="W37" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -8201,13 +8383,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W37" s="47" t="str">
+      <c r="X37" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X37" s="15" t="str">
+      <c r="Y37" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -8218,7 +8400,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B38" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -8335,23 +8517,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q38" s="14" t="str">
+      <c r="Q38" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R38" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R38" s="47" t="str">
+      <c r="S38" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S38" s="14" t="str">
+      <c r="T38" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T38" s="14" t="str">
+      <c r="U38" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -8361,11 +8547,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U38" s="47" t="str">
+      <c r="V38" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V38" s="14" t="str">
+      <c r="W38" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -8375,13 +8561,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W38" s="47" t="str">
+      <c r="X38" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X38" s="15" t="str">
+      <c r="Y38" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -8392,7 +8578,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B39" s="11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -8509,23 +8695,27 @@
         <f>tblHoras[[#This Row],[Saldo de Horas]]*24</f>
         <v>0</v>
       </c>
-      <c r="Q39" s="14" t="str">
+      <c r="Q39" s="14">
+        <f>tblHoras[[#This Row],[Entrada - 2 (Almoço)]]-tblHoras[[#This Row],[Saída - 1 (Almoço)]]</f>
+        <v>0</v>
+      </c>
+      <c r="R39" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&lt;0,IF(OR(tblHoras[Evento 
 (1º Período)]="",tblHoras[Evento 
 (2º Período)]=""),tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="R39" s="47" t="str">
+      <c r="S39" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Atrasos
 (horas)]]&lt;&gt;"",tblHoras[[#This Row],[Atrasos
 (horas)]]*24,"")</f>
         <v/>
       </c>
-      <c r="S39" s="14" t="str">
+      <c r="T39" s="14" t="str">
         <f>IF(tblHoras[Jornada Diária]&lt;&gt;"",IF((N(tblHoras[Jornada Diária])-ABS(N(tblHoras[Horas Trabalhadas Além Jornada])))=0,1,""),"")</f>
         <v/>
       </c>
-      <c r="T39" s="14" t="str">
+      <c r="U39" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(AND(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Sim",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -8535,11 +8725,11 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="U39" s="47" t="str">
+      <c r="V39" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra Normal]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra Normal]]*24,"")</f>
         <v/>
       </c>
-      <c r="V39" s="14" t="str">
+      <c r="W39" s="14" t="str">
         <f>IF(tblHoras[Horas Trabalhadas Além Jornada]&gt;0,
 IF(OR(VLOOKUP(TEXT(tblHoras[Data],"dddd"),tblDiaUtil[],3,FALSE)="Não",IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;"",IF(VLOOKUP(tblHoras[Evento 
@@ -8549,13 +8739,13 @@
 tblHoras[Horas Trabalhadas Além Jornada],""),"")</f>
         <v/>
       </c>
-      <c r="W39" s="47" t="str">
+      <c r="X39" s="47" t="str">
         <f>IF(tblHoras[[#This Row],[Hora Extra 
 Especial]]&lt;&gt;"",tblHoras[[#This Row],[Hora Extra 
 Especial]]*24,"")</f>
         <v/>
       </c>
-      <c r="X39" s="15" t="str">
+      <c r="Y39" s="15" t="str">
         <f>IF(tblHoras[Evento 
 (1º Período)]&lt;&gt;""," - " &amp;VLOOKUP(tblHoras[Evento 
 (1º Período)],tblEvento[],Tabelas!$F$1,FALSE),"")&amp;IF(AND(tblHoras[Evento 
@@ -8566,42 +8756,42 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:25" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="X40" s="24"/>
+    <row r="40" spans="2:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Y40" s="24"/>
+      <c r="Z40" s="24"/>
     </row>
-    <row r="41" spans="2:25" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="X41" s="34" t="s">
+    <row r="41" spans="2:26" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y41" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="Y41" s="24"/>
+      <c r="Z41" s="24"/>
     </row>
-    <row r="42" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
-      <c r="X42" s="24"/>
+    <row r="42" spans="2:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="Y42" s="24"/>
+      <c r="Z42" s="24"/>
     </row>
-    <row r="43" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
-      <c r="X43" s="24"/>
+    <row r="43" spans="2:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="Y43" s="24"/>
+      <c r="Z43" s="24"/>
     </row>
-    <row r="44" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
-      <c r="X44" s="24"/>
+    <row r="44" spans="2:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="Y44" s="24"/>
+      <c r="Z44" s="24"/>
     </row>
-    <row r="45" spans="2:25" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="2:25" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="2:25" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="2:26" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:26" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="2:26" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="wh/+VoYVVnak25x5YuNiGaeakyCVDleTTx/mzFqjy4I51lJuZrooeyoIHS6E9Pw2n2SxRorcnw2F9MW/h2C07w==" saltValue="1qHqpbONbfSXejfoMLEoFg==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" selectLockedCells="1" autoFilter="0" pivotTables="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="kT811iAGysTXdhZ9MCGXJz5lW9RSpiHxrQNhaqadPTmvX6bVArBra70CTrEAgK+zQqLDhRlhfd9K6zPU/JwhKw==" saltValue="h9CxrTGujFvjQ1McsEZKoA==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" selectLockedCells="1" autoFilter="0" pivotTables="0"/>
   <dataConsolidate/>
   <mergeCells count="7">
-    <mergeCell ref="O1:X4"/>
+    <mergeCell ref="O1:Y4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="H3:I3"/>
-    <mergeCell ref="Q6:W6"/>
+    <mergeCell ref="Q6:X6"/>
   </mergeCells>
   <dataValidations xWindow="263" yWindow="440" count="5">
     <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Aviso" error="Erro na inserção de dados:_x000a__x000a_'Hora Inválida'_x000a__x000a_Favor inserir uma hora válida no formato: hh:mm (ex. 12:00)" sqref="E9:H39">
@@ -8637,7 +8827,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="20" id="{33616478-990B-44FE-BB07-40117DF3ADA1}">
+          <x14:cfRule type="expression" priority="23" id="{33616478-990B-44FE-BB07-40117DF3ADA1}">
             <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)),FALSE,IF(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
             <x14:dxf>
               <fill>
@@ -8647,10 +8837,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B9:X9 S7 V7 J10:X39</xm:sqref>
+          <xm:sqref>B9:P9 T7 W7 J10:P39 R9:Y39</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="17" id="{D79C2469-95B2-4490-A707-5C27A171E816}">
+          <x14:cfRule type="expression" priority="20" id="{D79C2469-95B2-4490-A707-5C27A171E816}">
             <xm:f>IF(IF(ISERROR(VLOOKUP($D9,Tabelas!$A$3:$C$51,3,FALSE)),FALSE,VLOOKUP($D9,Tabelas!$A$3:$C$51,3,FALSE)="Sim"),TRUE,FALSE)</xm:f>
             <x14:dxf>
               <fill>
@@ -8663,7 +8853,7 @@
           <xm:sqref>D9:F9 J9:J39</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="23" id="{31CF979C-12F0-4F54-B477-D65B5CC060E6}">
+          <x14:cfRule type="expression" priority="26" id="{31CF979C-12F0-4F54-B477-D65B5CC060E6}">
             <xm:f>IF(IF(ISERROR(VLOOKUP($I9,Tabelas!$A$3:$C$51,3,FALSE)),FALSE,VLOOKUP($I9,Tabelas!$A$3:$C$51,3,FALSE)="Sim"),TRUE,FALSE)</xm:f>
             <x14:dxf>
               <fill>
@@ -8676,7 +8866,7 @@
           <xm:sqref>K9:M9 G9:I9 K10:K39 M10:M39</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="13" id="{CF3EF681-ADA3-454F-BD4D-136E8407E816}">
+          <x14:cfRule type="expression" priority="16" id="{CF3EF681-ADA3-454F-BD4D-136E8407E816}">
             <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)),FALSE,IF(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
             <x14:dxf>
               <fill>
@@ -8686,10 +8876,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>Q7</xm:sqref>
+          <xm:sqref>Q7:R7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="8" id="{9015B1FB-D320-45D4-903E-B40FCBE5CA69}">
+          <x14:cfRule type="expression" priority="11" id="{9015B1FB-D320-45D4-903E-B40FCBE5CA69}">
             <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C10,Config!$C$1:$D$18,2,FALSE)),FALSE,IF(VLOOKUP($C10,Config!$C$1:$D$18,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D10,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D10,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I10,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I10,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
             <x14:dxf>
               <fill>
@@ -8702,7 +8892,7 @@
           <xm:sqref>B10:I39</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="7" id="{956628B0-9BEE-401E-B2E2-0213C7CEE5C0}">
+          <x14:cfRule type="expression" priority="10" id="{956628B0-9BEE-401E-B2E2-0213C7CEE5C0}">
             <xm:f>IF(IF(ISERROR(VLOOKUP($D10,Tabelas!$A$3:$C$51,3,FALSE)),FALSE,VLOOKUP($D10,Tabelas!$A$3:$C$51,3,FALSE)="Sim"),TRUE,FALSE)</xm:f>
             <x14:dxf>
               <fill>
@@ -8715,7 +8905,7 @@
           <xm:sqref>D10:F39</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="9" id="{37400795-195C-4039-B9AA-275DE3D968EE}">
+          <x14:cfRule type="expression" priority="12" id="{37400795-195C-4039-B9AA-275DE3D968EE}">
             <xm:f>IF(IF(ISERROR(VLOOKUP($I10,Tabelas!$A$3:$C$51,3,FALSE)),FALSE,VLOOKUP($I10,Tabelas!$A$3:$C$51,3,FALSE)="Sim"),TRUE,FALSE)</xm:f>
             <x14:dxf>
               <fill>
@@ -8728,7 +8918,7 @@
           <xm:sqref>L10:M39 G10:I39</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="6" id="{6833BDA1-C45D-4AD2-B5F4-CA013523FCA7}">
+          <x14:cfRule type="expression" priority="9" id="{6833BDA1-C45D-4AD2-B5F4-CA013523FCA7}">
             <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)),FALSE,IF(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
             <x14:dxf>
               <fill>
@@ -8741,7 +8931,7 @@
           <xm:sqref>O7:P7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="5" id="{ED503053-E09B-4D43-A8D9-9598E4076ED6}">
+          <x14:cfRule type="expression" priority="8" id="{ED503053-E09B-4D43-A8D9-9598E4076ED6}">
             <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)),FALSE,IF(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
             <x14:dxf>
               <fill>
@@ -8751,10 +8941,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>R7</xm:sqref>
+          <xm:sqref>S7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="3" id="{C09E7684-AED8-438C-B68E-2E7738ECC073}">
+          <x14:cfRule type="expression" priority="6" id="{C09E7684-AED8-438C-B68E-2E7738ECC073}">
             <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)),FALSE,IF(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
             <x14:dxf>
               <fill>
@@ -8764,10 +8954,23 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>W7</xm:sqref>
+          <xm:sqref>X7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="2" id="{BD039133-8410-430E-A4D9-B20483016ECF}">
+          <x14:cfRule type="expression" priority="5" id="{BD039133-8410-430E-A4D9-B20483016ECF}">
+            <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)),FALSE,IF(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFFFCC"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>V7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="4" id="{18861696-7153-4870-9908-43C72D087D0E}">
             <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)),FALSE,IF(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
             <x14:dxf>
               <fill>
@@ -8780,8 +8983,8 @@
           <xm:sqref>U7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{18861696-7153-4870-9908-43C72D087D0E}">
-            <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)),FALSE,IF(VLOOKUP($C7,Config!$C$1:$D$18,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I7,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
+          <x14:cfRule type="expression" priority="3" id="{9C04CB79-E69D-4418-BA83-3C05490DDE48}">
+            <xm:f>IF(OR(IF(ISERROR(VLOOKUP($C9,Config!$C$1:$D$18,2,FALSE)),FALSE,IF(VLOOKUP($C9,Config!$C$1:$D$18,2,FALSE)="Não",TRUE,FALSE)),IF(ISERROR(VLOOKUP($D9,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($D9,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE)),IF(ISERROR(VLOOKUP($I9,Tabelas!$A$3:$B$51,2,FALSE)),FALSE,IF(VLOOKUP($I9,Tabelas!$A$3:$B$51,2,FALSE)="Sim",TRUE,FALSE))),TRUE,FALSE)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -8790,7 +8993,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>T7</xm:sqref>
+          <xm:sqref>Q9:Q39</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>